<commit_message>
add all components to network object
</commit_message>
<xml_diff>
--- a/network-data/LineGeo_Selector.xlsx
+++ b/network-data/LineGeo_Selector.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spenceregan/Repos/CU/Distribution_Systems/Project1/ECEN5437-Proj1/network-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C106E9-C4DC-7C4D-A7C1-417D81F17639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63195EC3-1667-1E49-A1A2-3B0D7D73F202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6640" yWindow="760" windowWidth="23600" windowHeight="17440" activeTab="2" xr2:uid="{7AEC5E2E-397B-8345-871E-9ED757579969}"/>
+    <workbookView xWindow="6640" yWindow="760" windowWidth="23600" windowHeight="17440" activeTab="5" xr2:uid="{7AEC5E2E-397B-8345-871E-9ED757579969}"/>
   </bookViews>
   <sheets>
     <sheet name="Buses" sheetId="7" r:id="rId1"/>
     <sheet name="LineGeometry" sheetId="1" r:id="rId2"/>
     <sheet name="Lines" sheetId="6" r:id="rId3"/>
-    <sheet name="Ref" sheetId="5" r:id="rId4"/>
-    <sheet name="Wire_data" sheetId="2" r:id="rId5"/>
-    <sheet name="CN_data" sheetId="3" r:id="rId6"/>
-    <sheet name="TS_data" sheetId="4" r:id="rId7"/>
+    <sheet name="Loads" sheetId="8" r:id="rId4"/>
+    <sheet name="Ref" sheetId="5" r:id="rId5"/>
+    <sheet name="WireData" sheetId="2" r:id="rId6"/>
+    <sheet name="CNData" sheetId="3" r:id="rId7"/>
+    <sheet name="TSData" sheetId="4" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="170">
   <si>
     <t>OH3p</t>
   </si>
@@ -59,12 +60,6 @@
     <t>UG1p</t>
   </si>
   <si>
-    <t>phase conductor</t>
-  </si>
-  <si>
-    <t>neutral conductor</t>
-  </si>
-  <si>
     <t>Size</t>
   </si>
   <si>
@@ -383,15 +378,6 @@
     <t>4_z</t>
   </si>
   <si>
-    <t>node a</t>
-  </si>
-  <si>
-    <t>node b</t>
-  </si>
-  <si>
-    <t>line type</t>
-  </si>
-  <si>
     <t>n0</t>
   </si>
   <si>
@@ -540,6 +526,33 @@
   </si>
   <si>
     <t>n28</t>
+  </si>
+  <si>
+    <t>kW</t>
+  </si>
+  <si>
+    <t>kVAr</t>
+  </si>
+  <si>
+    <t>n44</t>
+  </si>
+  <si>
+    <t>LineGeometry</t>
+  </si>
+  <si>
+    <t>bus1</t>
+  </si>
+  <si>
+    <t>bus2</t>
+  </si>
+  <si>
+    <t>phase_conductor</t>
+  </si>
+  <si>
+    <t>neutral_conductor</t>
+  </si>
+  <si>
+    <t>runits</t>
   </si>
 </sst>
 </file>
@@ -632,7 +645,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -656,12 +669,109 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="49">
+  <dxfs count="54">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1717,16 +1827,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{43240ADB-710B-E440-9B4B-064F1493B981}" name="Buses" displayName="Buses" ref="A1:C46" totalsRowShown="0" dataDxfId="0">
-  <autoFilter ref="A1:C46" xr:uid="{43240ADB-710B-E440-9B4B-064F1493B981}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{43240ADB-710B-E440-9B4B-064F1493B981}" name="Buses" displayName="Buses" ref="A1:C47" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A1:C47" xr:uid="{43240ADB-710B-E440-9B4B-064F1493B981}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{37E9F5EA-051D-BE40-B622-31D4B83CE6AA}" name="Bus" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{41D4B11A-15CC-A540-9052-95C4F3006357}" name="Graph_Loc_x" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{871540F1-C33C-6346-9F71-C67E6A5F5C63}" name="Graph_Loc_y" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{37E9F5EA-051D-BE40-B622-31D4B83CE6AA}" name="Bus" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{41D4B11A-15CC-A540-9052-95C4F3006357}" name="Graph_Loc_x" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{871540F1-C33C-6346-9F71-C67E6A5F5C63}" name="Graph_Loc_y" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1754,8 +1864,8 @@
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{2280FF94-C83E-444E-8E42-3510351A4DF6}" name="LineGeo"/>
     <tableColumn id="2" xr3:uid="{3DDFC765-300B-7846-9085-AB03B6A261F4}" name="Type"/>
-    <tableColumn id="3" xr3:uid="{02F910B6-BE16-CE4C-89A1-71F43049235B}" name="phase conductor"/>
-    <tableColumn id="4" xr3:uid="{520CD3FE-AB23-3943-8829-73CAAC013F53}" name="neutral conductor" dataDxfId="28">
+    <tableColumn id="3" xr3:uid="{02F910B6-BE16-CE4C-89A1-71F43049235B}" name="phase_conductor"/>
+    <tableColumn id="4" xr3:uid="{520CD3FE-AB23-3943-8829-73CAAC013F53}" name="neutral_conductor" dataDxfId="33">
       <calculatedColumnFormula>IF(LineGeo[[#This Row],[Type]]="OH",1,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="13" xr3:uid="{DE9BDE1B-5E39-604D-9957-E0C3A3473BC8}" name="Phases"/>
@@ -1775,7 +1885,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{12D9EB82-8B48-7449-95A6-3BE76017FBF1}" name="Table7" displayName="Table7" ref="A1:E38" totalsRowShown="0" headerRowDxfId="5" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{12D9EB82-8B48-7449-95A6-3BE76017FBF1}" name="Table7" displayName="Table7" ref="A1:E38" totalsRowShown="0" headerRowDxfId="10" dataDxfId="11">
   <autoFilter ref="A1:E38" xr:uid="{12D9EB82-8B48-7449-95A6-3BE76017FBF1}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1784,17 +1894,33 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{B526205E-98EF-F34B-B24D-F8218A008415}" name="node a" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{D2CD9147-9358-C04D-8316-3FB3A9A16CB0}" name="node b" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{99BA8C9D-330B-A24F-BC6C-A45D5466D8F3}" name="Length" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{24B6C05D-6629-B248-BB9C-1AF1BAA7ADB7}" name="line type" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{CDFF2292-878E-CE4B-BF6E-6CE7168C35B8}" name="Units" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{B526205E-98EF-F34B-B24D-F8218A008415}" name="bus1" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{D2CD9147-9358-C04D-8316-3FB3A9A16CB0}" name="bus2" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{99BA8C9D-330B-A24F-BC6C-A45D5466D8F3}" name="Length" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{24B6C05D-6629-B248-BB9C-1AF1BAA7ADB7}" name="LineGeometry" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{CDFF2292-878E-CE4B-BF6E-6CE7168C35B8}" name="Units" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{CDAC5F4F-CC5E-714A-A10A-32F2E90176D7}" name="Table9" displayName="Table9" ref="A1:C28" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A1:C28" xr:uid="{CDAC5F4F-CC5E-714A-A10A-32F2E90176D7}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{49EC89B8-2142-0A4A-B8EF-264BCDD715FA}" name="Bus" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{13C1D0C2-6357-484D-ADEB-105711D6B1A5}" name="kW" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{A5C493EA-CBB6-854A-A97A-1FDDCAB8D84F}" name="kVAr" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{045739EA-1F28-0E41-AB74-C2C34C8286AB}" name="Type" displayName="Type" ref="A1:A3" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{CF2DB599-7394-FB45-9EE6-02953B6FA5D3}" name="Column1"/>
@@ -1803,7 +1929,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{197E6DD9-1E95-E144-A54E-7BD8668CA6E8}" name="Units" displayName="Units" ref="C2:C8" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{D4C1F671-A0A2-9147-89DB-D689DF977101}" name="Column1"/>
@@ -1812,7 +1938,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E4FB8847-4274-D04D-A64C-15B4CD5C8D60}" name="OH" displayName="OH" ref="A1:K100" totalsRowShown="0">
   <autoFilter ref="A1:K100" xr:uid="{E4FB8847-4274-D04D-A64C-15B4CD5C8D60}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -1828,23 +1954,23 @@
     <filterColumn colId="10" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{E903BA16-38F3-EE44-A1B4-2B0F344DDB1D}" name="Type" dataDxfId="20">
+    <tableColumn id="1" xr3:uid="{E903BA16-38F3-EE44-A1B4-2B0F344DDB1D}" name="Type" dataDxfId="25">
       <calculatedColumnFormula>_xlfn.CONCAT(OH[[#This Row],[Size]], "_",OH[[#This Row],[Stranding]], "_", OH[[#This Row],[Material]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{B69CA351-3694-B545-8563-7479CF50BC67}" name="Size" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{B69CA351-3694-B545-8563-7479CF50BC67}" name="Size" dataDxfId="24"/>
     <tableColumn id="3" xr3:uid="{3576FC0F-75EE-6F4B-B709-5C5715FE540E}" name="Stranding"/>
     <tableColumn id="4" xr3:uid="{C31618D9-7DA8-804A-A013-69A802FF7774}" name="Material"/>
     <tableColumn id="5" xr3:uid="{804C85FC-06A5-4645-A278-FD8271A5F0ED}" name="Diam"/>
     <tableColumn id="6" xr3:uid="{ED80EC98-63E4-C94C-BAF3-F13294EE8381}" name="GMRac"/>
     <tableColumn id="7" xr3:uid="{41A91B17-FB89-1F4F-899A-3761661447FD}" name="rac"/>
     <tableColumn id="8" xr3:uid="{C9144B25-D7C0-D444-8605-CEBD77A9171D}" name="normamps"/>
-    <tableColumn id="13" xr3:uid="{041E70E4-975E-254A-81CF-95C5EF9E73D2}" name="GMRunits" dataDxfId="27">
+    <tableColumn id="13" xr3:uid="{041E70E4-975E-254A-81CF-95C5EF9E73D2}" name="GMRunits" dataDxfId="32">
       <calculatedColumnFormula>"ft"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{2AEFB39D-D6D8-D14D-A990-9BB4F5164639}" name="Runits" dataDxfId="26">
+    <tableColumn id="14" xr3:uid="{2AEFB39D-D6D8-D14D-A990-9BB4F5164639}" name="runits" dataDxfId="31">
       <calculatedColumnFormula>"mi"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{21A61F38-5A94-2142-A9A8-D6E0BB77AB1E}" name="Size_Material" dataDxfId="18">
+    <tableColumn id="15" xr3:uid="{21A61F38-5A94-2142-A9A8-D6E0BB77AB1E}" name="Size_Material" dataDxfId="23">
       <calculatedColumnFormula>_xlfn.CONCAT(OH[[#This Row],[Size]], "_", OH[[#This Row],[Material]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1852,8 +1978,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{661274D6-1D68-5542-8D94-45D5C86243F5}" name="CN" displayName="CN" ref="A1:T19" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39" tableBorderDxfId="48">
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{661274D6-1D68-5542-8D94-45D5C86243F5}" name="CN" displayName="CN" ref="A1:T19" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44" tableBorderDxfId="53">
   <autoFilter ref="A1:T19" xr:uid="{661274D6-1D68-5542-8D94-45D5C86243F5}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1877,46 +2003,46 @@
     <filterColumn colId="19" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="20">
-    <tableColumn id="9" xr3:uid="{869F190C-19C4-2243-84CA-F6CB8F4281C2}" name="Type" dataDxfId="31">
+    <tableColumn id="9" xr3:uid="{869F190C-19C4-2243-84CA-F6CB8F4281C2}" name="Type" dataDxfId="36">
       <calculatedColumnFormula>_xlfn.CONCAT(CN[[#This Row],[Neutral Ampacity]], "_", CN[[#This Row],[Conductor Size]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{1DFBB787-8CEC-A946-969E-C8B3E35D5AEB}" name="Neutral Ampacity" dataDxfId="47"/>
-    <tableColumn id="2" xr3:uid="{EFDAEEF3-E5BA-4B49-BA44-2340320EA290}" name="Conductor Size" dataDxfId="46"/>
-    <tableColumn id="18" xr3:uid="{703A2A0A-5882-4349-9ACB-A05C1C032238}" name="Phase Conductor Name" dataDxfId="17">
+    <tableColumn id="1" xr3:uid="{1DFBB787-8CEC-A946-969E-C8B3E35D5AEB}" name="Neutral Ampacity" dataDxfId="52"/>
+    <tableColumn id="2" xr3:uid="{EFDAEEF3-E5BA-4B49-BA44-2340320EA290}" name="Conductor Size" dataDxfId="51"/>
+    <tableColumn id="18" xr3:uid="{703A2A0A-5882-4349-9ACB-A05C1C032238}" name="Phase Conductor Name" dataDxfId="22">
       <calculatedColumnFormula>_xlfn.XLOOKUP(_xlfn.CONCAT(LEFT(CN[[#This Row],[Conductor Size]], SEARCH("(", CN[[#This Row],[Conductor Size]])-1), "_AA"), OH[Size_Material], OH[Type], NA(),-1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8E5F5E70-58CE-0D4E-A970-1B53EA80FE07}" name="Diameter Over Insulation (in)" dataDxfId="45"/>
-    <tableColumn id="4" xr3:uid="{D154B6B5-D516-AC44-879B-B0BC6ACADF64}" name="Diameter Over Screen (in)" dataDxfId="44"/>
-    <tableColumn id="5" xr3:uid="{51092775-E14C-4945-BD12-6F609313AC1A}" name="Outside Diameter" dataDxfId="43"/>
-    <tableColumn id="6" xr3:uid="{FE25AF87-2C02-C642-B28A-81AF2224011F}" name="Copper Neutral" dataDxfId="42"/>
-    <tableColumn id="7" xr3:uid="{167EFF3D-5388-5C47-9405-F0CE90C78333}" name="Ampacity in Underground Duct (A)" dataDxfId="41"/>
-    <tableColumn id="8" xr3:uid="{D4CA2780-FAB4-FE44-BAA2-A16B53A68DE8}" name="Voltage Rating (kV)" dataDxfId="25"/>
-    <tableColumn id="11" xr3:uid="{830817DB-B122-D444-8DFC-58C1CE7D7901}" name="Neutral Strand AWG" dataDxfId="23" dataCellStyle="Percent">
+    <tableColumn id="3" xr3:uid="{8E5F5E70-58CE-0D4E-A970-1B53EA80FE07}" name="Diameter Over Insulation (in)" dataDxfId="50"/>
+    <tableColumn id="4" xr3:uid="{D154B6B5-D516-AC44-879B-B0BC6ACADF64}" name="Diameter Over Screen (in)" dataDxfId="49"/>
+    <tableColumn id="5" xr3:uid="{51092775-E14C-4945-BD12-6F609313AC1A}" name="Outside Diameter" dataDxfId="48"/>
+    <tableColumn id="6" xr3:uid="{FE25AF87-2C02-C642-B28A-81AF2224011F}" name="Copper Neutral" dataDxfId="47"/>
+    <tableColumn id="7" xr3:uid="{167EFF3D-5388-5C47-9405-F0CE90C78333}" name="Ampacity in Underground Duct (A)" dataDxfId="46"/>
+    <tableColumn id="8" xr3:uid="{D4CA2780-FAB4-FE44-BAA2-A16B53A68DE8}" name="Voltage Rating (kV)" dataDxfId="30"/>
+    <tableColumn id="11" xr3:uid="{830817DB-B122-D444-8DFC-58C1CE7D7901}" name="Neutral Strand AWG" dataDxfId="28" dataCellStyle="Percent">
       <calculatedColumnFormula>VALUE(RIGHT(CN[[#This Row],[Copper Neutral]],2))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{A0775550-BA03-5542-A01E-64482C59971C}" name="Rstrand" dataDxfId="24">
+    <tableColumn id="10" xr3:uid="{A0775550-BA03-5542-A01E-64482C59971C}" name="Rstrand" dataDxfId="29">
       <calculatedColumnFormula>_xlfn.XLOOKUP(CN[[#This Row],[Neutral Strand AWG]], OH[Size], OH[rac])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{4B541559-291A-4941-9353-F59C621A9E18}" name="k" dataDxfId="22">
+    <tableColumn id="12" xr3:uid="{4B541559-291A-4941-9353-F59C621A9E18}" name="k" dataDxfId="27">
       <calculatedColumnFormula>VALUE(LEFT(CN[[#This Row],[Copper Neutral]], SEARCH(" ",CN[[#This Row],[Copper Neutral]])-1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{60128454-1EE5-9C4B-9AA2-D0CE6F9C4CF7}" name="GMRac" dataDxfId="16">
+    <tableColumn id="13" xr3:uid="{60128454-1EE5-9C4B-9AA2-D0CE6F9C4CF7}" name="GMRac" dataDxfId="21">
       <calculatedColumnFormula>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]], OH[Type], OH[GMRac])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{AA242217-BC74-AB48-8D9A-86A3970B8399}" name="GmrStrand" dataDxfId="15">
+    <tableColumn id="14" xr3:uid="{AA242217-BC74-AB48-8D9A-86A3970B8399}" name="GmrStrand" dataDxfId="20">
       <calculatedColumnFormula>_xlfn.XLOOKUP(CN[[#This Row],[Neutral Strand AWG]], OH[Size], OH[GMRac])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{BDF03C79-D2AE-394A-9557-0FEAE0AA392C}" name="GMRUnits" dataDxfId="21"/>
-    <tableColumn id="16" xr3:uid="{E6B7FA4C-2968-AE41-84BD-9EA25CF9A089}" name="Rac" dataDxfId="14">
+    <tableColumn id="15" xr3:uid="{BDF03C79-D2AE-394A-9557-0FEAE0AA392C}" name="GMRUnits" dataDxfId="26"/>
+    <tableColumn id="16" xr3:uid="{E6B7FA4C-2968-AE41-84BD-9EA25CF9A089}" name="Rac" dataDxfId="19">
       <calculatedColumnFormula>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[rac])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{60CA6D09-ACAD-FA47-9A7F-D8BCB54C2191}" name="Runits" dataDxfId="13">
-      <calculatedColumnFormula>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[Runits])</calculatedColumnFormula>
+    <tableColumn id="17" xr3:uid="{60CA6D09-ACAD-FA47-9A7F-D8BCB54C2191}" name="Runits" dataDxfId="18">
+      <calculatedColumnFormula>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[runits])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{A335B60A-8482-494F-9920-64B3CC7615EB}" name="Diam" dataDxfId="12">
+    <tableColumn id="19" xr3:uid="{A335B60A-8482-494F-9920-64B3CC7615EB}" name="Diam" dataDxfId="17">
       <calculatedColumnFormula>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[Diam])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{D37687B3-1580-7845-A711-F39AB1A49147}" name="normamps" dataDxfId="11">
+    <tableColumn id="20" xr3:uid="{D37687B3-1580-7845-A711-F39AB1A49147}" name="normamps" dataDxfId="16">
       <calculatedColumnFormula>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[normamps])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1924,8 +2050,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{13D01E9F-2651-EF45-A492-F190721E7BE9}" name="TS" displayName="TS" ref="A1:G10" totalsRowShown="0" headerRowDxfId="32" dataDxfId="33">
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{13D01E9F-2651-EF45-A492-F190721E7BE9}" name="TS" displayName="TS" ref="A1:G10" totalsRowShown="0" headerRowDxfId="37" dataDxfId="38">
   <autoFilter ref="A1:G10" xr:uid="{13D01E9F-2651-EF45-A492-F190721E7BE9}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1936,13 +2062,13 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{19CDDA2D-9812-404F-A70E-F8C42AD526DB}" name="Type" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{C1A0B38B-F04B-0A4C-913A-B68BB0D6C78E}" name="Diameter Over Insulation (in)" dataDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{D6D141BB-2B57-4B4B-8667-6762392800DB}" name="Diameter Over Screen (in)" dataDxfId="38"/>
-    <tableColumn id="4" xr3:uid="{401114E4-AC5F-DA47-A949-534E36354F8D}" name="Jacket Thickness (mils)" dataDxfId="37"/>
-    <tableColumn id="5" xr3:uid="{244E8C6F-E27A-B344-A042-CF80AF18FA7C}" name="Outside Diameter" dataDxfId="36"/>
-    <tableColumn id="6" xr3:uid="{D80F22EC-CB8C-E549-AC7C-4BA81E9F5164}" name="Ampacity in UG Duct (A)" dataDxfId="35"/>
-    <tableColumn id="7" xr3:uid="{A989CB28-4027-F249-A88C-9A2D66CB1557}" name="Rated Voltage (kV)" dataDxfId="34"/>
+    <tableColumn id="1" xr3:uid="{19CDDA2D-9812-404F-A70E-F8C42AD526DB}" name="Type" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{C1A0B38B-F04B-0A4C-913A-B68BB0D6C78E}" name="Diameter Over Insulation (in)" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{D6D141BB-2B57-4B4B-8667-6762392800DB}" name="Diameter Over Screen (in)" dataDxfId="43"/>
+    <tableColumn id="4" xr3:uid="{401114E4-AC5F-DA47-A949-534E36354F8D}" name="Jacket Thickness (mils)" dataDxfId="42"/>
+    <tableColumn id="5" xr3:uid="{244E8C6F-E27A-B344-A042-CF80AF18FA7C}" name="Outside Diameter" dataDxfId="41"/>
+    <tableColumn id="6" xr3:uid="{D80F22EC-CB8C-E549-AC7C-4BA81E9F5164}" name="Ampacity in UG Duct (A)" dataDxfId="40"/>
+    <tableColumn id="7" xr3:uid="{A989CB28-4027-F249-A88C-9A2D66CB1557}" name="Rated Voltage (kV)" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2245,10 +2371,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC2FAF4C-A38A-5148-8683-163D7FE8FD2D}">
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A2" sqref="A2:A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2258,18 +2384,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B2" s="17">
         <v>4</v>
@@ -2280,7 +2406,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B3" s="17">
         <v>4</v>
@@ -2291,7 +2417,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B4" s="17">
         <v>0</v>
@@ -2302,7 +2428,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B5" s="17">
         <v>0</v>
@@ -2313,7 +2439,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B6" s="17">
         <v>0</v>
@@ -2324,7 +2450,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B7" s="17">
         <v>0</v>
@@ -2335,7 +2461,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B8" s="17">
         <v>1</v>
@@ -2346,7 +2472,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B9" s="17">
         <v>1</v>
@@ -2357,7 +2483,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B10" s="17">
         <v>1</v>
@@ -2368,7 +2494,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B11" s="17">
         <v>1</v>
@@ -2379,7 +2505,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B12" s="17">
         <v>2</v>
@@ -2390,7 +2516,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B13" s="17">
         <v>2</v>
@@ -2401,7 +2527,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B14" s="17">
         <v>2</v>
@@ -2412,7 +2538,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B15" s="17">
         <v>2</v>
@@ -2423,7 +2549,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B16" s="17">
         <v>2</v>
@@ -2434,7 +2560,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B17" s="17">
         <v>3</v>
@@ -2445,7 +2571,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B18" s="17">
         <v>3</v>
@@ -2456,7 +2582,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B19" s="17">
         <v>3</v>
@@ -2467,7 +2593,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B20" s="17">
         <v>3</v>
@@ -2478,7 +2604,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B21" s="17">
         <v>3</v>
@@ -2489,7 +2615,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B22" s="17">
         <v>3</v>
@@ -2500,7 +2626,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B23" s="17">
         <v>4</v>
@@ -2511,7 +2637,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B24" s="17">
         <v>3</v>
@@ -2522,7 +2648,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B25" s="17">
         <v>3</v>
@@ -2533,7 +2659,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B26" s="17">
         <v>3</v>
@@ -2544,7 +2670,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B27" s="17">
         <v>4</v>
@@ -2555,7 +2681,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B28" s="17">
         <v>4</v>
@@ -2566,7 +2692,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B29" s="17">
         <v>4</v>
@@ -2577,7 +2703,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B30" s="17">
         <v>4</v>
@@ -2588,7 +2714,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B31" s="17">
         <v>4</v>
@@ -2599,7 +2725,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B32" s="17">
         <v>5</v>
@@ -2610,7 +2736,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B33" s="17">
         <v>5</v>
@@ -2621,7 +2747,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="17" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B34" s="17">
         <v>5</v>
@@ -2632,7 +2758,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B35" s="17">
         <v>5</v>
@@ -2643,7 +2769,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B36" s="17">
         <v>5</v>
@@ -2654,7 +2780,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="17" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B37" s="17">
         <v>5</v>
@@ -2665,7 +2791,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="17" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B38" s="17">
         <v>6</v>
@@ -2676,7 +2802,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="17" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B39" s="17">
         <v>6</v>
@@ -2687,7 +2813,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="17" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B40" s="17">
         <v>6</v>
@@ -2698,7 +2824,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="17" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B41" s="17">
         <v>6</v>
@@ -2709,7 +2835,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="17" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B42" s="17">
         <v>5</v>
@@ -2720,7 +2846,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="17" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B43" s="17">
         <v>5</v>
@@ -2731,7 +2857,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="17" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B44" s="17">
         <v>5</v>
@@ -2742,7 +2868,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="17" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B45" s="17">
         <v>6</v>
@@ -2753,13 +2879,24 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="17" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B46" s="17">
         <v>6</v>
       </c>
       <c r="C46" s="17">
         <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="B47" s="17">
+        <v>3</v>
+      </c>
+      <c r="C47" s="17">
+        <v>-1</v>
       </c>
     </row>
   </sheetData>
@@ -2775,7 +2912,7 @@
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2789,49 +2926,49 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>167</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>168</v>
       </c>
       <c r="E1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I1" t="s">
         <v>105</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>106</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>107</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>108</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>109</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>110</v>
       </c>
-      <c r="M1" t="s">
-        <v>111</v>
-      </c>
-      <c r="N1" t="s">
-        <v>112</v>
-      </c>
       <c r="O1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -2839,13 +2976,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -2878,7 +3015,7 @@
         <v>24</v>
       </c>
       <c r="O2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
@@ -2886,10 +3023,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -2910,7 +3047,7 @@
         <v>28</v>
       </c>
       <c r="O3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -2918,13 +3055,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -2945,7 +3082,7 @@
         <v>24</v>
       </c>
       <c r="O4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -2953,13 +3090,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -2988,7 +3125,7 @@
         <v>-4</v>
       </c>
       <c r="O5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -2996,13 +3133,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -3017,7 +3154,7 @@
         <v>-4</v>
       </c>
       <c r="O6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -3046,8 +3183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3B959F-BA38-1C45-8F28-8937DDD91101}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3058,27 +3195,27 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
-        <v>113</v>
+        <v>165</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>114</v>
+        <v>166</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>115</v>
+        <v>164</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C2" s="17">
         <v>15840</v>
@@ -3087,15 +3224,15 @@
         <v>0</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C3" s="17">
         <v>15840</v>
@@ -3104,15 +3241,15 @@
         <v>0</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C4" s="17">
         <v>15840</v>
@@ -3121,15 +3258,15 @@
         <v>0</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C5" s="17">
         <v>15840</v>
@@ -3138,15 +3275,15 @@
         <v>0</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C6" s="17">
         <v>15840</v>
@@ -3155,15 +3292,15 @@
         <v>0</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C7" s="17">
         <v>15840</v>
@@ -3172,15 +3309,15 @@
         <v>0</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C8" s="17">
         <v>15840</v>
@@ -3189,15 +3326,15 @@
         <v>2</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C9" s="17">
         <v>15840</v>
@@ -3206,15 +3343,15 @@
         <v>0</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C10" s="17">
         <v>15840</v>
@@ -3223,15 +3360,15 @@
         <v>0</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C11" s="17">
         <v>15840</v>
@@ -3240,15 +3377,15 @@
         <v>0</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C12" s="17">
         <v>100</v>
@@ -3257,15 +3394,15 @@
         <v>1</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C13" s="17">
         <v>100</v>
@@ -3274,15 +3411,15 @@
         <v>1</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C14" s="17">
         <v>100</v>
@@ -3291,15 +3428,15 @@
         <v>1</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C15" s="17">
         <v>100</v>
@@ -3308,15 +3445,15 @@
         <v>1</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C16" s="17">
         <v>100</v>
@@ -3325,15 +3462,15 @@
         <v>1</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C17" s="17">
         <v>100</v>
@@ -3342,15 +3479,15 @@
         <v>1</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C18" s="17">
         <v>100</v>
@@ -3359,15 +3496,15 @@
         <v>1</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C19" s="17">
         <v>100</v>
@@ -3376,15 +3513,15 @@
         <v>1</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C20" s="17">
         <v>100</v>
@@ -3393,15 +3530,15 @@
         <v>1</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C21" s="17">
         <v>100</v>
@@ -3410,15 +3547,15 @@
         <v>1</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C22" s="17">
         <v>100</v>
@@ -3427,15 +3564,15 @@
         <v>1</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C23" s="17">
         <v>15840</v>
@@ -3444,15 +3581,15 @@
         <v>2</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C24" s="17">
         <v>15840</v>
@@ -3461,15 +3598,15 @@
         <v>2</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C25" s="17">
         <v>100</v>
@@ -3478,15 +3615,15 @@
         <v>2</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C26" s="17">
         <v>100</v>
@@ -3495,15 +3632,15 @@
         <v>2</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C27" s="17">
         <v>100</v>
@@ -3512,15 +3649,15 @@
         <v>2</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C28" s="17">
         <v>100</v>
@@ -3529,15 +3666,15 @@
         <v>2</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C29" s="17">
         <v>15840</v>
@@ -3546,15 +3683,15 @@
         <v>3</v>
       </c>
       <c r="E29" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C30" s="17">
         <v>15840</v>
@@ -3563,15 +3700,15 @@
         <v>3</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C31" s="17">
         <v>15840</v>
@@ -3580,15 +3717,15 @@
         <v>3</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C32" s="17">
         <v>15840</v>
@@ -3597,15 +3734,15 @@
         <v>3</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C33" s="17">
         <v>15840</v>
@@ -3614,15 +3751,15 @@
         <v>3</v>
       </c>
       <c r="E33" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="17" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C34" s="17">
         <v>15840</v>
@@ -3631,15 +3768,15 @@
         <v>3</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="B35" s="17" t="s">
         <v>147</v>
-      </c>
-      <c r="B35" s="17" t="s">
-        <v>152</v>
       </c>
       <c r="C35" s="17">
         <v>15840</v>
@@ -3648,15 +3785,15 @@
         <v>4</v>
       </c>
       <c r="E35" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C36" s="17">
         <v>15840</v>
@@ -3665,15 +3802,15 @@
         <v>4</v>
       </c>
       <c r="E36" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="17" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C37" s="17">
         <v>15840</v>
@@ -3682,15 +3819,15 @@
         <v>4</v>
       </c>
       <c r="E37" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="17" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C38" s="17">
         <v>15840</v>
@@ -3699,16 +3836,19 @@
         <v>4</v>
       </c>
       <c r="E38" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Undefined LineGeometery" error="Use a defined LineGeometry, or make a new geometry" sqref="D2:D38" xr:uid="{FB0F891B-6660-7D4C-AC5B-0346D13948B8}">
       <formula1>INDIRECT("LineGeo[LineGeo]")</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E38" xr:uid="{B4F4E3E6-2E21-244D-ADFB-DDC8B351103E}">
       <formula1>INDIRECT("Units")</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:B38" xr:uid="{49F4DC04-A3BE-1845-8DA3-7CDFAE95089C}">
+      <formula1>INDIRECT("Buses[Bus]")</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3719,6 +3859,337 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CE5CFF8-7828-B948-AF88-0BAE820E01A6}">
+  <dimension ref="A1:C28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" s="17">
+        <v>7</v>
+      </c>
+      <c r="C2" s="17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" s="17">
+        <v>6</v>
+      </c>
+      <c r="C3" s="17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="17">
+        <v>15</v>
+      </c>
+      <c r="C4" s="17">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" s="17">
+        <v>10</v>
+      </c>
+      <c r="C5" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="B6" s="17">
+        <v>50</v>
+      </c>
+      <c r="C6" s="17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="B7" s="17">
+        <v>2</v>
+      </c>
+      <c r="C7" s="17">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="B8" s="17">
+        <v>3</v>
+      </c>
+      <c r="C8" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="B9" s="17">
+        <v>10</v>
+      </c>
+      <c r="C9" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="17">
+        <v>70</v>
+      </c>
+      <c r="C10" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="B11" s="17">
+        <v>30</v>
+      </c>
+      <c r="C11" s="17">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="B12" s="17">
+        <v>60</v>
+      </c>
+      <c r="C12" s="17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="B13" s="17">
+        <v>60</v>
+      </c>
+      <c r="C13" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="B14" s="17">
+        <v>130</v>
+      </c>
+      <c r="C14" s="17">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="B15" s="17">
+        <v>90</v>
+      </c>
+      <c r="C15" s="17">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="B16" s="17">
+        <v>115</v>
+      </c>
+      <c r="C16" s="17">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B17" s="17">
+        <v>66</v>
+      </c>
+      <c r="C17" s="17">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="B18" s="17">
+        <v>70</v>
+      </c>
+      <c r="C18" s="17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="B19" s="17">
+        <v>25</v>
+      </c>
+      <c r="C19" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="B20" s="17">
+        <v>35</v>
+      </c>
+      <c r="C20" s="17">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="B21" s="17">
+        <v>30</v>
+      </c>
+      <c r="C21" s="17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="B22" s="17">
+        <v>95</v>
+      </c>
+      <c r="C22" s="17">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="B23" s="17">
+        <v>40</v>
+      </c>
+      <c r="C23" s="17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="B24" s="17">
+        <v>7</v>
+      </c>
+      <c r="C24" s="17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="B25" s="17">
+        <v>6</v>
+      </c>
+      <c r="C25" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="B26" s="17">
+        <v>7</v>
+      </c>
+      <c r="C26" s="17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="B27" s="17">
+        <v>14</v>
+      </c>
+      <c r="C27" s="17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="B28" s="17">
+        <v>140</v>
+      </c>
+      <c r="C28" s="17">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A28" xr:uid="{2CD306AF-C17F-0245-A541-447F0C38ED7C}">
+      <formula1>INDIRECT("Buses[Bus]")</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37ABA1BE-A562-EA4D-912C-91965FAA05A8}">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -3730,48 +4201,48 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -3783,12 +4254,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5904AC-ECAC-4945-B9B6-B220AC818209}">
   <dimension ref="A1:N100"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3805,37 +4276,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
       <c r="E1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" t="s">
         <v>98</v>
       </c>
-      <c r="F1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J1" t="s">
+        <v>169</v>
+      </c>
+      <c r="K1" t="s">
         <v>100</v>
-      </c>
-      <c r="H1" t="s">
-        <v>99</v>
-      </c>
-      <c r="I1" t="s">
-        <v>101</v>
-      </c>
-      <c r="J1" t="s">
-        <v>90</v>
-      </c>
-      <c r="K1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -3847,7 +4318,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E2">
         <v>0.35499999999999998</v>
@@ -3883,10 +4354,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E3">
         <v>0.32800000000000001</v>
@@ -3922,10 +4393,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E4">
         <v>0.32800000000000001</v>
@@ -3961,10 +4432,10 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E5">
         <v>0.316</v>
@@ -4000,10 +4471,10 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E6">
         <v>0.29199999999999998</v>
@@ -4039,10 +4510,10 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E7">
         <v>0.32500000000000001</v>
@@ -4078,10 +4549,10 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E8">
         <v>0.25800000000000001</v>
@@ -4117,10 +4588,10 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E9">
         <v>0.29199999999999998</v>
@@ -4156,10 +4627,10 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E10">
         <v>0.28100000000000003</v>
@@ -4195,10 +4666,10 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E11">
         <v>0.22900000000000001</v>
@@ -4234,10 +4705,10 @@
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E12">
         <v>0.25</v>
@@ -4273,10 +4744,10 @@
         <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E13">
         <v>0.25700000000000001</v>
@@ -4312,10 +4783,10 @@
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E14">
         <v>0.20399999999999999</v>
@@ -4351,10 +4822,10 @@
         <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E15">
         <v>0.23200000000000001</v>
@@ -4390,10 +4861,10 @@
         <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E16">
         <v>0.223</v>
@@ -4429,10 +4900,10 @@
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D17" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E17">
         <v>0.18190000000000001</v>
@@ -4468,10 +4939,10 @@
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D18" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E18">
         <v>0.19800000000000001</v>
@@ -4507,10 +4978,10 @@
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D19" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E19">
         <v>0.16200000000000001</v>
@@ -4546,10 +5017,10 @@
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D20" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E20">
         <v>0.184</v>
@@ -4585,10 +5056,10 @@
         <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E21">
         <v>0.14430000000000001</v>
@@ -4624,10 +5095,10 @@
         <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D22" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E22">
         <v>0.1285</v>
@@ -4663,10 +5134,10 @@
         <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D23" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E23">
         <v>0.1144</v>
@@ -4702,10 +5173,10 @@
         <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E24">
         <v>0.1019</v>
@@ -4741,10 +5212,10 @@
         <v>12</v>
       </c>
       <c r="C25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D25" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E25">
         <v>8.0799999999999997E-2</v>
@@ -4780,10 +5251,10 @@
         <v>14</v>
       </c>
       <c r="C26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D26" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E26">
         <v>6.4100000000000004E-2</v>
@@ -4819,10 +5290,10 @@
         <v>16</v>
       </c>
       <c r="C27" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D27" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E27">
         <v>5.0799999999999998E-2</v>
@@ -4858,10 +5329,10 @@
         <v>18</v>
       </c>
       <c r="C28" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D28" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E28">
         <v>4.0300000000000002E-2</v>
@@ -4897,10 +5368,10 @@
         <v>19</v>
       </c>
       <c r="C29" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D29" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E29">
         <v>3.5900000000000001E-2</v>
@@ -4936,10 +5407,10 @@
         <v>20</v>
       </c>
       <c r="C30" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D30" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E30">
         <v>3.2000000000000001E-2</v>
@@ -4975,10 +5446,10 @@
         <v>22</v>
       </c>
       <c r="C31" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D31" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E31">
         <v>2.53E-2</v>
@@ -5014,10 +5485,10 @@
         <v>24</v>
       </c>
       <c r="C32" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D32" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E32">
         <v>2.01E-2</v>
@@ -5050,10 +5521,10 @@
         <v>1/0__ACSR</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D33" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E33">
         <v>0.39800000000000002</v>
@@ -5086,13 +5557,13 @@
         <v>1/0_7 STRD_Copper</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C34" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D34" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E34">
         <v>0.36799999999999999</v>
@@ -5125,13 +5596,13 @@
         <v>1/0_CLASS A_AA</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C35" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D35" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E35">
         <v>0.36799999999999999</v>
@@ -5164,10 +5635,10 @@
         <v>2/0__ACSR</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D36" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E36">
         <v>0.44700000000000001</v>
@@ -5200,13 +5671,13 @@
         <v>2/0_7 STRD_Copper</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C37" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D37" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E37">
         <v>0.41399999999999998</v>
@@ -5239,13 +5710,13 @@
         <v>2/0_CLASS A_AA</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C38" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D38" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E38">
         <v>0.41399999999999998</v>
@@ -5278,13 +5749,13 @@
         <v>3/0_12 STRD_Copper</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C39" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D39" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E39">
         <v>0.49199999999999999</v>
@@ -5317,13 +5788,13 @@
         <v>3/0_6/1_ACSR</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C40" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D40" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E40">
         <v>0.502</v>
@@ -5356,13 +5827,13 @@
         <v>3/0_7 STRD_Copper</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C41" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D41" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E41">
         <v>0.46400000000000002</v>
@@ -5395,13 +5866,13 @@
         <v>3/0_CLASS A_AA</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C42" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D42" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E42">
         <v>0.46400000000000002</v>
@@ -5434,13 +5905,13 @@
         <v>3/8_INCH STE_Steel</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C43" t="s">
+        <v>21</v>
+      </c>
+      <c r="D43" t="s">
         <v>22</v>
-      </c>
-      <c r="C43" t="s">
-        <v>23</v>
-      </c>
-      <c r="D43" t="s">
-        <v>24</v>
       </c>
       <c r="E43">
         <v>0.375</v>
@@ -5473,13 +5944,13 @@
         <v>4/0_12 STRD_Copper</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C44" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E44">
         <v>0.55200000000000005</v>
@@ -5512,13 +5983,13 @@
         <v>4/0_19 STRD_Copper</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C45" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D45" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E45">
         <v>0.52800000000000002</v>
@@ -5551,13 +6022,13 @@
         <v>4/0_6/1_ACSR</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C46" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D46" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E46">
         <v>0.56299999999999994</v>
@@ -5590,13 +6061,13 @@
         <v>4/0_7 STRD_Copper</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C47" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D47" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E47">
         <v>0.52200000000000002</v>
@@ -5629,13 +6100,13 @@
         <v>4/0_CLASS A_AA</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C48" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D48" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E48">
         <v>0.52200000000000002</v>
@@ -5671,10 +6142,10 @@
         <v>250</v>
       </c>
       <c r="C49" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D49" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E49">
         <v>0.6</v>
@@ -5711,10 +6182,10 @@
         <v>250</v>
       </c>
       <c r="C50" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D50" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E50">
         <v>0.57399999999999995</v>
@@ -5751,10 +6222,10 @@
         <v>250</v>
       </c>
       <c r="C51" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D51" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E51">
         <v>0.56699999999999995</v>
@@ -5791,10 +6262,10 @@
         <v>266.8</v>
       </c>
       <c r="C52" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D52" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E52">
         <v>0.64200000000000002</v>
@@ -5831,10 +6302,10 @@
         <v>266.8</v>
       </c>
       <c r="C53" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D53" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E53">
         <v>0.58599999999999997</v>
@@ -5871,10 +6342,10 @@
         <v>300</v>
       </c>
       <c r="C54" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D54" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E54">
         <v>0.65700000000000003</v>
@@ -5911,10 +6382,10 @@
         <v>300</v>
       </c>
       <c r="C55" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D55" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E55">
         <v>0.629</v>
@@ -5951,10 +6422,10 @@
         <v>300</v>
       </c>
       <c r="C56" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D56" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E56">
         <v>0.68</v>
@@ -5991,10 +6462,10 @@
         <v>300</v>
       </c>
       <c r="C57" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D57" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E57">
         <v>0.7</v>
@@ -6031,10 +6502,10 @@
         <v>300</v>
       </c>
       <c r="C58" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D58" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E58">
         <v>0.629</v>
@@ -6071,10 +6542,10 @@
         <v>336.4</v>
       </c>
       <c r="C59" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D59" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E59">
         <v>0.72099999999999997</v>
@@ -6111,10 +6582,10 @@
         <v>336.4</v>
       </c>
       <c r="C60" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D60" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E60">
         <v>0.74099999999999999</v>
@@ -6151,10 +6622,10 @@
         <v>336.4</v>
       </c>
       <c r="C61" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D61" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E61">
         <v>0.66600000000000004</v>
@@ -6191,10 +6662,10 @@
         <v>350</v>
       </c>
       <c r="C62" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D62" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E62">
         <v>0.71</v>
@@ -6231,10 +6702,10 @@
         <v>350</v>
       </c>
       <c r="C63" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D63" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E63">
         <v>0.67900000000000005</v>
@@ -6271,10 +6742,10 @@
         <v>350</v>
       </c>
       <c r="C64" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D64" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E64">
         <v>0.67900000000000005</v>
@@ -6311,10 +6782,10 @@
         <v>397.5</v>
       </c>
       <c r="C65" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D65" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E65">
         <v>0.78300000000000003</v>
@@ -6351,10 +6822,10 @@
         <v>397.5</v>
       </c>
       <c r="C66" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D66" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E66">
         <v>0.80600000000000005</v>
@@ -6391,10 +6862,10 @@
         <v>397.5</v>
       </c>
       <c r="C67" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D67" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E67">
         <v>0.72399999999999998</v>
@@ -6431,10 +6902,10 @@
         <v>400</v>
       </c>
       <c r="C68" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D68" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E68">
         <v>0.72599999999999998</v>
@@ -6471,10 +6942,10 @@
         <v>450</v>
       </c>
       <c r="C69" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D69" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E69">
         <v>0.77</v>
@@ -6511,10 +6982,10 @@
         <v>450</v>
       </c>
       <c r="C70" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D70" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E70">
         <v>0.77</v>
@@ -6551,10 +7022,10 @@
         <v>477</v>
       </c>
       <c r="C71" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D71" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E71">
         <v>0.85799999999999998</v>
@@ -6591,10 +7062,10 @@
         <v>477</v>
       </c>
       <c r="C72" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D72" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E72">
         <v>0.88300000000000001</v>
@@ -6631,10 +7102,10 @@
         <v>477</v>
       </c>
       <c r="C73" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D73" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E73">
         <v>0.79500000000000004</v>
@@ -6671,10 +7142,10 @@
         <v>500</v>
       </c>
       <c r="C74" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D74" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E74">
         <v>0.81100000000000005</v>
@@ -6711,10 +7182,10 @@
         <v>500</v>
       </c>
       <c r="C75" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D75" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E75">
         <v>0.81399999999999995</v>
@@ -6751,10 +7222,10 @@
         <v>500</v>
       </c>
       <c r="C76" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D76" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E76">
         <v>0.81299999999999994</v>
@@ -6791,10 +7262,10 @@
         <v>556.5</v>
       </c>
       <c r="C77" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D77" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E77">
         <v>0.92700000000000005</v>
@@ -6831,10 +7302,10 @@
         <v>556.5</v>
       </c>
       <c r="C78" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D78" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E78">
         <v>0.95299999999999996</v>
@@ -6871,10 +7342,10 @@
         <v>556.5</v>
       </c>
       <c r="C79" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D79" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E79">
         <v>0.85799999999999998</v>
@@ -6911,10 +7382,10 @@
         <v>600</v>
       </c>
       <c r="C80" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D80" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E80">
         <v>0.89100000000000001</v>
@@ -6951,10 +7422,10 @@
         <v>600</v>
       </c>
       <c r="C81" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D81" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E81">
         <v>0.89100000000000001</v>
@@ -6991,10 +7462,10 @@
         <v>605</v>
       </c>
       <c r="C82" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D82" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E82">
         <v>0.96599999999999997</v>
@@ -7031,10 +7502,10 @@
         <v>605</v>
       </c>
       <c r="C83" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D83" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E83">
         <v>0.95299999999999996</v>
@@ -7071,10 +7542,10 @@
         <v>636</v>
       </c>
       <c r="C84" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D84" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E84">
         <v>0.99</v>
@@ -7111,10 +7582,10 @@
         <v>636</v>
       </c>
       <c r="C85" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D85" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E85">
         <v>1.0189999999999999</v>
@@ -7151,10 +7622,10 @@
         <v>636</v>
       </c>
       <c r="C86" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D86" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E86">
         <v>0.97699999999999998</v>
@@ -7191,10 +7662,10 @@
         <v>636</v>
       </c>
       <c r="C87" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D87" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E87">
         <v>0.91800000000000004</v>
@@ -7231,10 +7702,10 @@
         <v>666.6</v>
       </c>
       <c r="C88" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D88" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E88">
         <v>1</v>
@@ -7271,10 +7742,10 @@
         <v>700</v>
       </c>
       <c r="C89" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D89" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E89">
         <v>0.96299999999999997</v>
@@ -7311,10 +7782,10 @@
         <v>700</v>
       </c>
       <c r="C90" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D90" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E90">
         <v>0.96299999999999997</v>
@@ -7351,10 +7822,10 @@
         <v>715.5</v>
       </c>
       <c r="C91" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D91" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E91">
         <v>1.0509999999999999</v>
@@ -7391,10 +7862,10 @@
         <v>715.5</v>
       </c>
       <c r="C92" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D92" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E92">
         <v>1.081</v>
@@ -7431,10 +7902,10 @@
         <v>715.5</v>
       </c>
       <c r="C93" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D93" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E93">
         <v>1.036</v>
@@ -7471,10 +7942,10 @@
         <v>715.5</v>
       </c>
       <c r="C94" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D94" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E94">
         <v>0.97399999999999998</v>
@@ -7511,10 +7982,10 @@
         <v>750</v>
       </c>
       <c r="C95" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D95" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E95">
         <v>0.997</v>
@@ -7551,10 +8022,10 @@
         <v>750</v>
       </c>
       <c r="C96" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D96" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E96">
         <v>0.997</v>
@@ -7591,10 +8062,10 @@
         <v>795</v>
       </c>
       <c r="C97" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D97" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E97">
         <v>1.1080000000000001</v>
@@ -7631,10 +8102,10 @@
         <v>795</v>
       </c>
       <c r="C98" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D98" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E98">
         <v>1.1399999999999999</v>
@@ -7671,10 +8142,10 @@
         <v>795</v>
       </c>
       <c r="C99" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D99" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E99">
         <v>1.093</v>
@@ -7711,10 +8182,10 @@
         <v>795</v>
       </c>
       <c r="C100" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D100" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E100">
         <v>1.026</v>
@@ -7751,12 +8222,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A60AA9E-251E-2D4D-A9AC-C0697DAD560B}">
   <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T1" sqref="T1:T1048576"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7774,64 +8245,64 @@
   <sheetData>
     <row r="1" spans="1:20" s="3" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="G1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="S1" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="K1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -7840,10 +8311,10 @@
         <v>Full_2(7×)</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D2" s="4" t="str">
         <f>_xlfn.XLOOKUP(_xlfn.CONCAT(LEFT(CN[[#This Row],[Conductor Size]], SEARCH("(", CN[[#This Row],[Conductor Size]])-1), "_AA"), OH[Size_Material], OH[Type], NA(),-1)</f>
@@ -7859,7 +8330,7 @@
         <v>0.98</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I2" s="4">
         <v>120</v>
@@ -7888,14 +8359,14 @@
         <v>2.0799999999999998E-3</v>
       </c>
       <c r="P2" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Q2" s="15">
         <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[rac])</f>
         <v>1.5409999999999999</v>
       </c>
       <c r="R2" s="15" t="str">
-        <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[Runits])</f>
+        <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[runits])</f>
         <v>mi</v>
       </c>
       <c r="S2" s="16">
@@ -7913,10 +8384,10 @@
         <v>Full_1(19×)</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D3" s="4" t="str">
         <f>_xlfn.XLOOKUP(_xlfn.CONCAT(LEFT(CN[[#This Row],[Conductor Size]], SEARCH("(", CN[[#This Row],[Conductor Size]])-1), "_AA"), OH[Size_Material], OH[Type], NA(),-1)</f>
@@ -7932,7 +8403,7 @@
         <v>1.02</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I3" s="4">
         <v>135</v>
@@ -7961,14 +8432,14 @@
         <v>2.0799999999999998E-3</v>
       </c>
       <c r="P3" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Q3" s="15">
         <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[rac])</f>
         <v>1.224</v>
       </c>
       <c r="R3" s="15" t="str">
-        <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[Runits])</f>
+        <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[runits])</f>
         <v>mi</v>
       </c>
       <c r="S3" s="16">
@@ -7986,10 +8457,10 @@
         <v>Full_1/0(19×)</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D4" s="4" t="str">
         <f>_xlfn.XLOOKUP(_xlfn.CONCAT(LEFT(CN[[#This Row],[Conductor Size]], SEARCH("(", CN[[#This Row],[Conductor Size]])-1), "_AA"), OH[Size_Material], OH[Type], NA(),-1)</f>
@@ -8005,7 +8476,7 @@
         <v>1.06</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I4" s="4">
         <v>155</v>
@@ -8034,14 +8505,14 @@
         <v>2.0799999999999998E-3</v>
       </c>
       <c r="P4" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Q4" s="15">
         <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[rac])</f>
         <v>0.97</v>
       </c>
       <c r="R4" s="15" t="str">
-        <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[Runits])</f>
+        <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[runits])</f>
         <v>mi</v>
       </c>
       <c r="S4" s="16">
@@ -8059,10 +8530,10 @@
         <v>Full_2/0(19×)</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D5" s="4" t="str">
         <f>_xlfn.XLOOKUP(_xlfn.CONCAT(LEFT(CN[[#This Row],[Conductor Size]], SEARCH("(", CN[[#This Row],[Conductor Size]])-1), "_AA"), OH[Size_Material], OH[Type], NA(),-1)</f>
@@ -8078,7 +8549,7 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I5" s="4">
         <v>175</v>
@@ -8107,14 +8578,14 @@
         <v>2.6199999999999999E-3</v>
       </c>
       <c r="P5" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Q5" s="15">
         <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[rac])</f>
         <v>0.76900000000000002</v>
       </c>
       <c r="R5" s="15" t="str">
-        <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[Runits])</f>
+        <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[runits])</f>
         <v>mi</v>
       </c>
       <c r="S5" s="16">
@@ -8132,10 +8603,10 @@
         <v>Full_3/0(19×)</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D6" s="4" t="str">
         <f>_xlfn.XLOOKUP(_xlfn.CONCAT(LEFT(CN[[#This Row],[Conductor Size]], SEARCH("(", CN[[#This Row],[Conductor Size]])-1), "_AA"), OH[Size_Material], OH[Type], NA(),-1)</f>
@@ -8151,7 +8622,7 @@
         <v>1.18</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I6" s="4">
         <v>200</v>
@@ -8180,14 +8651,14 @@
         <v>2.6199999999999999E-3</v>
       </c>
       <c r="P6" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Q6" s="15">
         <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[rac])</f>
         <v>0.61099999999999999</v>
       </c>
       <c r="R6" s="15" t="str">
-        <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[Runits])</f>
+        <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[runits])</f>
         <v>mi</v>
       </c>
       <c r="S6" s="16">
@@ -8205,10 +8676,10 @@
         <v>Full_4/0(19×)</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D7" s="4" t="str">
         <f>_xlfn.XLOOKUP(_xlfn.CONCAT(LEFT(CN[[#This Row],[Conductor Size]], SEARCH("(", CN[[#This Row],[Conductor Size]])-1), "_AA"), OH[Size_Material], OH[Type], NA(),-1)</f>
@@ -8224,7 +8695,7 @@
         <v>1.28</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I7" s="4">
         <v>230</v>
@@ -8253,14 +8724,14 @@
         <v>3.3E-3</v>
       </c>
       <c r="P7" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Q7" s="15">
         <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[rac])</f>
         <v>0.48399999999999999</v>
       </c>
       <c r="R7" s="15" t="str">
-        <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[Runits])</f>
+        <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[runits])</f>
         <v>mi</v>
       </c>
       <c r="S7" s="16">
@@ -8278,10 +8749,10 @@
         <v>Full_250(37×)</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D8" s="4" t="str">
         <f>_xlfn.XLOOKUP(_xlfn.CONCAT(LEFT(CN[[#This Row],[Conductor Size]], SEARCH("(", CN[[#This Row],[Conductor Size]])-1), "_AA"), OH[Size_Material], OH[Type], NA(),-1)</f>
@@ -8297,7 +8768,7 @@
         <v>1.37</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I8" s="4">
         <v>255</v>
@@ -8326,14 +8797,14 @@
         <v>3.3E-3</v>
       </c>
       <c r="P8" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Q8" s="15">
         <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[rac])</f>
         <v>0.41</v>
       </c>
       <c r="R8" s="15" t="str">
-        <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[Runits])</f>
+        <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[runits])</f>
         <v>mi</v>
       </c>
       <c r="S8" s="16">
@@ -8351,10 +8822,10 @@
         <v>Full_350(37×)</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D9" s="4" t="str">
         <f>_xlfn.XLOOKUP(_xlfn.CONCAT(LEFT(CN[[#This Row],[Conductor Size]], SEARCH("(", CN[[#This Row],[Conductor Size]])-1), "_AA"), OH[Size_Material], OH[Type], NA(),-1)</f>
@@ -8370,7 +8841,7 @@
         <v>1.47</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I9" s="4">
         <v>300</v>
@@ -8399,14 +8870,14 @@
         <v>3.3E-3</v>
       </c>
       <c r="P9" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Q9" s="15">
         <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[rac])</f>
         <v>0.29399999999999998</v>
       </c>
       <c r="R9" s="15" t="str">
-        <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[Runits])</f>
+        <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[runits])</f>
         <v>mi</v>
       </c>
       <c r="S9" s="16">
@@ -8424,10 +8895,10 @@
         <v>1/3_2(7×)</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D10" s="4" t="str">
         <f>_xlfn.XLOOKUP(_xlfn.CONCAT(LEFT(CN[[#This Row],[Conductor Size]], SEARCH("(", CN[[#This Row],[Conductor Size]])-1), "_AA"), OH[Size_Material], OH[Type], NA(),-1)</f>
@@ -8443,7 +8914,7 @@
         <v>0.98</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I10" s="4">
         <v>135</v>
@@ -8472,14 +8943,14 @@
         <v>2.0799999999999998E-3</v>
       </c>
       <c r="P10" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Q10" s="15">
         <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[rac])</f>
         <v>1.5409999999999999</v>
       </c>
       <c r="R10" s="15" t="str">
-        <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[Runits])</f>
+        <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[runits])</f>
         <v>mi</v>
       </c>
       <c r="S10" s="16">
@@ -8497,10 +8968,10 @@
         <v>1/3_1(19×)</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D11" s="4" t="str">
         <f>_xlfn.XLOOKUP(_xlfn.CONCAT(LEFT(CN[[#This Row],[Conductor Size]], SEARCH("(", CN[[#This Row],[Conductor Size]])-1), "_AA"), OH[Size_Material], OH[Type], NA(),-1)</f>
@@ -8516,7 +8987,7 @@
         <v>1.02</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I11" s="4">
         <v>155</v>
@@ -8545,14 +9016,14 @@
         <v>2.0799999999999998E-3</v>
       </c>
       <c r="P11" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Q11" s="15">
         <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[rac])</f>
         <v>1.224</v>
       </c>
       <c r="R11" s="15" t="str">
-        <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[Runits])</f>
+        <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[runits])</f>
         <v>mi</v>
       </c>
       <c r="S11" s="16">
@@ -8570,10 +9041,10 @@
         <v>1/3_1/0(19×)</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D12" s="4" t="str">
         <f>_xlfn.XLOOKUP(_xlfn.CONCAT(LEFT(CN[[#This Row],[Conductor Size]], SEARCH("(", CN[[#This Row],[Conductor Size]])-1), "_AA"), OH[Size_Material], OH[Type], NA(),-1)</f>
@@ -8589,7 +9060,7 @@
         <v>1.06</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I12" s="4">
         <v>175</v>
@@ -8618,14 +9089,14 @@
         <v>2.0799999999999998E-3</v>
       </c>
       <c r="P12" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Q12" s="15">
         <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[rac])</f>
         <v>0.97</v>
       </c>
       <c r="R12" s="15" t="str">
-        <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[Runits])</f>
+        <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[runits])</f>
         <v>mi</v>
       </c>
       <c r="S12" s="16">
@@ -8643,10 +9114,10 @@
         <v>1/3_2/0(19×)</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D13" s="4" t="str">
         <f>_xlfn.XLOOKUP(_xlfn.CONCAT(LEFT(CN[[#This Row],[Conductor Size]], SEARCH("(", CN[[#This Row],[Conductor Size]])-1), "_AA"), OH[Size_Material], OH[Type], NA(),-1)</f>
@@ -8662,7 +9133,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I13" s="4">
         <v>200</v>
@@ -8691,14 +9162,14 @@
         <v>2.0799999999999998E-3</v>
       </c>
       <c r="P13" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Q13" s="15">
         <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[rac])</f>
         <v>0.76900000000000002</v>
       </c>
       <c r="R13" s="15" t="str">
-        <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[Runits])</f>
+        <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[runits])</f>
         <v>mi</v>
       </c>
       <c r="S13" s="16">
@@ -8716,10 +9187,10 @@
         <v>1/3_3/0(19×)</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D14" s="4" t="str">
         <f>_xlfn.XLOOKUP(_xlfn.CONCAT(LEFT(CN[[#This Row],[Conductor Size]], SEARCH("(", CN[[#This Row],[Conductor Size]])-1), "_AA"), OH[Size_Material], OH[Type], NA(),-1)</f>
@@ -8735,7 +9206,7 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I14" s="4">
         <v>230</v>
@@ -8764,14 +9235,14 @@
         <v>2.0799999999999998E-3</v>
       </c>
       <c r="P14" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Q14" s="15">
         <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[rac])</f>
         <v>0.61099999999999999</v>
       </c>
       <c r="R14" s="15" t="str">
-        <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[Runits])</f>
+        <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[runits])</f>
         <v>mi</v>
       </c>
       <c r="S14" s="16">
@@ -8789,10 +9260,10 @@
         <v>1/3_4/0(19×)</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D15" s="4" t="str">
         <f>_xlfn.XLOOKUP(_xlfn.CONCAT(LEFT(CN[[#This Row],[Conductor Size]], SEARCH("(", CN[[#This Row],[Conductor Size]])-1), "_AA"), OH[Size_Material], OH[Type], NA(),-1)</f>
@@ -8808,7 +9279,7 @@
         <v>1.21</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I15" s="4">
         <v>240</v>
@@ -8837,14 +9308,14 @@
         <v>2.0799999999999998E-3</v>
       </c>
       <c r="P15" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Q15" s="15">
         <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[rac])</f>
         <v>0.48399999999999999</v>
       </c>
       <c r="R15" s="15" t="str">
-        <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[Runits])</f>
+        <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[runits])</f>
         <v>mi</v>
       </c>
       <c r="S15" s="16">
@@ -8862,10 +9333,10 @@
         <v>1/3_250(37×)</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D16" s="4" t="str">
         <f>_xlfn.XLOOKUP(_xlfn.CONCAT(LEFT(CN[[#This Row],[Conductor Size]], SEARCH("(", CN[[#This Row],[Conductor Size]])-1), "_AA"), OH[Size_Material], OH[Type], NA(),-1)</f>
@@ -8881,7 +9352,7 @@
         <v>1.29</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I16" s="4">
         <v>260</v>
@@ -8910,14 +9381,14 @@
         <v>2.0799999999999998E-3</v>
       </c>
       <c r="P16" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Q16" s="15">
         <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[rac])</f>
         <v>0.41</v>
       </c>
       <c r="R16" s="15" t="str">
-        <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[Runits])</f>
+        <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[runits])</f>
         <v>mi</v>
       </c>
       <c r="S16" s="16">
@@ -8935,10 +9406,10 @@
         <v>1/3_350(37×)</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D17" s="4" t="str">
         <f>_xlfn.XLOOKUP(_xlfn.CONCAT(LEFT(CN[[#This Row],[Conductor Size]], SEARCH("(", CN[[#This Row],[Conductor Size]])-1), "_AA"), OH[Size_Material], OH[Type], NA(),-1)</f>
@@ -8954,7 +9425,7 @@
         <v>1.39</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I17" s="4">
         <v>320</v>
@@ -8983,14 +9454,14 @@
         <v>2.0799999999999998E-3</v>
       </c>
       <c r="P17" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Q17" s="15">
         <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[rac])</f>
         <v>0.29399999999999998</v>
       </c>
       <c r="R17" s="15" t="str">
-        <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[Runits])</f>
+        <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[runits])</f>
         <v>mi</v>
       </c>
       <c r="S17" s="16">
@@ -9008,10 +9479,10 @@
         <v>1/3_500(37×)</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D18" s="4" t="str">
         <f>_xlfn.XLOOKUP(_xlfn.CONCAT(LEFT(CN[[#This Row],[Conductor Size]], SEARCH("(", CN[[#This Row],[Conductor Size]])-1), "_AA"), OH[Size_Material], OH[Type], NA(),-1)</f>
@@ -9027,7 +9498,7 @@
         <v>1.56</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I18" s="4">
         <v>385</v>
@@ -9056,14 +9527,14 @@
         <v>2.6199999999999999E-3</v>
       </c>
       <c r="P18" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Q18" s="15">
         <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[rac])</f>
         <v>0.20599999999999999</v>
       </c>
       <c r="R18" s="15" t="str">
-        <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[Runits])</f>
+        <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[runits])</f>
         <v>mi</v>
       </c>
       <c r="S18" s="16">
@@ -9081,10 +9552,10 @@
         <v>1/3_750(61×)</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D19" s="4" t="str">
         <f>_xlfn.XLOOKUP(_xlfn.CONCAT(LEFT(CN[[#This Row],[Conductor Size]], SEARCH("(", CN[[#This Row],[Conductor Size]])-1), "_AA"), OH[Size_Material], OH[Type], NA(),-1)</f>
@@ -9100,7 +9571,7 @@
         <v>1.79</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I19" s="4">
         <v>470</v>
@@ -9129,14 +9600,14 @@
         <v>3.3E-3</v>
       </c>
       <c r="P19" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Q19" s="15">
         <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[rac])</f>
         <v>8.8800000000000004E-2</v>
       </c>
       <c r="R19" s="15" t="str">
-        <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[Runits])</f>
+        <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[runits])</f>
         <v>mi</v>
       </c>
       <c r="S19" s="16">
@@ -9181,12 +9652,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67452CAF-D40E-2344-8B7E-ABD55E102AF6}">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9202,30 +9673,30 @@
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" ht="52" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B2" s="9">
         <v>0.82</v>
@@ -9248,7 +9719,7 @@
     </row>
     <row r="3" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3" s="9">
         <v>0.87</v>
@@ -9271,7 +9742,7 @@
     </row>
     <row r="4" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B4" s="9">
         <v>0.91</v>
@@ -9294,7 +9765,7 @@
     </row>
     <row r="5" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B5" s="9">
         <v>0.96</v>

</xml_diff>

<commit_message>
add code to send dss wiredata cmds
</commit_message>
<xml_diff>
--- a/network-data/LineGeo_Selector.xlsx
+++ b/network-data/LineGeo_Selector.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spenceregan/Repos/CU/Distribution_Systems/Project1/ECEN5437-Proj1/network-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63195EC3-1667-1E49-A1A2-3B0D7D73F202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72CD6436-E154-8E48-9A6D-9F2FD5B9F630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6640" yWindow="760" windowWidth="23600" windowHeight="17440" activeTab="5" xr2:uid="{7AEC5E2E-397B-8345-871E-9ED757579969}"/>
+    <workbookView xWindow="6640" yWindow="760" windowWidth="23600" windowHeight="17440" activeTab="6" xr2:uid="{7AEC5E2E-397B-8345-871E-9ED757579969}"/>
   </bookViews>
   <sheets>
     <sheet name="Buses" sheetId="7" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="174">
   <si>
     <t>OH3p</t>
   </si>
@@ -306,9 +306,6 @@
     <t>Units</t>
   </si>
   <si>
-    <t>GMRUnits</t>
-  </si>
-  <si>
     <t>Runits</t>
   </si>
   <si>
@@ -378,6 +375,9 @@
     <t>4_z</t>
   </si>
   <si>
+    <t>Radunits</t>
+  </si>
+  <si>
     <t>n0</t>
   </si>
   <si>
@@ -553,6 +553,18 @@
   </si>
   <si>
     <t>runits</t>
+  </si>
+  <si>
+    <t>diam</t>
+  </si>
+  <si>
+    <t>DiaCable</t>
+  </si>
+  <si>
+    <t>DiaIns</t>
+  </si>
+  <si>
+    <t>DiaStrand</t>
   </si>
 </sst>
 </file>
@@ -675,7 +687,55 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="54">
+  <dxfs count="56">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1827,16 +1887,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{43240ADB-710B-E440-9B4B-064F1493B981}" name="Buses" displayName="Buses" ref="A1:C47" totalsRowShown="0" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{43240ADB-710B-E440-9B4B-064F1493B981}" name="Buses" displayName="Buses" ref="A1:C47" totalsRowShown="0" dataDxfId="7">
   <autoFilter ref="A1:C47" xr:uid="{43240ADB-710B-E440-9B4B-064F1493B981}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{37E9F5EA-051D-BE40-B622-31D4B83CE6AA}" name="Bus" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{41D4B11A-15CC-A540-9052-95C4F3006357}" name="Graph_Loc_x" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{871540F1-C33C-6346-9F71-C67E6A5F5C63}" name="Graph_Loc_y" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{37E9F5EA-051D-BE40-B622-31D4B83CE6AA}" name="Bus" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{41D4B11A-15CC-A540-9052-95C4F3006357}" name="Graph_Loc_x" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{871540F1-C33C-6346-9F71-C67E6A5F5C63}" name="Graph_Loc_y" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1865,7 +1925,7 @@
     <tableColumn id="1" xr3:uid="{2280FF94-C83E-444E-8E42-3510351A4DF6}" name="LineGeo"/>
     <tableColumn id="2" xr3:uid="{3DDFC765-300B-7846-9085-AB03B6A261F4}" name="Type"/>
     <tableColumn id="3" xr3:uid="{02F910B6-BE16-CE4C-89A1-71F43049235B}" name="phase_conductor"/>
-    <tableColumn id="4" xr3:uid="{520CD3FE-AB23-3943-8829-73CAAC013F53}" name="neutral_conductor" dataDxfId="33">
+    <tableColumn id="4" xr3:uid="{520CD3FE-AB23-3943-8829-73CAAC013F53}" name="neutral_conductor" dataDxfId="35">
       <calculatedColumnFormula>IF(LineGeo[[#This Row],[Type]]="OH",1,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="13" xr3:uid="{DE9BDE1B-5E39-604D-9957-E0C3A3473BC8}" name="Phases"/>
@@ -1885,7 +1945,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{12D9EB82-8B48-7449-95A6-3BE76017FBF1}" name="Table7" displayName="Table7" ref="A1:E38" totalsRowShown="0" headerRowDxfId="10" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{12D9EB82-8B48-7449-95A6-3BE76017FBF1}" name="Table7" displayName="Table7" ref="A1:E38" totalsRowShown="0" headerRowDxfId="12" dataDxfId="13">
   <autoFilter ref="A1:E38" xr:uid="{12D9EB82-8B48-7449-95A6-3BE76017FBF1}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1894,27 +1954,27 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{B526205E-98EF-F34B-B24D-F8218A008415}" name="bus1" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{D2CD9147-9358-C04D-8316-3FB3A9A16CB0}" name="bus2" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{99BA8C9D-330B-A24F-BC6C-A45D5466D8F3}" name="Length" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{24B6C05D-6629-B248-BB9C-1AF1BAA7ADB7}" name="LineGeometry" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{CDFF2292-878E-CE4B-BF6E-6CE7168C35B8}" name="Units" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{B526205E-98EF-F34B-B24D-F8218A008415}" name="bus1" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{D2CD9147-9358-C04D-8316-3FB3A9A16CB0}" name="bus2" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{99BA8C9D-330B-A24F-BC6C-A45D5466D8F3}" name="Length" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{24B6C05D-6629-B248-BB9C-1AF1BAA7ADB7}" name="LineGeometry" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{CDFF2292-878E-CE4B-BF6E-6CE7168C35B8}" name="Units" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{CDAC5F4F-CC5E-714A-A10A-32F2E90176D7}" name="Table9" displayName="Table9" ref="A1:C28" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{CDAC5F4F-CC5E-714A-A10A-32F2E90176D7}" name="Table9" displayName="Table9" ref="A1:C28" totalsRowShown="0" headerRowDxfId="2" dataDxfId="3">
   <autoFilter ref="A1:C28" xr:uid="{CDAC5F4F-CC5E-714A-A10A-32F2E90176D7}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{49EC89B8-2142-0A4A-B8EF-264BCDD715FA}" name="Bus" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{13C1D0C2-6357-484D-ADEB-105711D6B1A5}" name="kW" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{A5C493EA-CBB6-854A-A97A-1FDDCAB8D84F}" name="kVAr" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{49EC89B8-2142-0A4A-B8EF-264BCDD715FA}" name="Bus" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{13C1D0C2-6357-484D-ADEB-105711D6B1A5}" name="kW" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{A5C493EA-CBB6-854A-A97A-1FDDCAB8D84F}" name="kVAr" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1954,23 +2014,23 @@
     <filterColumn colId="10" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{E903BA16-38F3-EE44-A1B4-2B0F344DDB1D}" name="Type" dataDxfId="25">
+    <tableColumn id="1" xr3:uid="{E903BA16-38F3-EE44-A1B4-2B0F344DDB1D}" name="Type" dataDxfId="27">
       <calculatedColumnFormula>_xlfn.CONCAT(OH[[#This Row],[Size]], "_",OH[[#This Row],[Stranding]], "_", OH[[#This Row],[Material]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{B69CA351-3694-B545-8563-7479CF50BC67}" name="Size" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{B69CA351-3694-B545-8563-7479CF50BC67}" name="Size" dataDxfId="26"/>
     <tableColumn id="3" xr3:uid="{3576FC0F-75EE-6F4B-B709-5C5715FE540E}" name="Stranding"/>
     <tableColumn id="4" xr3:uid="{C31618D9-7DA8-804A-A013-69A802FF7774}" name="Material"/>
     <tableColumn id="5" xr3:uid="{804C85FC-06A5-4645-A278-FD8271A5F0ED}" name="Diam"/>
     <tableColumn id="6" xr3:uid="{ED80EC98-63E4-C94C-BAF3-F13294EE8381}" name="GMRac"/>
     <tableColumn id="7" xr3:uid="{41A91B17-FB89-1F4F-899A-3761661447FD}" name="rac"/>
     <tableColumn id="8" xr3:uid="{C9144B25-D7C0-D444-8605-CEBD77A9171D}" name="normamps"/>
-    <tableColumn id="13" xr3:uid="{041E70E4-975E-254A-81CF-95C5EF9E73D2}" name="GMRunits" dataDxfId="32">
+    <tableColumn id="13" xr3:uid="{041E70E4-975E-254A-81CF-95C5EF9E73D2}" name="GMRunits" dataDxfId="34">
       <calculatedColumnFormula>"ft"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{2AEFB39D-D6D8-D14D-A990-9BB4F5164639}" name="runits" dataDxfId="31">
+    <tableColumn id="14" xr3:uid="{2AEFB39D-D6D8-D14D-A990-9BB4F5164639}" name="runits" dataDxfId="33">
       <calculatedColumnFormula>"mi"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{21A61F38-5A94-2142-A9A8-D6E0BB77AB1E}" name="Size_Material" dataDxfId="23">
+    <tableColumn id="15" xr3:uid="{21A61F38-5A94-2142-A9A8-D6E0BB77AB1E}" name="Size_Material" dataDxfId="25">
       <calculatedColumnFormula>_xlfn.CONCAT(OH[[#This Row],[Size]], "_", OH[[#This Row],[Material]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1979,8 +2039,8 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{661274D6-1D68-5542-8D94-45D5C86243F5}" name="CN" displayName="CN" ref="A1:T19" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44" tableBorderDxfId="53">
-  <autoFilter ref="A1:T19" xr:uid="{661274D6-1D68-5542-8D94-45D5C86243F5}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{661274D6-1D68-5542-8D94-45D5C86243F5}" name="CN" displayName="CN" ref="A1:V19" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46" tableBorderDxfId="55">
+  <autoFilter ref="A1:V19" xr:uid="{661274D6-1D68-5542-8D94-45D5C86243F5}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2001,57 +2061,63 @@
     <filterColumn colId="17" hiddenButton="1"/>
     <filterColumn colId="18" hiddenButton="1"/>
     <filterColumn colId="19" hiddenButton="1"/>
+    <filterColumn colId="20" hiddenButton="1"/>
+    <filterColumn colId="21" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="20">
-    <tableColumn id="9" xr3:uid="{869F190C-19C4-2243-84CA-F6CB8F4281C2}" name="Type" dataDxfId="36">
+  <tableColumns count="22">
+    <tableColumn id="9" xr3:uid="{869F190C-19C4-2243-84CA-F6CB8F4281C2}" name="Type" dataDxfId="38">
       <calculatedColumnFormula>_xlfn.CONCAT(CN[[#This Row],[Neutral Ampacity]], "_", CN[[#This Row],[Conductor Size]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{1DFBB787-8CEC-A946-969E-C8B3E35D5AEB}" name="Neutral Ampacity" dataDxfId="52"/>
-    <tableColumn id="2" xr3:uid="{EFDAEEF3-E5BA-4B49-BA44-2340320EA290}" name="Conductor Size" dataDxfId="51"/>
-    <tableColumn id="18" xr3:uid="{703A2A0A-5882-4349-9ACB-A05C1C032238}" name="Phase Conductor Name" dataDxfId="22">
+    <tableColumn id="1" xr3:uid="{1DFBB787-8CEC-A946-969E-C8B3E35D5AEB}" name="Neutral Ampacity" dataDxfId="54"/>
+    <tableColumn id="2" xr3:uid="{EFDAEEF3-E5BA-4B49-BA44-2340320EA290}" name="Conductor Size" dataDxfId="53"/>
+    <tableColumn id="18" xr3:uid="{703A2A0A-5882-4349-9ACB-A05C1C032238}" name="Phase Conductor Name" dataDxfId="24">
       <calculatedColumnFormula>_xlfn.XLOOKUP(_xlfn.CONCAT(LEFT(CN[[#This Row],[Conductor Size]], SEARCH("(", CN[[#This Row],[Conductor Size]])-1), "_AA"), OH[Size_Material], OH[Type], NA(),-1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8E5F5E70-58CE-0D4E-A970-1B53EA80FE07}" name="Diameter Over Insulation (in)" dataDxfId="50"/>
-    <tableColumn id="4" xr3:uid="{D154B6B5-D516-AC44-879B-B0BC6ACADF64}" name="Diameter Over Screen (in)" dataDxfId="49"/>
-    <tableColumn id="5" xr3:uid="{51092775-E14C-4945-BD12-6F609313AC1A}" name="Outside Diameter" dataDxfId="48"/>
-    <tableColumn id="6" xr3:uid="{FE25AF87-2C02-C642-B28A-81AF2224011F}" name="Copper Neutral" dataDxfId="47"/>
-    <tableColumn id="7" xr3:uid="{167EFF3D-5388-5C47-9405-F0CE90C78333}" name="Ampacity in Underground Duct (A)" dataDxfId="46"/>
-    <tableColumn id="8" xr3:uid="{D4CA2780-FAB4-FE44-BAA2-A16B53A68DE8}" name="Voltage Rating (kV)" dataDxfId="30"/>
-    <tableColumn id="11" xr3:uid="{830817DB-B122-D444-8DFC-58C1CE7D7901}" name="Neutral Strand AWG" dataDxfId="28" dataCellStyle="Percent">
+    <tableColumn id="3" xr3:uid="{8E5F5E70-58CE-0D4E-A970-1B53EA80FE07}" name="DiaIns" dataDxfId="52"/>
+    <tableColumn id="4" xr3:uid="{D154B6B5-D516-AC44-879B-B0BC6ACADF64}" name="Diameter Over Screen (in)" dataDxfId="51"/>
+    <tableColumn id="5" xr3:uid="{51092775-E14C-4945-BD12-6F609313AC1A}" name="DiaCable" dataDxfId="50"/>
+    <tableColumn id="6" xr3:uid="{FE25AF87-2C02-C642-B28A-81AF2224011F}" name="Copper Neutral" dataDxfId="49"/>
+    <tableColumn id="7" xr3:uid="{167EFF3D-5388-5C47-9405-F0CE90C78333}" name="Ampacity in Underground Duct (A)" dataDxfId="48"/>
+    <tableColumn id="8" xr3:uid="{D4CA2780-FAB4-FE44-BAA2-A16B53A68DE8}" name="Voltage Rating (kV)" dataDxfId="32"/>
+    <tableColumn id="11" xr3:uid="{830817DB-B122-D444-8DFC-58C1CE7D7901}" name="Neutral Strand AWG" dataDxfId="30" dataCellStyle="Percent">
       <calculatedColumnFormula>VALUE(RIGHT(CN[[#This Row],[Copper Neutral]],2))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{A0775550-BA03-5542-A01E-64482C59971C}" name="Rstrand" dataDxfId="29">
+    <tableColumn id="10" xr3:uid="{A0775550-BA03-5542-A01E-64482C59971C}" name="Rstrand" dataDxfId="31">
       <calculatedColumnFormula>_xlfn.XLOOKUP(CN[[#This Row],[Neutral Strand AWG]], OH[Size], OH[rac])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{4B541559-291A-4941-9353-F59C621A9E18}" name="k" dataDxfId="27">
+    <tableColumn id="12" xr3:uid="{4B541559-291A-4941-9353-F59C621A9E18}" name="k" dataDxfId="29">
       <calculatedColumnFormula>VALUE(LEFT(CN[[#This Row],[Copper Neutral]], SEARCH(" ",CN[[#This Row],[Copper Neutral]])-1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{60128454-1EE5-9C4B-9AA2-D0CE6F9C4CF7}" name="GMRac" dataDxfId="21">
+    <tableColumn id="13" xr3:uid="{60128454-1EE5-9C4B-9AA2-D0CE6F9C4CF7}" name="GMRac" dataDxfId="23">
       <calculatedColumnFormula>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]], OH[Type], OH[GMRac])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{AA242217-BC74-AB48-8D9A-86A3970B8399}" name="GmrStrand" dataDxfId="20">
+    <tableColumn id="14" xr3:uid="{AA242217-BC74-AB48-8D9A-86A3970B8399}" name="GmrStrand" dataDxfId="22">
       <calculatedColumnFormula>_xlfn.XLOOKUP(CN[[#This Row],[Neutral Strand AWG]], OH[Size], OH[GMRac])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{BDF03C79-D2AE-394A-9557-0FEAE0AA392C}" name="GMRUnits" dataDxfId="26"/>
-    <tableColumn id="16" xr3:uid="{E6B7FA4C-2968-AE41-84BD-9EA25CF9A089}" name="Rac" dataDxfId="19">
+    <tableColumn id="15" xr3:uid="{BDF03C79-D2AE-394A-9557-0FEAE0AA392C}" name="GMRunits" dataDxfId="28"/>
+    <tableColumn id="16" xr3:uid="{E6B7FA4C-2968-AE41-84BD-9EA25CF9A089}" name="Rac" dataDxfId="21">
       <calculatedColumnFormula>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[rac])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{60CA6D09-ACAD-FA47-9A7F-D8BCB54C2191}" name="Runits" dataDxfId="18">
+    <tableColumn id="17" xr3:uid="{60CA6D09-ACAD-FA47-9A7F-D8BCB54C2191}" name="Runits" dataDxfId="20">
       <calculatedColumnFormula>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[runits])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{A335B60A-8482-494F-9920-64B3CC7615EB}" name="Diam" dataDxfId="17">
+    <tableColumn id="19" xr3:uid="{A335B60A-8482-494F-9920-64B3CC7615EB}" name="diam" dataDxfId="19">
       <calculatedColumnFormula>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[Diam])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{D37687B3-1580-7845-A711-F39AB1A49147}" name="normamps" dataDxfId="16">
+    <tableColumn id="20" xr3:uid="{D37687B3-1580-7845-A711-F39AB1A49147}" name="normamps" dataDxfId="18">
       <calculatedColumnFormula>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[normamps])</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="22" xr3:uid="{D2E6A1F4-79B9-0D45-BE31-8E41DE3A29BC}" name="DiaStrand" dataDxfId="1">
+      <calculatedColumnFormula>_xlfn.XLOOKUP(CN[[#This Row],[Neutral Strand AWG]], OH[Size], OH[Diam])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="23" xr3:uid="{E3B20767-C678-7E4D-8C37-6DA7A2305EDB}" name="Radunits" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{13D01E9F-2651-EF45-A492-F190721E7BE9}" name="TS" displayName="TS" ref="A1:G10" totalsRowShown="0" headerRowDxfId="37" dataDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{13D01E9F-2651-EF45-A492-F190721E7BE9}" name="TS" displayName="TS" ref="A1:G10" totalsRowShown="0" headerRowDxfId="39" dataDxfId="40">
   <autoFilter ref="A1:G10" xr:uid="{13D01E9F-2651-EF45-A492-F190721E7BE9}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2062,13 +2128,13 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{19CDDA2D-9812-404F-A70E-F8C42AD526DB}" name="Type" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{C1A0B38B-F04B-0A4C-913A-B68BB0D6C78E}" name="Diameter Over Insulation (in)" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{D6D141BB-2B57-4B4B-8667-6762392800DB}" name="Diameter Over Screen (in)" dataDxfId="43"/>
-    <tableColumn id="4" xr3:uid="{401114E4-AC5F-DA47-A949-534E36354F8D}" name="Jacket Thickness (mils)" dataDxfId="42"/>
-    <tableColumn id="5" xr3:uid="{244E8C6F-E27A-B344-A042-CF80AF18FA7C}" name="Outside Diameter" dataDxfId="41"/>
-    <tableColumn id="6" xr3:uid="{D80F22EC-CB8C-E549-AC7C-4BA81E9F5164}" name="Ampacity in UG Duct (A)" dataDxfId="40"/>
-    <tableColumn id="7" xr3:uid="{A989CB28-4027-F249-A88C-9A2D66CB1557}" name="Rated Voltage (kV)" dataDxfId="39"/>
+    <tableColumn id="1" xr3:uid="{19CDDA2D-9812-404F-A70E-F8C42AD526DB}" name="Type" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{C1A0B38B-F04B-0A4C-913A-B68BB0D6C78E}" name="Diameter Over Insulation (in)" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{D6D141BB-2B57-4B4B-8667-6762392800DB}" name="Diameter Over Screen (in)" dataDxfId="45"/>
+    <tableColumn id="4" xr3:uid="{401114E4-AC5F-DA47-A949-534E36354F8D}" name="Jacket Thickness (mils)" dataDxfId="44"/>
+    <tableColumn id="5" xr3:uid="{244E8C6F-E27A-B344-A042-CF80AF18FA7C}" name="Outside Diameter" dataDxfId="43"/>
+    <tableColumn id="6" xr3:uid="{D80F22EC-CB8C-E549-AC7C-4BA81E9F5164}" name="Ampacity in UG Duct (A)" dataDxfId="42"/>
+    <tableColumn id="7" xr3:uid="{A989CB28-4027-F249-A88C-9A2D66CB1557}" name="Rated Voltage (kV)" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2944,28 +3010,28 @@
         <v>79</v>
       </c>
       <c r="G1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H1" t="s">
         <v>103</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>104</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>105</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>106</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>107</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>108</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>109</v>
-      </c>
-      <c r="N1" t="s">
-        <v>110</v>
       </c>
       <c r="O1" t="s">
         <v>86</v>
@@ -3093,7 +3159,7 @@
         <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D5" t="s">
         <v>77</v>
@@ -3136,7 +3202,7 @@
         <v>71</v>
       </c>
       <c r="C6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D6" t="s">
         <v>76</v>
@@ -4258,7 +4324,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5904AC-ECAC-4945-B9B6-B220AC818209}">
   <dimension ref="A1:N100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
@@ -4288,25 +4354,25 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" t="s">
         <v>96</v>
       </c>
-      <c r="F1" t="s">
-        <v>90</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>98</v>
-      </c>
-      <c r="H1" t="s">
-        <v>97</v>
-      </c>
-      <c r="I1" t="s">
-        <v>99</v>
       </c>
       <c r="J1" t="s">
         <v>169</v>
       </c>
       <c r="K1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -8224,10 +8290,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A60AA9E-251E-2D4D-A9AC-C0697DAD560B}">
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:V20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8243,7 +8309,7 @@
     <col min="11" max="11" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="3" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" s="3" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>33</v>
       </c>
@@ -8254,16 +8320,16 @@
         <v>61</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>62</v>
+        <v>172</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>63</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>64</v>
+        <v>171</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>65</v>
@@ -8275,37 +8341,43 @@
         <v>73</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M1" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q1" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="Q1" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>88</v>
-      </c>
       <c r="S1" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="T1" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="T1" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U1" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="str">
         <f>_xlfn.CONCAT(CN[[#This Row],[Neutral Ampacity]], "_", CN[[#This Row],[Conductor Size]])</f>
         <v>Full_2(7×)</v>
@@ -8377,8 +8449,15 @@
         <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[normamps])</f>
         <v>156</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U2" s="16">
+        <f>_xlfn.XLOOKUP(CN[[#This Row],[Neutral Strand AWG]], OH[Size], OH[Diam])</f>
+        <v>6.4100000000000004E-2</v>
+      </c>
+      <c r="V2" s="16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="str">
         <f>_xlfn.CONCAT(CN[[#This Row],[Neutral Ampacity]], "_", CN[[#This Row],[Conductor Size]])</f>
         <v>Full_1(19×)</v>
@@ -8450,8 +8529,15 @@
         <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[normamps])</f>
         <v>177</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U3" s="16">
+        <f>_xlfn.XLOOKUP(CN[[#This Row],[Neutral Strand AWG]], OH[Size], OH[Diam])</f>
+        <v>6.4100000000000004E-2</v>
+      </c>
+      <c r="V3" s="16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="str">
         <f>_xlfn.CONCAT(CN[[#This Row],[Neutral Ampacity]], "_", CN[[#This Row],[Conductor Size]])</f>
         <v>Full_1/0(19×)</v>
@@ -8523,8 +8609,15 @@
         <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[normamps])</f>
         <v>202</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U4" s="16">
+        <f>_xlfn.XLOOKUP(CN[[#This Row],[Neutral Strand AWG]], OH[Size], OH[Diam])</f>
+        <v>6.4100000000000004E-2</v>
+      </c>
+      <c r="V4" s="16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="str">
         <f>_xlfn.CONCAT(CN[[#This Row],[Neutral Ampacity]], "_", CN[[#This Row],[Conductor Size]])</f>
         <v>Full_2/0(19×)</v>
@@ -8596,8 +8689,15 @@
         <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[normamps])</f>
         <v>230</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U5" s="16">
+        <f>_xlfn.XLOOKUP(CN[[#This Row],[Neutral Strand AWG]], OH[Size], OH[Diam])</f>
+        <v>8.0799999999999997E-2</v>
+      </c>
+      <c r="V5" s="16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="str">
         <f>_xlfn.CONCAT(CN[[#This Row],[Neutral Ampacity]], "_", CN[[#This Row],[Conductor Size]])</f>
         <v>Full_3/0(19×)</v>
@@ -8669,8 +8769,15 @@
         <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[normamps])</f>
         <v>263</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U6" s="16">
+        <f>_xlfn.XLOOKUP(CN[[#This Row],[Neutral Strand AWG]], OH[Size], OH[Diam])</f>
+        <v>8.0799999999999997E-2</v>
+      </c>
+      <c r="V6" s="16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="str">
         <f>_xlfn.CONCAT(CN[[#This Row],[Neutral Ampacity]], "_", CN[[#This Row],[Conductor Size]])</f>
         <v>Full_4/0(19×)</v>
@@ -8742,8 +8849,15 @@
         <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[normamps])</f>
         <v>299</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U7" s="16">
+        <f>_xlfn.XLOOKUP(CN[[#This Row],[Neutral Strand AWG]], OH[Size], OH[Diam])</f>
+        <v>0.1019</v>
+      </c>
+      <c r="V7" s="16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="str">
         <f>_xlfn.CONCAT(CN[[#This Row],[Neutral Ampacity]], "_", CN[[#This Row],[Conductor Size]])</f>
         <v>Full_250(37×)</v>
@@ -8815,8 +8929,15 @@
         <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[normamps])</f>
         <v>329</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U8" s="16">
+        <f>_xlfn.XLOOKUP(CN[[#This Row],[Neutral Strand AWG]], OH[Size], OH[Diam])</f>
+        <v>0.1019</v>
+      </c>
+      <c r="V8" s="16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="str">
         <f>_xlfn.CONCAT(CN[[#This Row],[Neutral Ampacity]], "_", CN[[#This Row],[Conductor Size]])</f>
         <v>Full_350(37×)</v>
@@ -8888,8 +9009,15 @@
         <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[normamps])</f>
         <v>399</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U9" s="16">
+        <f>_xlfn.XLOOKUP(CN[[#This Row],[Neutral Strand AWG]], OH[Size], OH[Diam])</f>
+        <v>0.1019</v>
+      </c>
+      <c r="V9" s="16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="str">
         <f>_xlfn.CONCAT(CN[[#This Row],[Neutral Ampacity]], "_", CN[[#This Row],[Conductor Size]])</f>
         <v>1/3_2(7×)</v>
@@ -8961,8 +9089,15 @@
         <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[normamps])</f>
         <v>156</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U10" s="16">
+        <f>_xlfn.XLOOKUP(CN[[#This Row],[Neutral Strand AWG]], OH[Size], OH[Diam])</f>
+        <v>6.4100000000000004E-2</v>
+      </c>
+      <c r="V10" s="16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="str">
         <f>_xlfn.CONCAT(CN[[#This Row],[Neutral Ampacity]], "_", CN[[#This Row],[Conductor Size]])</f>
         <v>1/3_1(19×)</v>
@@ -9034,8 +9169,15 @@
         <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[normamps])</f>
         <v>177</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U11" s="16">
+        <f>_xlfn.XLOOKUP(CN[[#This Row],[Neutral Strand AWG]], OH[Size], OH[Diam])</f>
+        <v>6.4100000000000004E-2</v>
+      </c>
+      <c r="V11" s="16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="str">
         <f>_xlfn.CONCAT(CN[[#This Row],[Neutral Ampacity]], "_", CN[[#This Row],[Conductor Size]])</f>
         <v>1/3_1/0(19×)</v>
@@ -9107,8 +9249,15 @@
         <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[normamps])</f>
         <v>202</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U12" s="16">
+        <f>_xlfn.XLOOKUP(CN[[#This Row],[Neutral Strand AWG]], OH[Size], OH[Diam])</f>
+        <v>6.4100000000000004E-2</v>
+      </c>
+      <c r="V12" s="16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="str">
         <f>_xlfn.CONCAT(CN[[#This Row],[Neutral Ampacity]], "_", CN[[#This Row],[Conductor Size]])</f>
         <v>1/3_2/0(19×)</v>
@@ -9180,8 +9329,15 @@
         <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[normamps])</f>
         <v>230</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U13" s="16">
+        <f>_xlfn.XLOOKUP(CN[[#This Row],[Neutral Strand AWG]], OH[Size], OH[Diam])</f>
+        <v>6.4100000000000004E-2</v>
+      </c>
+      <c r="V13" s="16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="str">
         <f>_xlfn.CONCAT(CN[[#This Row],[Neutral Ampacity]], "_", CN[[#This Row],[Conductor Size]])</f>
         <v>1/3_3/0(19×)</v>
@@ -9253,8 +9409,15 @@
         <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[normamps])</f>
         <v>263</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U14" s="16">
+        <f>_xlfn.XLOOKUP(CN[[#This Row],[Neutral Strand AWG]], OH[Size], OH[Diam])</f>
+        <v>6.4100000000000004E-2</v>
+      </c>
+      <c r="V14" s="16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="str">
         <f>_xlfn.CONCAT(CN[[#This Row],[Neutral Ampacity]], "_", CN[[#This Row],[Conductor Size]])</f>
         <v>1/3_4/0(19×)</v>
@@ -9326,8 +9489,15 @@
         <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[normamps])</f>
         <v>299</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U15" s="16">
+        <f>_xlfn.XLOOKUP(CN[[#This Row],[Neutral Strand AWG]], OH[Size], OH[Diam])</f>
+        <v>6.4100000000000004E-2</v>
+      </c>
+      <c r="V15" s="16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="str">
         <f>_xlfn.CONCAT(CN[[#This Row],[Neutral Ampacity]], "_", CN[[#This Row],[Conductor Size]])</f>
         <v>1/3_250(37×)</v>
@@ -9399,8 +9569,15 @@
         <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[normamps])</f>
         <v>329</v>
       </c>
-    </row>
-    <row r="17" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U16" s="16">
+        <f>_xlfn.XLOOKUP(CN[[#This Row],[Neutral Strand AWG]], OH[Size], OH[Diam])</f>
+        <v>6.4100000000000004E-2</v>
+      </c>
+      <c r="V16" s="16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="str">
         <f>_xlfn.CONCAT(CN[[#This Row],[Neutral Ampacity]], "_", CN[[#This Row],[Conductor Size]])</f>
         <v>1/3_350(37×)</v>
@@ -9472,8 +9649,15 @@
         <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[normamps])</f>
         <v>399</v>
       </c>
-    </row>
-    <row r="18" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U17" s="16">
+        <f>_xlfn.XLOOKUP(CN[[#This Row],[Neutral Strand AWG]], OH[Size], OH[Diam])</f>
+        <v>6.4100000000000004E-2</v>
+      </c>
+      <c r="V17" s="16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="str">
         <f>_xlfn.CONCAT(CN[[#This Row],[Neutral Ampacity]], "_", CN[[#This Row],[Conductor Size]])</f>
         <v>1/3_500(37×)</v>
@@ -9545,8 +9729,15 @@
         <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[normamps])</f>
         <v>483</v>
       </c>
-    </row>
-    <row r="19" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U18" s="16">
+        <f>_xlfn.XLOOKUP(CN[[#This Row],[Neutral Strand AWG]], OH[Size], OH[Diam])</f>
+        <v>8.0799999999999997E-2</v>
+      </c>
+      <c r="V18" s="16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="str">
         <f>_xlfn.CONCAT(CN[[#This Row],[Neutral Ampacity]], "_", CN[[#This Row],[Conductor Size]])</f>
         <v>1/3_750(61×)</v>
@@ -9618,8 +9809,15 @@
         <f>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[normamps])</f>
         <v>1090</v>
       </c>
-    </row>
-    <row r="20" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U19" s="16">
+        <f>_xlfn.XLOOKUP(CN[[#This Row],[Neutral Strand AWG]], OH[Size], OH[Diam])</f>
+        <v>0.1019</v>
+      </c>
+      <c r="V19" s="16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="8"/>
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>

</xml_diff>

<commit_message>
fix naming bug in lineGeometries csv
</commit_message>
<xml_diff>
--- a/network-data/LineGeo_Selector.xlsx
+++ b/network-data/LineGeo_Selector.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spenceregan/Repos/CU/Distribution_Systems/Project1/ECEN5437-Proj1/network-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1FD2F1C-F0EA-3E44-BF9B-E5F60FA88A90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1FFA95-2472-A44E-88CD-91FB56DB7044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6640" yWindow="760" windowWidth="23600" windowHeight="17440" activeTab="1" xr2:uid="{7AEC5E2E-397B-8345-871E-9ED757579969}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="174">
   <si>
     <t>OH3p</t>
   </si>
@@ -559,9 +559,6 @@
   </si>
   <si>
     <t>Nphases</t>
-  </si>
-  <si>
-    <t>795_26/7_ACSR</t>
   </si>
   <si>
     <t>phase_cond</t>
@@ -2442,8 +2439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC2FAF4C-A38A-5148-8683-163D7FE8FD2D}">
   <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A26"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2981,7 +2978,7 @@
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3001,10 +2998,10 @@
         <v>33</v>
       </c>
       <c r="C1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D1" t="s">
         <v>173</v>
-      </c>
-      <c r="D1" t="s">
-        <v>174</v>
       </c>
       <c r="E1" t="s">
         <v>171</v>
@@ -3130,7 +3127,7 @@
         <v>75</v>
       </c>
       <c r="D4" t="s">
-        <v>172</v>
+        <v>75</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -3253,7 +3250,7 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3932,7 +3929,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4327,7 +4324,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5904AC-ECAC-4945-B9B6-B220AC818209}">
   <dimension ref="A1:N100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
@@ -8296,7 +8293,7 @@
   <dimension ref="A1:V20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
clean up line geometry compile
</commit_message>
<xml_diff>
--- a/network-data/LineGeo_Selector.xlsx
+++ b/network-data/LineGeo_Selector.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spenceregan/Repos/CU/Distribution_Systems/Project1/ECEN5437-Proj1/network-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1FFA95-2472-A44E-88CD-91FB56DB7044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004CB0E0-92D7-664E-951A-36363661CF60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6640" yWindow="760" windowWidth="23600" windowHeight="17440" activeTab="1" xr2:uid="{7AEC5E2E-397B-8345-871E-9ED757579969}"/>
+    <workbookView xWindow="45040" yWindow="320" windowWidth="23600" windowHeight="17440" activeTab="2" xr2:uid="{7AEC5E2E-397B-8345-871E-9ED757579969}"/>
   </bookViews>
   <sheets>
     <sheet name="Buses" sheetId="7" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="182">
   <si>
     <t>OH3p</t>
   </si>
@@ -565,6 +565,30 @@
   </si>
   <si>
     <t>neutral_cond</t>
+  </si>
+  <si>
+    <t>ac</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>cond_pos</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>ab</t>
+  </si>
+  <si>
+    <t>bc</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>c</t>
   </si>
 </sst>
 </file>
@@ -657,7 +681,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -682,12 +706,68 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="56">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -935,60 +1015,6 @@
         <vertAlign val="baseline"/>
         <sz val="12"/>
         <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -1887,24 +1913,48 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{43240ADB-710B-E440-9B4B-064F1493B981}" name="Buses" displayName="Buses" ref="A1:C47" totalsRowShown="0" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{43240ADB-710B-E440-9B4B-064F1493B981}" name="Buses" displayName="Buses" ref="A1:C47" totalsRowShown="0" dataDxfId="10">
   <autoFilter ref="A1:C47" xr:uid="{43240ADB-710B-E440-9B4B-064F1493B981}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{37E9F5EA-051D-BE40-B622-31D4B83CE6AA}" name="Bus" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{41D4B11A-15CC-A540-9052-95C4F3006357}" name="Graph_Loc_x" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{871540F1-C33C-6346-9F71-C67E6A5F5C63}" name="Graph_Loc_y" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{37E9F5EA-051D-BE40-B622-31D4B83CE6AA}" name="Bus" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{41D4B11A-15CC-A540-9052-95C4F3006357}" name="Graph_Loc_x" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{871540F1-C33C-6346-9F71-C67E6A5F5C63}" name="Graph_Loc_y" dataDxfId="11"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{13D01E9F-2651-EF45-A492-F190721E7BE9}" name="TS" displayName="TS" ref="A1:G10" totalsRowShown="0" headerRowDxfId="39" dataDxfId="40">
+  <autoFilter ref="A1:G10" xr:uid="{13D01E9F-2651-EF45-A492-F190721E7BE9}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{19CDDA2D-9812-404F-A70E-F8C42AD526DB}" name="Type" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{C1A0B38B-F04B-0A4C-913A-B68BB0D6C78E}" name="Diameter Over Insulation (in)" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{D6D141BB-2B57-4B4B-8667-6762392800DB}" name="Diameter Over Screen (in)" dataDxfId="45"/>
+    <tableColumn id="4" xr3:uid="{401114E4-AC5F-DA47-A949-534E36354F8D}" name="Jacket Thickness (mils)" dataDxfId="44"/>
+    <tableColumn id="5" xr3:uid="{244E8C6F-E27A-B344-A042-CF80AF18FA7C}" name="Outside Diameter" dataDxfId="43"/>
+    <tableColumn id="6" xr3:uid="{D80F22EC-CB8C-E549-AC7C-4BA81E9F5164}" name="Ampacity in UG Duct (A)" dataDxfId="42"/>
+    <tableColumn id="7" xr3:uid="{A989CB28-4027-F249-A88C-9A2D66CB1557}" name="Rated Voltage (kV)" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0AF27DE9-2ECA-6A4E-84A5-C298787FAAED}" name="LineGeo" displayName="LineGeo" ref="A1:O6" totalsRowShown="0">
-  <autoFilter ref="A1:O6" xr:uid="{0AF27DE9-2ECA-6A4E-84A5-C298787FAAED}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0AF27DE9-2ECA-6A4E-84A5-C298787FAAED}" name="LineGeo" displayName="LineGeo" ref="A1:P6" totalsRowShown="0">
+  <autoFilter ref="A1:P6" xr:uid="{0AF27DE9-2ECA-6A4E-84A5-C298787FAAED}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1920,8 +1970,9 @@
     <filterColumn colId="12" hiddenButton="1"/>
     <filterColumn colId="13" hiddenButton="1"/>
     <filterColumn colId="14" hiddenButton="1"/>
+    <filterColumn colId="15" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="15">
+  <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{2280FF94-C83E-444E-8E42-3510351A4DF6}" name="LineGeo"/>
     <tableColumn id="2" xr3:uid="{3DDFC765-300B-7846-9085-AB03B6A261F4}" name="Type"/>
     <tableColumn id="3" xr3:uid="{02F910B6-BE16-CE4C-89A1-71F43049235B}" name="phase_cond"/>
@@ -1939,13 +1990,14 @@
     <tableColumn id="11" xr3:uid="{F2274653-629E-134E-BBF5-C325DBF3EA16}" name="4_x"/>
     <tableColumn id="12" xr3:uid="{BD8B48A0-76F9-974B-9D8A-D27303D1602B}" name="4_z"/>
     <tableColumn id="15" xr3:uid="{25261513-8FAF-4F4C-AB29-7DAD255766AB}" name="Units"/>
+    <tableColumn id="16" xr3:uid="{5C4EE22D-BF12-B440-B404-EE8CFF19B8DA}" name="cond_pos"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{12D9EB82-8B48-7449-95A6-3BE76017FBF1}" name="Table7" displayName="Table7" ref="A1:E38" totalsRowShown="0" headerRowDxfId="12" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{12D9EB82-8B48-7449-95A6-3BE76017FBF1}" name="Table7" displayName="Table7" ref="A1:E38" totalsRowShown="0" headerRowDxfId="15" dataDxfId="16">
   <autoFilter ref="A1:E38" xr:uid="{12D9EB82-8B48-7449-95A6-3BE76017FBF1}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1955,26 +2007,26 @@
   </autoFilter>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{B526205E-98EF-F34B-B24D-F8218A008415}" name="bus1" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{D2CD9147-9358-C04D-8316-3FB3A9A16CB0}" name="bus2" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{99BA8C9D-330B-A24F-BC6C-A45D5466D8F3}" name="Length" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{24B6C05D-6629-B248-BB9C-1AF1BAA7ADB7}" name="LineGeometry" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{CDFF2292-878E-CE4B-BF6E-6CE7168C35B8}" name="Units" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{D2CD9147-9358-C04D-8316-3FB3A9A16CB0}" name="bus2" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{99BA8C9D-330B-A24F-BC6C-A45D5466D8F3}" name="Length" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{24B6C05D-6629-B248-BB9C-1AF1BAA7ADB7}" name="LineGeometry" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{CDFF2292-878E-CE4B-BF6E-6CE7168C35B8}" name="Units" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{CDAC5F4F-CC5E-714A-A10A-32F2E90176D7}" name="Table9" displayName="Table9" ref="A1:C28" totalsRowShown="0" headerRowDxfId="2" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{CDAC5F4F-CC5E-714A-A10A-32F2E90176D7}" name="Table9" displayName="Table9" ref="A1:C28" totalsRowShown="0" headerRowDxfId="5" dataDxfId="6">
   <autoFilter ref="A1:C28" xr:uid="{CDAC5F4F-CC5E-714A-A10A-32F2E90176D7}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{49EC89B8-2142-0A4A-B8EF-264BCDD715FA}" name="Bus" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{13C1D0C2-6357-484D-ADEB-105711D6B1A5}" name="kW" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{A5C493EA-CBB6-854A-A97A-1FDDCAB8D84F}" name="kVAr" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{49EC89B8-2142-0A4A-B8EF-264BCDD715FA}" name="Bus" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{13C1D0C2-6357-484D-ADEB-105711D6B1A5}" name="kW" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{A5C493EA-CBB6-854A-A97A-1FDDCAB8D84F}" name="kVAr" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1990,7 +2042,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{197E6DD9-1E95-E144-A54E-7BD8668CA6E8}" name="Units" displayName="Units" ref="C2:C8" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{197E6DD9-1E95-E144-A54E-7BD8668CA6E8}" name="Units" displayName="Units" ref="C1:C7" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{D4C1F671-A0A2-9147-89DB-D689DF977101}" name="Column1"/>
   </tableColumns>
@@ -1999,6 +2051,15 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{62FB5798-3249-9746-9DD5-608AFE9823D7}" name="Phases" displayName="Phases" ref="E1:E7" headerRowCount="0" totalsRowShown="0">
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{A5FD9FF9-B621-734F-9BCC-F153897F2CAB}" name="Column1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E4FB8847-4274-D04D-A64C-15B4CD5C8D60}" name="OH" displayName="OH" ref="A1:K100" totalsRowShown="0">
   <autoFilter ref="A1:K100" xr:uid="{E4FB8847-4274-D04D-A64C-15B4CD5C8D60}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -2038,7 +2099,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{661274D6-1D68-5542-8D94-45D5C86243F5}" name="CN" displayName="CN" ref="A1:V19" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46" tableBorderDxfId="55">
   <autoFilter ref="A1:V19" xr:uid="{661274D6-1D68-5542-8D94-45D5C86243F5}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -2107,34 +2168,10 @@
     <tableColumn id="20" xr3:uid="{D37687B3-1580-7845-A711-F39AB1A49147}" name="normamps" dataDxfId="18">
       <calculatedColumnFormula>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[normamps])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{D2E6A1F4-79B9-0D45-BE31-8E41DE3A29BC}" name="DiaStrand" dataDxfId="1">
+    <tableColumn id="22" xr3:uid="{D2E6A1F4-79B9-0D45-BE31-8E41DE3A29BC}" name="DiaStrand" dataDxfId="4">
       <calculatedColumnFormula>_xlfn.XLOOKUP(CN[[#This Row],[Neutral Strand AWG]], OH[Size], OH[Diam])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{E3B20767-C678-7E4D-8C37-6DA7A2305EDB}" name="Radunits" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{13D01E9F-2651-EF45-A492-F190721E7BE9}" name="TS" displayName="TS" ref="A1:G10" totalsRowShown="0" headerRowDxfId="39" dataDxfId="40">
-  <autoFilter ref="A1:G10" xr:uid="{13D01E9F-2651-EF45-A492-F190721E7BE9}">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-    <filterColumn colId="6" hiddenButton="1"/>
-  </autoFilter>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{19CDDA2D-9812-404F-A70E-F8C42AD526DB}" name="Type" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{C1A0B38B-F04B-0A4C-913A-B68BB0D6C78E}" name="Diameter Over Insulation (in)" dataDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{D6D141BB-2B57-4B4B-8667-6762392800DB}" name="Diameter Over Screen (in)" dataDxfId="45"/>
-    <tableColumn id="4" xr3:uid="{401114E4-AC5F-DA47-A949-534E36354F8D}" name="Jacket Thickness (mils)" dataDxfId="44"/>
-    <tableColumn id="5" xr3:uid="{244E8C6F-E27A-B344-A042-CF80AF18FA7C}" name="Outside Diameter" dataDxfId="43"/>
-    <tableColumn id="6" xr3:uid="{D80F22EC-CB8C-E549-AC7C-4BA81E9F5164}" name="Ampacity in UG Duct (A)" dataDxfId="42"/>
-    <tableColumn id="7" xr3:uid="{A989CB28-4027-F249-A88C-9A2D66CB1557}" name="Rated Voltage (kV)" dataDxfId="41"/>
+    <tableColumn id="23" xr3:uid="{E3B20767-C678-7E4D-8C37-6DA7A2305EDB}" name="Radunits" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2975,10 +3012,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF8D507D-491D-7543-AB0A-060D869CCAA9}">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2990,7 +3027,7 @@
     <col min="6" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>149</v>
       </c>
@@ -3036,8 +3073,11 @@
       <c r="O1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3083,8 +3123,11 @@
       <c r="O2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -3115,8 +3158,11 @@
       <c r="O3" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -3150,8 +3196,11 @@
       <c r="O4" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -3193,8 +3242,11 @@
       <c r="O5" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -3222,9 +3274,12 @@
       <c r="O6" t="s">
         <v>81</v>
       </c>
+      <c r="P6" t="s">
+        <v>177</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B6" xr:uid="{369739C0-1C03-AA46-834B-834C1A7F5EC8}">
       <formula1>INDIRECT("type")</formula1>
     </dataValidation>
@@ -3236,6 +3291,9 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O6" xr:uid="{C8CE36A8-15BC-CB4B-B80E-0326594F9F84}">
       <formula1>INDIRECT("Units")</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P6" xr:uid="{BBB7062F-A88A-A541-8E3E-2FE149FD666C}">
+      <formula1>INDIRECT("Phases")</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3249,8 +3307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3B959F-BA38-1C45-8F28-8937DDD91101}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3283,7 +3341,7 @@
       <c r="B2" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="C2" s="17">
+      <c r="C2" s="20">
         <v>15840</v>
       </c>
       <c r="D2" s="17" t="s">
@@ -3300,7 +3358,7 @@
       <c r="B3" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="C3" s="17">
+      <c r="C3" s="20">
         <v>15840</v>
       </c>
       <c r="D3" s="17" t="s">
@@ -3317,7 +3375,7 @@
       <c r="B4" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="20">
         <v>15840</v>
       </c>
       <c r="D4" s="17" t="s">
@@ -3334,7 +3392,7 @@
       <c r="B5" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="20">
         <v>15840</v>
       </c>
       <c r="D5" s="17" t="s">
@@ -3351,7 +3409,7 @@
       <c r="B6" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="20">
         <v>15840</v>
       </c>
       <c r="D6" s="17" t="s">
@@ -3368,7 +3426,7 @@
       <c r="B7" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="20">
         <v>15840</v>
       </c>
       <c r="D7" s="17" t="s">
@@ -3385,7 +3443,7 @@
       <c r="B8" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="20">
         <v>15840</v>
       </c>
       <c r="D8" s="17" t="s">
@@ -3402,7 +3460,7 @@
       <c r="B9" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="20">
         <v>15840</v>
       </c>
       <c r="D9" s="17" t="s">
@@ -3419,7 +3477,7 @@
       <c r="B10" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="20">
         <v>15840</v>
       </c>
       <c r="D10" s="17" t="s">
@@ -3436,7 +3494,7 @@
       <c r="B11" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="C11" s="17">
+      <c r="C11" s="20">
         <v>15840</v>
       </c>
       <c r="D11" s="17" t="s">
@@ -3453,7 +3511,7 @@
       <c r="B12" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="C12" s="17">
+      <c r="C12" s="20">
         <v>100</v>
       </c>
       <c r="D12" s="17" t="s">
@@ -3470,7 +3528,7 @@
       <c r="B13" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C13" s="20">
         <v>100</v>
       </c>
       <c r="D13" s="17" t="s">
@@ -3487,7 +3545,7 @@
       <c r="B14" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="C14" s="17">
+      <c r="C14" s="20">
         <v>100</v>
       </c>
       <c r="D14" s="17" t="s">
@@ -3504,7 +3562,7 @@
       <c r="B15" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="C15" s="17">
+      <c r="C15" s="20">
         <v>100</v>
       </c>
       <c r="D15" s="17" t="s">
@@ -3521,7 +3579,7 @@
       <c r="B16" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="C16" s="17">
+      <c r="C16" s="20">
         <v>100</v>
       </c>
       <c r="D16" s="17" t="s">
@@ -3538,7 +3596,7 @@
       <c r="B17" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="C17" s="17">
+      <c r="C17" s="20">
         <v>100</v>
       </c>
       <c r="D17" s="17" t="s">
@@ -3555,7 +3613,7 @@
       <c r="B18" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="C18" s="17">
+      <c r="C18" s="20">
         <v>100</v>
       </c>
       <c r="D18" s="17" t="s">
@@ -3572,7 +3630,7 @@
       <c r="B19" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="C19" s="17">
+      <c r="C19" s="20">
         <v>100</v>
       </c>
       <c r="D19" s="17" t="s">
@@ -3589,7 +3647,7 @@
       <c r="B20" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="C20" s="17">
+      <c r="C20" s="20">
         <v>100</v>
       </c>
       <c r="D20" s="17" t="s">
@@ -3606,7 +3664,7 @@
       <c r="B21" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="C21" s="17">
+      <c r="C21" s="20">
         <v>100</v>
       </c>
       <c r="D21" s="17" t="s">
@@ -3623,7 +3681,7 @@
       <c r="B22" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="C22" s="17">
+      <c r="C22" s="20">
         <v>100</v>
       </c>
       <c r="D22" s="17" t="s">
@@ -3640,7 +3698,7 @@
       <c r="B23" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="C23" s="17">
+      <c r="C23" s="20">
         <v>15840</v>
       </c>
       <c r="D23" s="17" t="s">
@@ -3657,7 +3715,7 @@
       <c r="B24" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="C24" s="17">
+      <c r="C24" s="20">
         <v>15840</v>
       </c>
       <c r="D24" s="17" t="s">
@@ -3674,7 +3732,7 @@
       <c r="B25" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="C25" s="17">
+      <c r="C25" s="20">
         <v>100</v>
       </c>
       <c r="D25" s="17" t="s">
@@ -3691,7 +3749,7 @@
       <c r="B26" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="C26" s="17">
+      <c r="C26" s="20">
         <v>100</v>
       </c>
       <c r="D26" s="17" t="s">
@@ -3708,7 +3766,7 @@
       <c r="B27" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="C27" s="17">
+      <c r="C27" s="20">
         <v>100</v>
       </c>
       <c r="D27" s="17" t="s">
@@ -3725,7 +3783,7 @@
       <c r="B28" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="C28" s="17">
+      <c r="C28" s="20">
         <v>100</v>
       </c>
       <c r="D28" s="17" t="s">
@@ -3742,7 +3800,7 @@
       <c r="B29" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="C29" s="17">
+      <c r="C29" s="20">
         <v>15840</v>
       </c>
       <c r="D29" s="17" t="s">
@@ -3759,7 +3817,7 @@
       <c r="B30" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="C30" s="17">
+      <c r="C30" s="20">
         <v>15840</v>
       </c>
       <c r="D30" s="17" t="s">
@@ -3776,7 +3834,7 @@
       <c r="B31" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="C31" s="17">
+      <c r="C31" s="20">
         <v>15840</v>
       </c>
       <c r="D31" s="17" t="s">
@@ -3793,7 +3851,7 @@
       <c r="B32" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="C32" s="17">
+      <c r="C32" s="20">
         <v>15840</v>
       </c>
       <c r="D32" s="17" t="s">
@@ -3810,7 +3868,7 @@
       <c r="B33" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="C33" s="17">
+      <c r="C33" s="20">
         <v>15840</v>
       </c>
       <c r="D33" s="17" t="s">
@@ -3827,7 +3885,7 @@
       <c r="B34" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="C34" s="17">
+      <c r="C34" s="20">
         <v>15840</v>
       </c>
       <c r="D34" s="17" t="s">
@@ -3844,7 +3902,7 @@
       <c r="B35" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="C35" s="17">
+      <c r="C35" s="20">
         <v>15840</v>
       </c>
       <c r="D35" s="17" t="s">
@@ -3861,7 +3919,7 @@
       <c r="B36" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="C36" s="17">
+      <c r="C36" s="20">
         <v>15840</v>
       </c>
       <c r="D36" s="17" t="s">
@@ -3878,7 +3936,7 @@
       <c r="B37" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="C37" s="17">
+      <c r="C37" s="20">
         <v>15840</v>
       </c>
       <c r="D37" s="17" t="s">
@@ -3895,7 +3953,7 @@
       <c r="B38" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="C38" s="17">
+      <c r="C38" s="20">
         <v>15840</v>
       </c>
       <c r="D38" s="17" t="s">
@@ -4257,65 +4315,85 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37ABA1BE-A562-EA4D-912C-91965FAA05A8}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>71</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+      <c r="E2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>72</v>
       </c>
       <c r="C3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+      <c r="E3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="E4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+      <c r="E5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+      <c r="E6" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C8" t="s">
         <v>83</v>
+      </c>
+      <c r="E7" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
add voltage plot feature
</commit_message>
<xml_diff>
--- a/network-data/LineGeo_Selector.xlsx
+++ b/network-data/LineGeo_Selector.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spenceregan/Repos/CU/Distribution_Systems/Project1/ECEN5437-Proj1/network-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D12106-575B-F640-9F87-A567B62F0E73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{937F87FB-243E-9042-BA2A-5801D19D25BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{7AEC5E2E-397B-8345-871E-9ED757579969}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="235">
   <si>
     <t>OH3p</t>
   </si>
@@ -649,9 +649,6 @@
     <t>1p_7.2_0.24_50_ww</t>
   </si>
   <si>
-    <t>1p_7.2_0.24_75_ww</t>
-  </si>
-  <si>
     <t>OH3pD</t>
   </si>
   <si>
@@ -749,6 +746,12 @@
   </si>
   <si>
     <t>CondPos</t>
+  </si>
+  <si>
+    <t>kV</t>
+  </si>
+  <si>
+    <t>1p_12.47_0.416_75_dd</t>
   </si>
 </sst>
 </file>
@@ -913,7 +916,25 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="92">
+  <dxfs count="93">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2557,16 +2578,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{43240ADB-710B-E440-9B4B-064F1493B981}" name="Buses" displayName="Buses" ref="A1:C47" totalsRowShown="0" dataDxfId="91">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{43240ADB-710B-E440-9B4B-064F1493B981}" name="Buses" displayName="Buses" ref="A1:C47" totalsRowShown="0" dataDxfId="92">
   <autoFilter ref="A1:C47" xr:uid="{43240ADB-710B-E440-9B4B-064F1493B981}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{37E9F5EA-051D-BE40-B622-31D4B83CE6AA}" name="Bus" dataDxfId="90"/>
-    <tableColumn id="2" xr3:uid="{41D4B11A-15CC-A540-9052-95C4F3006357}" name="Graph_Loc_x" dataDxfId="89"/>
-    <tableColumn id="3" xr3:uid="{871540F1-C33C-6346-9F71-C67E6A5F5C63}" name="Graph_Loc_y" dataDxfId="88"/>
+    <tableColumn id="1" xr3:uid="{37E9F5EA-051D-BE40-B622-31D4B83CE6AA}" name="Bus" dataDxfId="91"/>
+    <tableColumn id="2" xr3:uid="{41D4B11A-15CC-A540-9052-95C4F3006357}" name="Graph_Loc_x" dataDxfId="90"/>
+    <tableColumn id="3" xr3:uid="{871540F1-C33C-6346-9F71-C67E6A5F5C63}" name="Graph_Loc_y" dataDxfId="89"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2591,45 +2612,45 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{5F3073CA-6F2C-7643-A086-B783E9581317}" name="delta.delta" displayName="delta.delta" ref="H2:H7" headerRowCount="0" totalsRowShown="0" headerRowDxfId="20" dataDxfId="21" tableBorderDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{5F3073CA-6F2C-7643-A086-B783E9581317}" name="delta.delta" displayName="delta.delta" ref="H2:H7" headerRowCount="0" totalsRowShown="0" headerRowDxfId="21" dataDxfId="22" tableBorderDxfId="24">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{50958CF2-21D9-984F-97B5-085C4560A350}" name="Column1" headerRowDxfId="19" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{50958CF2-21D9-984F-97B5-085C4560A350}" name="Column1" headerRowDxfId="20" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{89D1A629-368D-0B4B-8525-B86A48878238}" name="delta.wye" displayName="delta.wye" ref="I2:I5" headerRowCount="0" totalsRowShown="0" headerRowDxfId="17" tableBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{89D1A629-368D-0B4B-8525-B86A48878238}" name="delta.wye" displayName="delta.wye" ref="I2:I5" headerRowCount="0" totalsRowShown="0" headerRowDxfId="18" tableBorderDxfId="19">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{A3625009-C857-274F-A122-CFD46E3541C5}" name="Column1" headerRowDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{A3625009-C857-274F-A122-CFD46E3541C5}" name="Column1" headerRowDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{D6E2BF91-ACF1-C849-9AC2-F7ED9921C73E}" name="wye.delta" displayName="wye.delta" ref="J2:J5" headerRowCount="0" totalsRowShown="0" headerRowDxfId="14" tableBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{D6E2BF91-ACF1-C849-9AC2-F7ED9921C73E}" name="wye.delta" displayName="wye.delta" ref="J2:J5" headerRowCount="0" totalsRowShown="0" headerRowDxfId="15" tableBorderDxfId="16">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{147B4193-B138-D749-BACA-A6E839012CE7}" name="Column1" headerRowDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{147B4193-B138-D749-BACA-A6E839012CE7}" name="Column1" headerRowDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{32FF552F-94F8-5F4A-A3CD-0CF8C4344854}" name="wye.wye" displayName="wye.wye" ref="K2:K3" headerRowCount="0" totalsRowShown="0" headerRowDxfId="11" tableBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{32FF552F-94F8-5F4A-A3CD-0CF8C4344854}" name="wye.wye" displayName="wye.wye" ref="K2:K3" headerRowCount="0" totalsRowShown="0" headerRowDxfId="12" tableBorderDxfId="13">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{9713DCA2-8057-6941-AB28-861C6CAD34E9}" name="Column1" headerRowDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{9713DCA2-8057-6941-AB28-861C6CAD34E9}" name="Column1" headerRowDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{F85F963E-7E0D-DA40-BC57-8F71010CE834}" name="Terminals" displayName="Terminals" ref="O1:O15" headerRowCount="0" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{F85F963E-7E0D-DA40-BC57-8F71010CE834}" name="Terminals" displayName="Terminals" ref="O1:O15" headerRowCount="0" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{B57E695F-4DAF-C041-9D98-90DA0E9FCF30}" name="Column1" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{B57E695F-4DAF-C041-9D98-90DA0E9FCF30}" name="Column1" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2660,23 +2681,23 @@
     <filterColumn colId="10" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{E903BA16-38F3-EE44-A1B4-2B0F344DDB1D}" name="Type" dataDxfId="62">
+    <tableColumn id="1" xr3:uid="{E903BA16-38F3-EE44-A1B4-2B0F344DDB1D}" name="Type" dataDxfId="63">
       <calculatedColumnFormula>_xlfn.CONCAT(OH[[#This Row],[Size]], "_",OH[[#This Row],[Stranding]], "_", OH[[#This Row],[Material]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{B69CA351-3694-B545-8563-7479CF50BC67}" name="Size" dataDxfId="61"/>
+    <tableColumn id="2" xr3:uid="{B69CA351-3694-B545-8563-7479CF50BC67}" name="Size" dataDxfId="62"/>
     <tableColumn id="3" xr3:uid="{3576FC0F-75EE-6F4B-B709-5C5715FE540E}" name="Stranding"/>
     <tableColumn id="4" xr3:uid="{C31618D9-7DA8-804A-A013-69A802FF7774}" name="Material"/>
     <tableColumn id="5" xr3:uid="{804C85FC-06A5-4645-A278-FD8271A5F0ED}" name="Diam"/>
     <tableColumn id="6" xr3:uid="{ED80EC98-63E4-C94C-BAF3-F13294EE8381}" name="GMRac"/>
     <tableColumn id="7" xr3:uid="{41A91B17-FB89-1F4F-899A-3761661447FD}" name="rac"/>
     <tableColumn id="8" xr3:uid="{C9144B25-D7C0-D444-8605-CEBD77A9171D}" name="normamps"/>
-    <tableColumn id="13" xr3:uid="{041E70E4-975E-254A-81CF-95C5EF9E73D2}" name="GMRunits" dataDxfId="60">
+    <tableColumn id="13" xr3:uid="{041E70E4-975E-254A-81CF-95C5EF9E73D2}" name="GMRunits" dataDxfId="61">
       <calculatedColumnFormula>"ft"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{2AEFB39D-D6D8-D14D-A990-9BB4F5164639}" name="runits" dataDxfId="59">
+    <tableColumn id="14" xr3:uid="{2AEFB39D-D6D8-D14D-A990-9BB4F5164639}" name="runits" dataDxfId="60">
       <calculatedColumnFormula>"mi"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{21A61F38-5A94-2142-A9A8-D6E0BB77AB1E}" name="Size_Material" dataDxfId="58">
+    <tableColumn id="15" xr3:uid="{21A61F38-5A94-2142-A9A8-D6E0BB77AB1E}" name="Size_Material" dataDxfId="59">
       <calculatedColumnFormula>_xlfn.CONCAT(OH[[#This Row],[Size]], "_", OH[[#This Row],[Material]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2685,7 +2706,7 @@
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{661274D6-1D68-5542-8D94-45D5C86243F5}" name="CN" displayName="CN" ref="A1:V19" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56" tableBorderDxfId="55">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{661274D6-1D68-5542-8D94-45D5C86243F5}" name="CN" displayName="CN" ref="A1:V19" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57" tableBorderDxfId="56">
   <autoFilter ref="A1:V19" xr:uid="{661274D6-1D68-5542-8D94-45D5C86243F5}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2711,52 +2732,52 @@
     <filterColumn colId="21" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="22">
-    <tableColumn id="9" xr3:uid="{869F190C-19C4-2243-84CA-F6CB8F4281C2}" name="Type" dataDxfId="54">
+    <tableColumn id="9" xr3:uid="{869F190C-19C4-2243-84CA-F6CB8F4281C2}" name="Type" dataDxfId="55">
       <calculatedColumnFormula>_xlfn.CONCAT(CN[[#This Row],[Neutral Ampacity]], "_", CN[[#This Row],[Conductor Size]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{1DFBB787-8CEC-A946-969E-C8B3E35D5AEB}" name="Neutral Ampacity" dataDxfId="53"/>
-    <tableColumn id="2" xr3:uid="{EFDAEEF3-E5BA-4B49-BA44-2340320EA290}" name="Conductor Size" dataDxfId="52"/>
-    <tableColumn id="18" xr3:uid="{703A2A0A-5882-4349-9ACB-A05C1C032238}" name="Phase Conductor Name" dataDxfId="51">
+    <tableColumn id="1" xr3:uid="{1DFBB787-8CEC-A946-969E-C8B3E35D5AEB}" name="Neutral Ampacity" dataDxfId="54"/>
+    <tableColumn id="2" xr3:uid="{EFDAEEF3-E5BA-4B49-BA44-2340320EA290}" name="Conductor Size" dataDxfId="53"/>
+    <tableColumn id="18" xr3:uid="{703A2A0A-5882-4349-9ACB-A05C1C032238}" name="Phase Conductor Name" dataDxfId="52">
       <calculatedColumnFormula>_xlfn.XLOOKUP(_xlfn.CONCAT(LEFT(CN[[#This Row],[Conductor Size]], SEARCH("(", CN[[#This Row],[Conductor Size]])-1), "_AA"), OH[Size_Material], OH[Type], NA(),-1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8E5F5E70-58CE-0D4E-A970-1B53EA80FE07}" name="DiaIns" dataDxfId="50"/>
-    <tableColumn id="4" xr3:uid="{D154B6B5-D516-AC44-879B-B0BC6ACADF64}" name="Diameter Over Screen (in)" dataDxfId="49"/>
-    <tableColumn id="5" xr3:uid="{51092775-E14C-4945-BD12-6F609313AC1A}" name="DiaCable" dataDxfId="48"/>
-    <tableColumn id="6" xr3:uid="{FE25AF87-2C02-C642-B28A-81AF2224011F}" name="Copper Neutral" dataDxfId="47"/>
-    <tableColumn id="7" xr3:uid="{167EFF3D-5388-5C47-9405-F0CE90C78333}" name="Ampacity in Underground Duct (A)" dataDxfId="46"/>
-    <tableColumn id="8" xr3:uid="{D4CA2780-FAB4-FE44-BAA2-A16B53A68DE8}" name="Voltage Rating (kV)" dataDxfId="45"/>
-    <tableColumn id="11" xr3:uid="{830817DB-B122-D444-8DFC-58C1CE7D7901}" name="Neutral Strand AWG" dataDxfId="44" dataCellStyle="Percent">
+    <tableColumn id="3" xr3:uid="{8E5F5E70-58CE-0D4E-A970-1B53EA80FE07}" name="DiaIns" dataDxfId="51"/>
+    <tableColumn id="4" xr3:uid="{D154B6B5-D516-AC44-879B-B0BC6ACADF64}" name="Diameter Over Screen (in)" dataDxfId="50"/>
+    <tableColumn id="5" xr3:uid="{51092775-E14C-4945-BD12-6F609313AC1A}" name="DiaCable" dataDxfId="49"/>
+    <tableColumn id="6" xr3:uid="{FE25AF87-2C02-C642-B28A-81AF2224011F}" name="Copper Neutral" dataDxfId="48"/>
+    <tableColumn id="7" xr3:uid="{167EFF3D-5388-5C47-9405-F0CE90C78333}" name="Ampacity in Underground Duct (A)" dataDxfId="47"/>
+    <tableColumn id="8" xr3:uid="{D4CA2780-FAB4-FE44-BAA2-A16B53A68DE8}" name="Voltage Rating (kV)" dataDxfId="46"/>
+    <tableColumn id="11" xr3:uid="{830817DB-B122-D444-8DFC-58C1CE7D7901}" name="Neutral Strand AWG" dataDxfId="45" dataCellStyle="Percent">
       <calculatedColumnFormula>VALUE(RIGHT(CN[[#This Row],[Copper Neutral]],2))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{A0775550-BA03-5542-A01E-64482C59971C}" name="Rstrand" dataDxfId="43">
+    <tableColumn id="10" xr3:uid="{A0775550-BA03-5542-A01E-64482C59971C}" name="Rstrand" dataDxfId="44">
       <calculatedColumnFormula>_xlfn.XLOOKUP(CN[[#This Row],[Neutral Strand AWG]], OH[Size], OH[rac])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{4B541559-291A-4941-9353-F59C621A9E18}" name="k" dataDxfId="42">
+    <tableColumn id="12" xr3:uid="{4B541559-291A-4941-9353-F59C621A9E18}" name="k" dataDxfId="43">
       <calculatedColumnFormula>VALUE(LEFT(CN[[#This Row],[Copper Neutral]], SEARCH(" ",CN[[#This Row],[Copper Neutral]])-1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{60128454-1EE5-9C4B-9AA2-D0CE6F9C4CF7}" name="GMRac" dataDxfId="41">
+    <tableColumn id="13" xr3:uid="{60128454-1EE5-9C4B-9AA2-D0CE6F9C4CF7}" name="GMRac" dataDxfId="42">
       <calculatedColumnFormula>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]], OH[Type], OH[GMRac])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{AA242217-BC74-AB48-8D9A-86A3970B8399}" name="GmrStrand" dataDxfId="40">
+    <tableColumn id="14" xr3:uid="{AA242217-BC74-AB48-8D9A-86A3970B8399}" name="GmrStrand" dataDxfId="41">
       <calculatedColumnFormula>_xlfn.XLOOKUP(CN[[#This Row],[Neutral Strand AWG]], OH[Size], OH[GMRac])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{BDF03C79-D2AE-394A-9557-0FEAE0AA392C}" name="GMRunits" dataDxfId="39"/>
-    <tableColumn id="16" xr3:uid="{E6B7FA4C-2968-AE41-84BD-9EA25CF9A089}" name="Rac" dataDxfId="38">
+    <tableColumn id="15" xr3:uid="{BDF03C79-D2AE-394A-9557-0FEAE0AA392C}" name="GMRunits" dataDxfId="40"/>
+    <tableColumn id="16" xr3:uid="{E6B7FA4C-2968-AE41-84BD-9EA25CF9A089}" name="Rac" dataDxfId="39">
       <calculatedColumnFormula>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[rac])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{60CA6D09-ACAD-FA47-9A7F-D8BCB54C2191}" name="Runits" dataDxfId="37">
+    <tableColumn id="17" xr3:uid="{60CA6D09-ACAD-FA47-9A7F-D8BCB54C2191}" name="Runits" dataDxfId="38">
       <calculatedColumnFormula>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[runits])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{A335B60A-8482-494F-9920-64B3CC7615EB}" name="diam" dataDxfId="36">
+    <tableColumn id="19" xr3:uid="{A335B60A-8482-494F-9920-64B3CC7615EB}" name="diam" dataDxfId="37">
       <calculatedColumnFormula>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[Diam])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{D37687B3-1580-7845-A711-F39AB1A49147}" name="normamps" dataDxfId="35">
+    <tableColumn id="20" xr3:uid="{D37687B3-1580-7845-A711-F39AB1A49147}" name="normamps" dataDxfId="36">
       <calculatedColumnFormula>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[normamps])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{D2E6A1F4-79B9-0D45-BE31-8E41DE3A29BC}" name="DiaStrand" dataDxfId="34">
+    <tableColumn id="22" xr3:uid="{D2E6A1F4-79B9-0D45-BE31-8E41DE3A29BC}" name="DiaStrand" dataDxfId="35">
       <calculatedColumnFormula>_xlfn.XLOOKUP(CN[[#This Row],[Neutral Strand AWG]], OH[Size], OH[Diam])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{E3B20767-C678-7E4D-8C37-6DA7A2305EDB}" name="Radunits" dataDxfId="33"/>
+    <tableColumn id="23" xr3:uid="{E3B20767-C678-7E4D-8C37-6DA7A2305EDB}" name="Radunits" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2786,7 +2807,7 @@
     <tableColumn id="1" xr3:uid="{2280FF94-C83E-444E-8E42-3510351A4DF6}" name="LineGeo"/>
     <tableColumn id="2" xr3:uid="{3DDFC765-300B-7846-9085-AB03B6A261F4}" name="Type"/>
     <tableColumn id="3" xr3:uid="{02F910B6-BE16-CE4C-89A1-71F43049235B}" name="phase_cond"/>
-    <tableColumn id="4" xr3:uid="{520CD3FE-AB23-3943-8829-73CAAC013F53}" name="neutral_cond" dataDxfId="87">
+    <tableColumn id="4" xr3:uid="{520CD3FE-AB23-3943-8829-73CAAC013F53}" name="neutral_cond" dataDxfId="88">
       <calculatedColumnFormula>IF(LineGeo[[#This Row],[Type]]="OH",1,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="13" xr3:uid="{DE9BDE1B-5E39-604D-9957-E0C3A3473BC8}" name="Nphases"/>
@@ -2807,7 +2828,7 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{13D01E9F-2651-EF45-A492-F190721E7BE9}" name="TS" displayName="TS" ref="A1:G10" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{13D01E9F-2651-EF45-A492-F190721E7BE9}" name="TS" displayName="TS" ref="A1:G10" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
   <autoFilter ref="A1:G10" xr:uid="{13D01E9F-2651-EF45-A492-F190721E7BE9}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2818,20 +2839,20 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{19CDDA2D-9812-404F-A70E-F8C42AD526DB}" name="Type" dataDxfId="30"/>
-    <tableColumn id="2" xr3:uid="{C1A0B38B-F04B-0A4C-913A-B68BB0D6C78E}" name="Diameter Over Insulation (in)" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{D6D141BB-2B57-4B4B-8667-6762392800DB}" name="Diameter Over Screen (in)" dataDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{401114E4-AC5F-DA47-A949-534E36354F8D}" name="Jacket Thickness (mils)" dataDxfId="27"/>
-    <tableColumn id="5" xr3:uid="{244E8C6F-E27A-B344-A042-CF80AF18FA7C}" name="Outside Diameter" dataDxfId="26"/>
-    <tableColumn id="6" xr3:uid="{D80F22EC-CB8C-E549-AC7C-4BA81E9F5164}" name="Ampacity in UG Duct (A)" dataDxfId="25"/>
-    <tableColumn id="7" xr3:uid="{A989CB28-4027-F249-A88C-9A2D66CB1557}" name="Rated Voltage (kV)" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{19CDDA2D-9812-404F-A70E-F8C42AD526DB}" name="Type" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{C1A0B38B-F04B-0A4C-913A-B68BB0D6C78E}" name="Diameter Over Insulation (in)" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{D6D141BB-2B57-4B4B-8667-6762392800DB}" name="Diameter Over Screen (in)" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{401114E4-AC5F-DA47-A949-534E36354F8D}" name="Jacket Thickness (mils)" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{244E8C6F-E27A-B344-A042-CF80AF18FA7C}" name="Outside Diameter" dataDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{D80F22EC-CB8C-E549-AC7C-4BA81E9F5164}" name="Ampacity in UG Duct (A)" dataDxfId="26"/>
+    <tableColumn id="7" xr3:uid="{A989CB28-4027-F249-A88C-9A2D66CB1557}" name="Rated Voltage (kV)" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{12D9EB82-8B48-7449-95A6-3BE76017FBF1}" name="Lines" displayName="Lines" ref="A1:G39" totalsRowShown="0" headerRowDxfId="86" dataDxfId="85">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{12D9EB82-8B48-7449-95A6-3BE76017FBF1}" name="Lines" displayName="Lines" ref="A1:G39" totalsRowShown="0" headerRowDxfId="87" dataDxfId="86">
   <autoFilter ref="A1:G39" xr:uid="{12D9EB82-8B48-7449-95A6-3BE76017FBF1}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2842,15 +2863,15 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{B526205E-98EF-F34B-B24D-F8218A008415}" name="bus1" dataDxfId="84"/>
-    <tableColumn id="2" xr3:uid="{D2CD9147-9358-C04D-8316-3FB3A9A16CB0}" name="bus2" dataDxfId="83"/>
-    <tableColumn id="3" xr3:uid="{99BA8C9D-330B-A24F-BC6C-A45D5466D8F3}" name="Length" dataDxfId="82"/>
-    <tableColumn id="4" xr3:uid="{24B6C05D-6629-B248-BB9C-1AF1BAA7ADB7}" name="LineGeometry" dataDxfId="81"/>
-    <tableColumn id="5" xr3:uid="{CDFF2292-878E-CE4B-BF6E-6CE7168C35B8}" name="Units" dataDxfId="80"/>
-    <tableColumn id="6" xr3:uid="{A8C38B34-2B32-C444-89AA-FDCCE25A82B7}" name="phases" dataDxfId="79">
+    <tableColumn id="1" xr3:uid="{B526205E-98EF-F34B-B24D-F8218A008415}" name="bus1" dataDxfId="85"/>
+    <tableColumn id="2" xr3:uid="{D2CD9147-9358-C04D-8316-3FB3A9A16CB0}" name="bus2" dataDxfId="84"/>
+    <tableColumn id="3" xr3:uid="{99BA8C9D-330B-A24F-BC6C-A45D5466D8F3}" name="Length" dataDxfId="83"/>
+    <tableColumn id="4" xr3:uid="{24B6C05D-6629-B248-BB9C-1AF1BAA7ADB7}" name="LineGeometry" dataDxfId="82"/>
+    <tableColumn id="5" xr3:uid="{CDFF2292-878E-CE4B-BF6E-6CE7168C35B8}" name="Units" dataDxfId="81"/>
+    <tableColumn id="6" xr3:uid="{A8C38B34-2B32-C444-89AA-FDCCE25A82B7}" name="phases" dataDxfId="80">
       <calculatedColumnFormula>_xlfn.XLOOKUP(Lines[[#This Row],[LineGeometry]],LineGeo[LineGeo],LineGeo[Nphases],0,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{17578AEA-5626-6A4C-B5EA-E2A9D6CF3223}" name="cond_pos" dataDxfId="78"/>
+    <tableColumn id="7" xr3:uid="{17578AEA-5626-6A4C-B5EA-E2A9D6CF3223}" name="cond_pos" dataDxfId="79"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2881,42 +2902,42 @@
     <tableColumn id="1" xr3:uid="{C58B47F9-739B-7B49-8572-5CF966DE57BF}" name="bus1"/>
     <tableColumn id="2" xr3:uid="{158E1C6F-2E86-A24E-A99E-F710460471A4}" name="bus2"/>
     <tableColumn id="3" xr3:uid="{1B8A6996-3AB7-224A-9AD8-27ED161B7D10}" name="xfmr"/>
-    <tableColumn id="4" xr3:uid="{A79FA7AF-C14D-2742-9392-2561ECAD3C4C}" name="kV1" dataDxfId="77">
+    <tableColumn id="4" xr3:uid="{A79FA7AF-C14D-2742-9392-2561ECAD3C4C}" name="kV1" dataDxfId="78">
       <calculatedColumnFormula>_xlfn.XLOOKUP(xfmrs[[#This Row],[xfmr]],xfmr_info[name],xfmr_info[kV_hv])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{8898BF2A-8518-E04A-9A6E-42AD088D8F6E}" name="kV2" dataDxfId="76">
+    <tableColumn id="5" xr3:uid="{8898BF2A-8518-E04A-9A6E-42AD088D8F6E}" name="kV2" dataDxfId="77">
       <calculatedColumnFormula>_xlfn.XLOOKUP(xfmrs[[#This Row],[xfmr]],xfmr_info[name],xfmr_info[kV_lv])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{D42902E7-C227-5B41-97A8-6AC8DF21E53C}" name="kVA1" dataDxfId="75">
+    <tableColumn id="6" xr3:uid="{D42902E7-C227-5B41-97A8-6AC8DF21E53C}" name="kVA1" dataDxfId="76">
       <calculatedColumnFormula>_xlfn.XLOOKUP(xfmrs[[#This Row],[xfmr]],xfmr_info[name],xfmr_info[kVA_hv])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{0BB098D2-D583-2146-8233-4EB095563D38}" name="kVA2" dataDxfId="74">
+    <tableColumn id="7" xr3:uid="{0BB098D2-D583-2146-8233-4EB095563D38}" name="kVA2" dataDxfId="75">
       <calculatedColumnFormula>_xlfn.XLOOKUP(xfmrs[[#This Row],[xfmr]],xfmr_info[name],xfmr_info[kVA_lv])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{1CE6ACB7-BD5A-BC43-86B4-D28A657C67B3}" name="conn1" dataDxfId="73">
+    <tableColumn id="8" xr3:uid="{1CE6ACB7-BD5A-BC43-86B4-D28A657C67B3}" name="conn1" dataDxfId="74">
       <calculatedColumnFormula>_xlfn.XLOOKUP(xfmrs[[#This Row],[xfmr]],xfmr_info[name],xfmr_info[Conn_hv])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{C1CD392B-A1E0-0E4D-9644-885A2CBC3563}" name="conn2" dataDxfId="72">
+    <tableColumn id="9" xr3:uid="{C1CD392B-A1E0-0E4D-9644-885A2CBC3563}" name="conn2" dataDxfId="73">
       <calculatedColumnFormula>_xlfn.XLOOKUP(xfmrs[[#This Row],[xfmr]],xfmr_info[name],xfmr_info[Conn_lv])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{D8DF443B-AF1C-264C-B64F-7EA66CBF65CC}" name="phases" dataDxfId="71">
+    <tableColumn id="10" xr3:uid="{D8DF443B-AF1C-264C-B64F-7EA66CBF65CC}" name="phases" dataDxfId="72">
       <calculatedColumnFormula>_xlfn.XLOOKUP(xfmrs[[#This Row],[xfmr]],xfmr_info[name],xfmr_info[Phases])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{5D9B233F-211C-BB47-9D7B-6B064811AE23}" name="windings" dataDxfId="3">
+    <tableColumn id="17" xr3:uid="{5D9B233F-211C-BB47-9D7B-6B064811AE23}" name="windings" dataDxfId="4">
       <calculatedColumnFormula>_xlfn.XLOOKUP(xfmrs[[#This Row],[xfmr]],xfmr_info[name],xfmr_info[Windings])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{2F73D725-1EF1-1646-AA1B-30806683307E}" name="R" dataDxfId="70">
+    <tableColumn id="11" xr3:uid="{2F73D725-1EF1-1646-AA1B-30806683307E}" name="R" dataDxfId="71">
       <calculatedColumnFormula>_xlfn.XLOOKUP(xfmrs[[#This Row],[xfmr]],xfmr_info[name],xfmr_info[R])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{5F54EB82-97EC-3641-9FD1-9EEAA4487A8C}" name="X" dataDxfId="69">
+    <tableColumn id="12" xr3:uid="{5F54EB82-97EC-3641-9FD1-9EEAA4487A8C}" name="X" dataDxfId="70">
       <calculatedColumnFormula>_xlfn.XLOOKUP(xfmrs[[#This Row],[xfmr]],xfmr_info[name],xfmr_info[X])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{5282C155-D5E7-FE49-8966-957D05B4F3D9}" name="nll" dataDxfId="4">
+    <tableColumn id="16" xr3:uid="{5282C155-D5E7-FE49-8966-957D05B4F3D9}" name="nll" dataDxfId="5">
       <calculatedColumnFormula>_xlfn.XLOOKUP(xfmrs[[#This Row],[xfmr]],xfmr_info[name],xfmr_info[nll])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{E19CAE52-E835-E54E-AC02-9A56DE7EC44D}" name="wnd1_terms" dataDxfId="6"/>
-    <tableColumn id="15" xr3:uid="{2AB55424-E657-6C44-A327-3B7EE71D6C9C}" name="wnd2_terms" dataDxfId="5"/>
-    <tableColumn id="18" xr3:uid="{69DA4BCE-2C58-0041-8D38-B07D3A767A8F}" name="wnd3_terms" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{E19CAE52-E835-E54E-AC02-9A56DE7EC44D}" name="wnd1_terms" dataDxfId="7"/>
+    <tableColumn id="15" xr3:uid="{2AB55424-E657-6C44-A327-3B7EE71D6C9C}" name="wnd2_terms" dataDxfId="6"/>
+    <tableColumn id="18" xr3:uid="{69DA4BCE-2C58-0041-8D38-B07D3A767A8F}" name="wnd3_terms" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2950,7 +2971,7 @@
     <tableColumn id="8" xr3:uid="{09E2D732-A304-6944-A2A0-1E51DBA4E1E9}" name="R"/>
     <tableColumn id="9" xr3:uid="{A6AD2380-16CB-204C-9DFD-B5F4D1F1AE3E}" name="X"/>
     <tableColumn id="11" xr3:uid="{54C6ABFF-F2E2-8047-9CFE-C8400D4265CF}" name="nll"/>
-    <tableColumn id="10" xr3:uid="{3027DC48-8D18-414F-A817-B76322236057}" name="name" dataDxfId="68">
+    <tableColumn id="10" xr3:uid="{3027DC48-8D18-414F-A817-B76322236057}" name="name" dataDxfId="69">
       <calculatedColumnFormula>_xlfn.CONCAT(xfmr_info[[#This Row],[Phases]],"p_",xfmr_info[[#This Row],[kV_hv]],"_",xfmr_info[[#This Row],[kV_lv]],"_",xfmr_info[[#This Row],[kVA_hv]],"_",LEFT(xfmr_info[[#This Row],[Conn_hv]],1),LEFT(xfmr_info[[#This Row],[Conn_lv]],1))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2959,22 +2980,24 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{CDAC5F4F-CC5E-714A-A10A-32F2E90176D7}" name="Loads" displayName="Loads" ref="A1:E28" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66">
-  <autoFilter ref="A1:E28" xr:uid="{CDAC5F4F-CC5E-714A-A10A-32F2E90176D7}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{CDAC5F4F-CC5E-714A-A10A-32F2E90176D7}" name="Loads" displayName="Loads" ref="A1:F28" totalsRowShown="0" headerRowDxfId="68" dataDxfId="67">
+  <autoFilter ref="A1:F28" xr:uid="{CDAC5F4F-CC5E-714A-A10A-32F2E90176D7}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
     <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{49EC89B8-2142-0A4A-B8EF-264BCDD715FA}" name="Bus" dataDxfId="65"/>
-    <tableColumn id="4" xr3:uid="{82843DB1-8D81-4741-83BB-3717AB506BFA}" name="Phases" dataDxfId="64">
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{49EC89B8-2142-0A4A-B8EF-264BCDD715FA}" name="Bus" dataDxfId="66"/>
+    <tableColumn id="4" xr3:uid="{82843DB1-8D81-4741-83BB-3717AB506BFA}" name="Phases" dataDxfId="65">
       <calculatedColumnFormula>_xlfn.XLOOKUP(Loads[[#This Row],[Bus]],Lines[bus2],Lines[phases],_xlfn.XLOOKUP(Loads[[#This Row],[Bus]],xfmrs[bus2],xfmrs[phases],0,0),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{13C1D0C2-6357-484D-ADEB-105711D6B1A5}" name="kW" dataDxfId="63"/>
-    <tableColumn id="3" xr3:uid="{A5C493EA-CBB6-854A-A97A-1FDDCAB8D84F}" name="kVAr" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{8D3CD5DC-3C01-EA41-B07F-F5CDB2FF56B0}" name="CondPos" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{13C1D0C2-6357-484D-ADEB-105711D6B1A5}" name="kW" dataDxfId="64"/>
+    <tableColumn id="3" xr3:uid="{A5C493EA-CBB6-854A-A97A-1FDDCAB8D84F}" name="kVAr" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{8D3CD5DC-3C01-EA41-B07F-F5CDB2FF56B0}" name="CondPos" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{65FC770D-1F3B-D142-9FDE-8782A4D0FBBA}" name="kV" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9909,7 +9932,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B7" t="s">
         <v>70</v>
@@ -9978,7 +10001,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10247,7 +10270,8 @@
         <v>81</v>
       </c>
       <c r="F12" s="10">
-        <v>1</v>
+        <f>_xlfn.XLOOKUP(Lines[[#This Row],[LineGeometry]],LineGeo[LineGeo],LineGeo[Nphases],0,0)</f>
+        <v>2</v>
       </c>
       <c r="G12" s="10"/>
     </row>
@@ -10268,7 +10292,8 @@
         <v>81</v>
       </c>
       <c r="F13" s="10">
-        <v>1</v>
+        <f>_xlfn.XLOOKUP(Lines[[#This Row],[LineGeometry]],LineGeo[LineGeo],LineGeo[Nphases],0,0)</f>
+        <v>2</v>
       </c>
       <c r="G13" s="10"/>
     </row>
@@ -10289,7 +10314,8 @@
         <v>81</v>
       </c>
       <c r="F14" s="10">
-        <v>1</v>
+        <f>_xlfn.XLOOKUP(Lines[[#This Row],[LineGeometry]],LineGeo[LineGeo],LineGeo[Nphases],0,0)</f>
+        <v>2</v>
       </c>
       <c r="G14" s="10"/>
     </row>
@@ -10310,7 +10336,8 @@
         <v>81</v>
       </c>
       <c r="F15" s="10">
-        <v>1</v>
+        <f>_xlfn.XLOOKUP(Lines[[#This Row],[LineGeometry]],LineGeo[LineGeo],LineGeo[Nphases],0,0)</f>
+        <v>2</v>
       </c>
       <c r="G15" s="10"/>
     </row>
@@ -10331,7 +10358,8 @@
         <v>81</v>
       </c>
       <c r="F16" s="10">
-        <v>1</v>
+        <f>_xlfn.XLOOKUP(Lines[[#This Row],[LineGeometry]],LineGeo[LineGeo],LineGeo[Nphases],0,0)</f>
+        <v>2</v>
       </c>
       <c r="G16" s="10"/>
     </row>
@@ -10352,7 +10380,8 @@
         <v>81</v>
       </c>
       <c r="F17" s="10">
-        <v>1</v>
+        <f>_xlfn.XLOOKUP(Lines[[#This Row],[LineGeometry]],LineGeo[LineGeo],LineGeo[Nphases],0,0)</f>
+        <v>2</v>
       </c>
       <c r="G17" s="10"/>
     </row>
@@ -10373,7 +10402,8 @@
         <v>81</v>
       </c>
       <c r="F18" s="10">
-        <v>1</v>
+        <f>_xlfn.XLOOKUP(Lines[[#This Row],[LineGeometry]],LineGeo[LineGeo],LineGeo[Nphases],0,0)</f>
+        <v>2</v>
       </c>
       <c r="G18" s="10"/>
     </row>
@@ -10394,7 +10424,8 @@
         <v>81</v>
       </c>
       <c r="F19" s="10">
-        <v>1</v>
+        <f>_xlfn.XLOOKUP(Lines[[#This Row],[LineGeometry]],LineGeo[LineGeo],LineGeo[Nphases],0,0)</f>
+        <v>2</v>
       </c>
       <c r="G19" s="10"/>
     </row>
@@ -10415,7 +10446,8 @@
         <v>81</v>
       </c>
       <c r="F20" s="10">
-        <v>1</v>
+        <f>_xlfn.XLOOKUP(Lines[[#This Row],[LineGeometry]],LineGeo[LineGeo],LineGeo[Nphases],0,0)</f>
+        <v>2</v>
       </c>
       <c r="G20" s="10"/>
     </row>
@@ -10436,7 +10468,8 @@
         <v>81</v>
       </c>
       <c r="F21" s="10">
-        <v>1</v>
+        <f>_xlfn.XLOOKUP(Lines[[#This Row],[LineGeometry]],LineGeo[LineGeo],LineGeo[Nphases],0,0)</f>
+        <v>2</v>
       </c>
       <c r="G21" s="10"/>
     </row>
@@ -10457,7 +10490,8 @@
         <v>81</v>
       </c>
       <c r="F22" s="10">
-        <v>1</v>
+        <f>_xlfn.XLOOKUP(Lines[[#This Row],[LineGeometry]],LineGeo[LineGeo],LineGeo[Nphases],0,0)</f>
+        <v>2</v>
       </c>
       <c r="G22" s="10"/>
     </row>
@@ -10824,7 +10858,7 @@
         <v>100</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E39" s="10" t="s">
         <v>81</v>
@@ -10859,7 +10893,7 @@
   <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10878,28 +10912,28 @@
         <v>193</v>
       </c>
       <c r="D1" t="s">
+        <v>224</v>
+      </c>
+      <c r="E1" t="s">
         <v>225</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>226</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>227</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>228</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>229</v>
-      </c>
-      <c r="I1" t="s">
-        <v>230</v>
       </c>
       <c r="J1" t="s">
         <v>195</v>
       </c>
       <c r="K1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="L1" t="s">
         <v>189</v>
@@ -10908,16 +10942,16 @@
         <v>190</v>
       </c>
       <c r="N1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="O1" t="s">
+        <v>218</v>
+      </c>
+      <c r="P1" t="s">
         <v>219</v>
       </c>
-      <c r="P1" t="s">
-        <v>220</v>
-      </c>
       <c r="Q1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -10975,10 +11009,10 @@
         <v>0.1</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Q2" s="13"/>
     </row>
@@ -11037,10 +11071,10 @@
         <v>0.18</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Q3" s="13"/>
     </row>
@@ -11099,10 +11133,10 @@
         <v>0.18</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Q4" s="13"/>
     </row>
@@ -11114,15 +11148,15 @@
         <v>120</v>
       </c>
       <c r="C5" t="s">
-        <v>200</v>
+        <v>234</v>
       </c>
       <c r="D5">
         <f>_xlfn.XLOOKUP(xfmrs[[#This Row],[xfmr]],xfmr_info[name],xfmr_info[kV_hv])</f>
-        <v>7.2</v>
+        <v>12.47</v>
       </c>
       <c r="E5">
         <f>_xlfn.XLOOKUP(xfmrs[[#This Row],[xfmr]],xfmr_info[name],xfmr_info[kV_lv])</f>
-        <v>0.24</v>
+        <v>0.41599999999999998</v>
       </c>
       <c r="F5">
         <f>_xlfn.XLOOKUP(xfmrs[[#This Row],[xfmr]],xfmr_info[name],xfmr_info[kVA_hv])</f>
@@ -11134,11 +11168,11 @@
       </c>
       <c r="H5" t="str">
         <f>_xlfn.XLOOKUP(xfmrs[[#This Row],[xfmr]],xfmr_info[name],xfmr_info[Conn_hv])</f>
-        <v>wye</v>
+        <v>delta</v>
       </c>
       <c r="I5" t="str">
         <f>_xlfn.XLOOKUP(xfmrs[[#This Row],[xfmr]],xfmr_info[name],xfmr_info[Conn_lv])</f>
-        <v>wye</v>
+        <v>delta</v>
       </c>
       <c r="J5">
         <f>_xlfn.XLOOKUP(xfmrs[[#This Row],[xfmr]],xfmr_info[name],xfmr_info[Phases])</f>
@@ -11158,13 +11192,13 @@
       </c>
       <c r="N5">
         <f>_xlfn.XLOOKUP(xfmrs[[#This Row],[xfmr]],xfmr_info[name],xfmr_info[nll])</f>
-        <v>0.2</v>
+        <v>0.18</v>
       </c>
       <c r="O5" s="1">
         <v>1.3</v>
       </c>
       <c r="P5" s="1">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="Q5" s="13"/>
     </row>
@@ -11223,10 +11257,10 @@
         <v>0.18</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Q6" s="13"/>
     </row>
@@ -11347,10 +11381,10 @@
         <v>0.12</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Q8" s="13"/>
     </row>
@@ -11394,7 +11428,7 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H10"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11425,7 +11459,7 @@
         <v>188</v>
       </c>
       <c r="H1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I1" t="s">
         <v>189</v>
@@ -11434,7 +11468,7 @@
         <v>190</v>
       </c>
       <c r="K1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="L1" t="s">
         <v>194</v>
@@ -11679,7 +11713,7 @@
         <v>12.47</v>
       </c>
       <c r="B8">
-        <v>0.24</v>
+        <v>0.41599999999999998</v>
       </c>
       <c r="C8">
         <v>75</v>
@@ -11688,10 +11722,10 @@
         <v>75</v>
       </c>
       <c r="E8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -11710,7 +11744,7 @@
       </c>
       <c r="L8" t="str">
         <f>_xlfn.CONCAT(xfmr_info[[#This Row],[Phases]],"p_",xfmr_info[[#This Row],[kV_hv]],"_",xfmr_info[[#This Row],[kV_lv]],"_",xfmr_info[[#This Row],[kVA_hv]],"_",LEFT(xfmr_info[[#This Row],[Conn_hv]],1),LEFT(xfmr_info[[#This Row],[Conn_lv]],1))</f>
-        <v>1p_12.47_0.24_75_ww</v>
+        <v>1p_12.47_0.416_75_dd</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -11801,15 +11835,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CE5CFF8-7828-B948-AF88-0BAE820E01A6}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>151</v>
       </c>
@@ -11823,16 +11857,19 @@
         <v>160</v>
       </c>
       <c r="E1" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="F1" s="20" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>125</v>
       </c>
       <c r="B2" s="10">
         <f>_xlfn.XLOOKUP(Loads[[#This Row],[Bus]],Lines[bus2],Lines[phases],_xlfn.XLOOKUP(Loads[[#This Row],[Bus]],xfmrs[bus2],xfmrs[phases],0,0),0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="10">
         <v>7</v>
@@ -11841,16 +11878,19 @@
         <v>2</v>
       </c>
       <c r="E2" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1.3</v>
+      </c>
+      <c r="F2" s="10">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>126</v>
       </c>
       <c r="B3" s="10">
         <f>_xlfn.XLOOKUP(Loads[[#This Row],[Bus]],Lines[bus2],Lines[phases],_xlfn.XLOOKUP(Loads[[#This Row],[Bus]],xfmrs[bus2],xfmrs[phases],0,0),0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" s="10">
         <v>6</v>
@@ -11859,16 +11899,17 @@
         <v>2</v>
       </c>
       <c r="E3" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1.3</v>
+      </c>
+      <c r="F3" s="10"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>127</v>
       </c>
       <c r="B4" s="10">
         <f>_xlfn.XLOOKUP(Loads[[#This Row],[Bus]],Lines[bus2],Lines[phases],_xlfn.XLOOKUP(Loads[[#This Row],[Bus]],xfmrs[bus2],xfmrs[phases],0,0),0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" s="10">
         <v>15</v>
@@ -11877,16 +11918,17 @@
         <v>4.5</v>
       </c>
       <c r="E4" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1.3</v>
+      </c>
+      <c r="F4" s="10"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>123</v>
       </c>
       <c r="B5" s="10">
         <f>_xlfn.XLOOKUP(Loads[[#This Row],[Bus]],Lines[bus2],Lines[phases],_xlfn.XLOOKUP(Loads[[#This Row],[Bus]],xfmrs[bus2],xfmrs[phases],0,0),0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" s="10">
         <v>10</v>
@@ -11895,10 +11937,11 @@
         <v>4</v>
       </c>
       <c r="E5" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1.3</v>
+      </c>
+      <c r="F5" s="10"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
         <v>155</v>
       </c>
@@ -11912,17 +11955,18 @@
       <c r="D6" s="10">
         <v>20</v>
       </c>
-      <c r="E6" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E6" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="F6" s="10"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>129</v>
       </c>
       <c r="B7" s="10">
         <f>_xlfn.XLOOKUP(Loads[[#This Row],[Bus]],Lines[bus2],Lines[phases],_xlfn.XLOOKUP(Loads[[#This Row],[Bus]],xfmrs[bus2],xfmrs[phases],0,0),0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" s="10">
         <v>2</v>
@@ -11931,16 +11975,17 @@
         <v>0.5</v>
       </c>
       <c r="E7" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1.3</v>
+      </c>
+      <c r="F7" s="10"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
         <v>130</v>
       </c>
       <c r="B8" s="10">
         <f>_xlfn.XLOOKUP(Loads[[#This Row],[Bus]],Lines[bus2],Lines[phases],_xlfn.XLOOKUP(Loads[[#This Row],[Bus]],xfmrs[bus2],xfmrs[phases],0,0),0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" s="10">
         <v>3</v>
@@ -11949,16 +11994,17 @@
         <v>1</v>
       </c>
       <c r="E8" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1.3</v>
+      </c>
+      <c r="F8" s="10"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>131</v>
       </c>
       <c r="B9" s="10">
         <f>_xlfn.XLOOKUP(Loads[[#This Row],[Bus]],Lines[bus2],Lines[phases],_xlfn.XLOOKUP(Loads[[#This Row],[Bus]],xfmrs[bus2],xfmrs[phases],0,0),0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" s="10">
         <v>10</v>
@@ -11967,10 +12013,11 @@
         <v>4</v>
       </c>
       <c r="E9" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1.3</v>
+      </c>
+      <c r="F9" s="10"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
         <v>112</v>
       </c>
@@ -11985,10 +12032,11 @@
         <v>10</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>208</v>
+      </c>
+      <c r="F10" s="10"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
         <v>114</v>
       </c>
@@ -12003,10 +12051,11 @@
         <v>13</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+        <v>208</v>
+      </c>
+      <c r="F11" s="10"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
         <v>117</v>
       </c>
@@ -12021,10 +12070,11 @@
         <v>20</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+        <v>208</v>
+      </c>
+      <c r="F12" s="10"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
         <v>157</v>
       </c>
@@ -12039,10 +12089,11 @@
         <v>15</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+        <v>208</v>
+      </c>
+      <c r="F13" s="10"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
         <v>132</v>
       </c>
@@ -12059,8 +12110,9 @@
       <c r="E14" s="21">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" s="10"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
         <v>133</v>
       </c>
@@ -12077,8 +12129,9 @@
       <c r="E15" s="21">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15" s="10"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
         <v>158</v>
       </c>
@@ -12093,10 +12146,11 @@
         <v>60</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+        <v>208</v>
+      </c>
+      <c r="F16" s="10"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
         <v>139</v>
       </c>
@@ -12111,10 +12165,11 @@
         <v>23</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+        <v>208</v>
+      </c>
+      <c r="F17" s="10"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
         <v>142</v>
       </c>
@@ -12129,10 +12184,11 @@
         <v>20</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+        <v>208</v>
+      </c>
+      <c r="F18" s="10"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
         <v>143</v>
       </c>
@@ -12147,10 +12203,11 @@
         <v>10</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+        <v>208</v>
+      </c>
+      <c r="F19" s="10"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
         <v>144</v>
       </c>
@@ -12165,10 +12222,11 @@
         <v>12</v>
       </c>
       <c r="E20" s="21" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+        <v>208</v>
+      </c>
+      <c r="F20" s="10"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
         <v>146</v>
       </c>
@@ -12185,8 +12243,9 @@
       <c r="E21" s="21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" s="10"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
         <v>147</v>
       </c>
@@ -12203,8 +12262,9 @@
       <c r="E22" s="21">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22" s="10"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
         <v>148</v>
       </c>
@@ -12221,8 +12281,9 @@
       <c r="E23" s="21">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23" s="10"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
         <v>135</v>
       </c>
@@ -12239,8 +12300,9 @@
       <c r="E24" s="21">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24" s="10"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
         <v>136</v>
       </c>
@@ -12257,8 +12319,9 @@
       <c r="E25" s="21">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25" s="10"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
         <v>137</v>
       </c>
@@ -12275,8 +12338,9 @@
       <c r="E26" s="21">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26" s="10"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
         <v>138</v>
       </c>
@@ -12293,8 +12357,9 @@
       <c r="E27" s="21">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27" s="10"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
         <v>161</v>
       </c>
@@ -12309,8 +12374,9 @@
         <v>70</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>209</v>
-      </c>
+        <v>208</v>
+      </c>
+      <c r="F28" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -12341,28 +12407,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B1" t="s">
         <v>206</v>
       </c>
-      <c r="B1" t="s">
-        <v>207</v>
-      </c>
       <c r="C1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D1" t="s">
         <v>195</v>
       </c>
       <c r="E1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F1" t="s">
         <v>203</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>204</v>
       </c>
-      <c r="G1" t="s">
-        <v>205</v>
-      </c>
       <c r="H1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -12425,16 +12491,16 @@
         <v>175</v>
       </c>
       <c r="H1" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="I1" s="15" t="s">
         <v>215</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="J1" s="14" t="s">
         <v>216</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="K1" s="15" t="s">
         <v>217</v>
-      </c>
-      <c r="K1" s="15" t="s">
-        <v>218</v>
       </c>
       <c r="M1" t="s">
         <v>191</v>
@@ -12443,7 +12509,7 @@
         <v>1</v>
       </c>
       <c r="Q1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -12475,7 +12541,7 @@
         <v>2</v>
       </c>
       <c r="Q2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -12588,32 +12654,32 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="O10" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="O11" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="O12" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="O13" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="O14" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="O15" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
move DistNetwork code to seperate python file
</commit_message>
<xml_diff>
--- a/network-data/LineGeo_Selector.xlsx
+++ b/network-data/LineGeo_Selector.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spenceregan/Repos/CU/Distribution_Systems/Project1/ECEN5437-Proj1/network-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{937F87FB-243E-9042-BA2A-5801D19D25BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3947D35-1B0B-4944-92D6-CC44CC8E893D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{7AEC5E2E-397B-8345-871E-9ED757579969}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{7AEC5E2E-397B-8345-871E-9ED757579969}"/>
   </bookViews>
   <sheets>
     <sheet name="Buses" sheetId="7" r:id="rId1"/>
@@ -751,7 +751,7 @@
     <t>kV</t>
   </si>
   <si>
-    <t>1p_12.47_0.416_75_dd</t>
+    <t>2p_12.47_0.416_75_dd</t>
   </si>
 </sst>
 </file>
@@ -916,7 +916,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="93">
+  <dxfs count="92">
     <dxf>
       <font>
         <b val="0"/>
@@ -2342,24 +2342,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -2578,16 +2560,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{43240ADB-710B-E440-9B4B-064F1493B981}" name="Buses" displayName="Buses" ref="A1:C47" totalsRowShown="0" dataDxfId="92">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{43240ADB-710B-E440-9B4B-064F1493B981}" name="Buses" displayName="Buses" ref="A1:C47" totalsRowShown="0" dataDxfId="91">
   <autoFilter ref="A1:C47" xr:uid="{43240ADB-710B-E440-9B4B-064F1493B981}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{37E9F5EA-051D-BE40-B622-31D4B83CE6AA}" name="Bus" dataDxfId="91"/>
-    <tableColumn id="2" xr3:uid="{41D4B11A-15CC-A540-9052-95C4F3006357}" name="Graph_Loc_x" dataDxfId="90"/>
-    <tableColumn id="3" xr3:uid="{871540F1-C33C-6346-9F71-C67E6A5F5C63}" name="Graph_Loc_y" dataDxfId="89"/>
+    <tableColumn id="1" xr3:uid="{37E9F5EA-051D-BE40-B622-31D4B83CE6AA}" name="Bus" dataDxfId="90"/>
+    <tableColumn id="2" xr3:uid="{41D4B11A-15CC-A540-9052-95C4F3006357}" name="Graph_Loc_x" dataDxfId="89"/>
+    <tableColumn id="3" xr3:uid="{871540F1-C33C-6346-9F71-C67E6A5F5C63}" name="Graph_Loc_y" dataDxfId="88"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2807,7 +2789,7 @@
     <tableColumn id="1" xr3:uid="{2280FF94-C83E-444E-8E42-3510351A4DF6}" name="LineGeo"/>
     <tableColumn id="2" xr3:uid="{3DDFC765-300B-7846-9085-AB03B6A261F4}" name="Type"/>
     <tableColumn id="3" xr3:uid="{02F910B6-BE16-CE4C-89A1-71F43049235B}" name="phase_cond"/>
-    <tableColumn id="4" xr3:uid="{520CD3FE-AB23-3943-8829-73CAAC013F53}" name="neutral_cond" dataDxfId="88">
+    <tableColumn id="4" xr3:uid="{520CD3FE-AB23-3943-8829-73CAAC013F53}" name="neutral_cond" dataDxfId="87">
       <calculatedColumnFormula>IF(LineGeo[[#This Row],[Type]]="OH",1,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="13" xr3:uid="{DE9BDE1B-5E39-604D-9957-E0C3A3473BC8}" name="Nphases"/>
@@ -2852,26 +2834,24 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{12D9EB82-8B48-7449-95A6-3BE76017FBF1}" name="Lines" displayName="Lines" ref="A1:G39" totalsRowShown="0" headerRowDxfId="87" dataDxfId="86">
-  <autoFilter ref="A1:G39" xr:uid="{12D9EB82-8B48-7449-95A6-3BE76017FBF1}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{12D9EB82-8B48-7449-95A6-3BE76017FBF1}" name="Lines" displayName="Lines" ref="A1:F39" totalsRowShown="0" headerRowDxfId="86" dataDxfId="85">
+  <autoFilter ref="A1:F39" xr:uid="{12D9EB82-8B48-7449-95A6-3BE76017FBF1}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
     <filterColumn colId="4" hiddenButton="1"/>
     <filterColumn colId="5" hiddenButton="1"/>
-    <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{B526205E-98EF-F34B-B24D-F8218A008415}" name="bus1" dataDxfId="85"/>
-    <tableColumn id="2" xr3:uid="{D2CD9147-9358-C04D-8316-3FB3A9A16CB0}" name="bus2" dataDxfId="84"/>
-    <tableColumn id="3" xr3:uid="{99BA8C9D-330B-A24F-BC6C-A45D5466D8F3}" name="Length" dataDxfId="83"/>
-    <tableColumn id="4" xr3:uid="{24B6C05D-6629-B248-BB9C-1AF1BAA7ADB7}" name="LineGeometry" dataDxfId="82"/>
-    <tableColumn id="5" xr3:uid="{CDFF2292-878E-CE4B-BF6E-6CE7168C35B8}" name="Units" dataDxfId="81"/>
-    <tableColumn id="6" xr3:uid="{A8C38B34-2B32-C444-89AA-FDCCE25A82B7}" name="phases" dataDxfId="80">
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{B526205E-98EF-F34B-B24D-F8218A008415}" name="bus1" dataDxfId="84"/>
+    <tableColumn id="2" xr3:uid="{D2CD9147-9358-C04D-8316-3FB3A9A16CB0}" name="bus2" dataDxfId="83"/>
+    <tableColumn id="3" xr3:uid="{99BA8C9D-330B-A24F-BC6C-A45D5466D8F3}" name="Length" dataDxfId="82"/>
+    <tableColumn id="4" xr3:uid="{24B6C05D-6629-B248-BB9C-1AF1BAA7ADB7}" name="LineGeometry" dataDxfId="81"/>
+    <tableColumn id="5" xr3:uid="{CDFF2292-878E-CE4B-BF6E-6CE7168C35B8}" name="Units" dataDxfId="80"/>
+    <tableColumn id="6" xr3:uid="{A8C38B34-2B32-C444-89AA-FDCCE25A82B7}" name="phases" dataDxfId="79">
       <calculatedColumnFormula>_xlfn.XLOOKUP(Lines[[#This Row],[LineGeometry]],LineGeo[LineGeo],LineGeo[Nphases],0,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{17578AEA-5626-6A4C-B5EA-E2A9D6CF3223}" name="cond_pos" dataDxfId="79"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -10000,8 +9980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3B959F-BA38-1C45-8F28-8937DDD91101}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10041,13 +10021,13 @@
         <v>110</v>
       </c>
       <c r="C2" s="12">
-        <v>15840</v>
+        <v>3</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F2" s="10">
         <f>_xlfn.XLOOKUP(Lines[[#This Row],[LineGeometry]],LineGeo[LineGeo],LineGeo[Nphases],0,0)</f>
@@ -10063,13 +10043,13 @@
         <v>111</v>
       </c>
       <c r="C3" s="12">
-        <v>15840</v>
+        <v>3</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>0</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F3" s="10">
         <f>_xlfn.XLOOKUP(Lines[[#This Row],[LineGeometry]],LineGeo[LineGeo],LineGeo[Nphases],0,0)</f>
@@ -10085,13 +10065,13 @@
         <v>112</v>
       </c>
       <c r="C4" s="12">
-        <v>15840</v>
+        <v>3</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F4" s="10">
         <f>_xlfn.XLOOKUP(Lines[[#This Row],[LineGeometry]],LineGeo[LineGeo],LineGeo[Nphases],0,0)</f>
@@ -10107,13 +10087,13 @@
         <v>113</v>
       </c>
       <c r="C5" s="12">
-        <v>15840</v>
+        <v>3</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F5" s="10">
         <f>_xlfn.XLOOKUP(Lines[[#This Row],[LineGeometry]],LineGeo[LineGeo],LineGeo[Nphases],0,0)</f>
@@ -10129,13 +10109,13 @@
         <v>114</v>
       </c>
       <c r="C6" s="12">
-        <v>15840</v>
+        <v>3</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F6" s="10">
         <f>_xlfn.XLOOKUP(Lines[[#This Row],[LineGeometry]],LineGeo[LineGeo],LineGeo[Nphases],0,0)</f>
@@ -10151,13 +10131,13 @@
         <v>115</v>
       </c>
       <c r="C7" s="12">
-        <v>15840</v>
+        <v>3</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F7" s="10">
         <f>_xlfn.XLOOKUP(Lines[[#This Row],[LineGeometry]],LineGeo[LineGeo],LineGeo[Nphases],0,0)</f>
@@ -10173,13 +10153,13 @@
         <v>116</v>
       </c>
       <c r="C8" s="12">
-        <v>15840</v>
+        <v>3</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F8" s="10">
         <f>_xlfn.XLOOKUP(Lines[[#This Row],[LineGeometry]],LineGeo[LineGeo],LineGeo[Nphases],0,0)</f>
@@ -10195,13 +10175,13 @@
         <v>117</v>
       </c>
       <c r="C9" s="12">
-        <v>15840</v>
+        <v>3</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F9" s="10">
         <f>_xlfn.XLOOKUP(Lines[[#This Row],[LineGeometry]],LineGeo[LineGeo],LineGeo[Nphases],0,0)</f>
@@ -10217,13 +10197,13 @@
         <v>118</v>
       </c>
       <c r="C10" s="12">
-        <v>15840</v>
+        <v>3</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F10" s="10">
         <f>_xlfn.XLOOKUP(Lines[[#This Row],[LineGeometry]],LineGeo[LineGeo],LineGeo[Nphases],0,0)</f>
@@ -10239,13 +10219,13 @@
         <v>119</v>
       </c>
       <c r="C11" s="12">
-        <v>15840</v>
+        <v>3</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F11" s="10">
         <f>_xlfn.XLOOKUP(Lines[[#This Row],[LineGeometry]],LineGeo[LineGeo],LineGeo[Nphases],0,0)</f>
@@ -10503,13 +10483,13 @@
         <v>132</v>
       </c>
       <c r="C23" s="12">
-        <v>15840</v>
+        <v>3</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>2</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F23" s="10">
         <f>_xlfn.XLOOKUP(Lines[[#This Row],[LineGeometry]],LineGeo[LineGeo],LineGeo[Nphases],0,0)</f>
@@ -10525,13 +10505,13 @@
         <v>133</v>
       </c>
       <c r="C24" s="12">
-        <v>15840</v>
+        <v>3</v>
       </c>
       <c r="D24" s="10" t="s">
         <v>2</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F24" s="10">
         <f>_xlfn.XLOOKUP(Lines[[#This Row],[LineGeometry]],LineGeo[LineGeo],LineGeo[Nphases],0,0)</f>
@@ -10635,13 +10615,13 @@
         <v>139</v>
       </c>
       <c r="C29" s="12">
-        <v>15840</v>
+        <v>3</v>
       </c>
       <c r="D29" s="10" t="s">
         <v>3</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F29" s="10">
         <f>_xlfn.XLOOKUP(Lines[[#This Row],[LineGeometry]],LineGeo[LineGeo],LineGeo[Nphases],0,0)</f>
@@ -10657,13 +10637,13 @@
         <v>140</v>
       </c>
       <c r="C30" s="12">
-        <v>15840</v>
+        <v>3</v>
       </c>
       <c r="D30" s="10" t="s">
         <v>3</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F30" s="10">
         <f>_xlfn.XLOOKUP(Lines[[#This Row],[LineGeometry]],LineGeo[LineGeo],LineGeo[Nphases],0,0)</f>
@@ -10679,13 +10659,13 @@
         <v>141</v>
       </c>
       <c r="C31" s="12">
-        <v>15840</v>
+        <v>3</v>
       </c>
       <c r="D31" s="10" t="s">
         <v>3</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F31" s="10">
         <f>_xlfn.XLOOKUP(Lines[[#This Row],[LineGeometry]],LineGeo[LineGeo],LineGeo[Nphases],0,0)</f>
@@ -10701,13 +10681,13 @@
         <v>142</v>
       </c>
       <c r="C32" s="12">
-        <v>15840</v>
+        <v>3</v>
       </c>
       <c r="D32" s="10" t="s">
         <v>3</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F32" s="10">
         <f>_xlfn.XLOOKUP(Lines[[#This Row],[LineGeometry]],LineGeo[LineGeo],LineGeo[Nphases],0,0)</f>
@@ -10723,13 +10703,13 @@
         <v>143</v>
       </c>
       <c r="C33" s="12">
-        <v>15840</v>
+        <v>3</v>
       </c>
       <c r="D33" s="10" t="s">
         <v>3</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F33" s="10">
         <f>_xlfn.XLOOKUP(Lines[[#This Row],[LineGeometry]],LineGeo[LineGeo],LineGeo[Nphases],0,0)</f>
@@ -10745,13 +10725,13 @@
         <v>144</v>
       </c>
       <c r="C34" s="12">
-        <v>15840</v>
+        <v>3</v>
       </c>
       <c r="D34" s="10" t="s">
         <v>3</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F34" s="10">
         <f>_xlfn.XLOOKUP(Lines[[#This Row],[LineGeometry]],LineGeo[LineGeo],LineGeo[Nphases],0,0)</f>
@@ -10767,13 +10747,13 @@
         <v>145</v>
       </c>
       <c r="C35" s="12">
-        <v>15840</v>
+        <v>3</v>
       </c>
       <c r="D35" s="10" t="s">
         <v>4</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F35" s="10">
         <f>_xlfn.XLOOKUP(Lines[[#This Row],[LineGeometry]],LineGeo[LineGeo],LineGeo[Nphases],0,0)</f>
@@ -10789,13 +10769,13 @@
         <v>146</v>
       </c>
       <c r="C36" s="12">
-        <v>15840</v>
+        <v>3</v>
       </c>
       <c r="D36" s="10" t="s">
         <v>4</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F36" s="10">
         <f>_xlfn.XLOOKUP(Lines[[#This Row],[LineGeometry]],LineGeo[LineGeo],LineGeo[Nphases],0,0)</f>
@@ -10811,13 +10791,13 @@
         <v>147</v>
       </c>
       <c r="C37" s="12">
-        <v>15840</v>
+        <v>3</v>
       </c>
       <c r="D37" s="10" t="s">
         <v>4</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F37" s="10">
         <f>_xlfn.XLOOKUP(Lines[[#This Row],[LineGeometry]],LineGeo[LineGeo],LineGeo[Nphases],0,0)</f>
@@ -10833,13 +10813,13 @@
         <v>148</v>
       </c>
       <c r="C38" s="12">
-        <v>15840</v>
+        <v>3</v>
       </c>
       <c r="D38" s="10" t="s">
         <v>4</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F38" s="10">
         <f>_xlfn.XLOOKUP(Lines[[#This Row],[LineGeometry]],LineGeo[LineGeo],LineGeo[Nphases],0,0)</f>
@@ -10892,7 +10872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DEFE584-74FB-4243-A125-89ADE808B1CA}">
   <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -11176,7 +11156,7 @@
       </c>
       <c r="J5">
         <f>_xlfn.XLOOKUP(xfmrs[[#This Row],[xfmr]],xfmr_info[name],xfmr_info[Phases])</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K5">
         <f>_xlfn.XLOOKUP(xfmrs[[#This Row],[xfmr]],xfmr_info[name],xfmr_info[Windings])</f>
@@ -11428,7 +11408,7 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11728,7 +11708,7 @@
         <v>191</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H8">
         <v>2</v>
@@ -11744,7 +11724,7 @@
       </c>
       <c r="L8" t="str">
         <f>_xlfn.CONCAT(xfmr_info[[#This Row],[Phases]],"p_",xfmr_info[[#This Row],[kV_hv]],"_",xfmr_info[[#This Row],[kV_lv]],"_",xfmr_info[[#This Row],[kVA_hv]],"_",LEFT(xfmr_info[[#This Row],[Conn_hv]],1),LEFT(xfmr_info[[#This Row],[Conn_lv]],1))</f>
-        <v>1p_12.47_0.416_75_dd</v>
+        <v>2p_12.47_0.416_75_dd</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add regulators to networkx and dss
</commit_message>
<xml_diff>
--- a/network-data/LineGeo_Selector.xlsx
+++ b/network-data/LineGeo_Selector.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spenceregan/Repos/CU/Distribution_Systems/Project1/ECEN5437-Proj1/network-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A91F39-0EAE-2B44-ABF6-0DED2F149909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440C85FC-2558-AB49-A8E3-4F7AFF304B62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="7" xr2:uid="{7AEC5E2E-397B-8345-871E-9ED757579969}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{7AEC5E2E-397B-8345-871E-9ED757579969}"/>
   </bookViews>
   <sheets>
     <sheet name="Buses" sheetId="7" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="242">
   <si>
     <t>OH3p</t>
   </si>
@@ -653,6 +653,9 @@
     <t>OH3pD</t>
   </si>
   <si>
+    <t>bus</t>
+  </si>
+  <si>
     <t>pu</t>
   </si>
   <si>
@@ -756,6 +759,21 @@
   </si>
   <si>
     <t>kVA</t>
+  </si>
+  <si>
+    <t>vreg</t>
+  </si>
+  <si>
+    <t>band</t>
+  </si>
+  <si>
+    <t>vbase</t>
+  </si>
+  <si>
+    <t>CTprim</t>
+  </si>
+  <si>
+    <t>Ctsec</t>
   </si>
 </sst>
 </file>
@@ -2580,6 +2598,15 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{197E6DD9-1E95-E144-A54E-7BD8668CA6E8}" name="Units" displayName="Units" ref="C1:C7" headerRowCount="0" totalsRowShown="0">
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{D4C1F671-A0A2-9147-89DB-D689DF977101}" name="Column1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{62FB5798-3249-9746-9DD5-608AFE9823D7}" name="Phases" displayName="Phases" ref="E1:E7" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{A5FD9FF9-B621-734F-9BCC-F153897F2CAB}" name="Column1"/>
@@ -2588,7 +2615,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{0D394314-B822-6C40-97B4-4F5CADFC1074}" name="xfmr_config" displayName="xfmr_config" ref="M1:M2" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{C224F9D5-0D1E-D648-9018-6D26270395C2}" name="Column1"/>
@@ -2597,7 +2624,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{5F3073CA-6F2C-7643-A086-B783E9581317}" name="delta.delta" displayName="delta.delta" ref="H2:H7" headerRowCount="0" totalsRowShown="0" headerRowDxfId="21" dataDxfId="22" tableBorderDxfId="24">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{50958CF2-21D9-984F-97B5-085C4560A350}" name="Column1" headerRowDxfId="20" dataDxfId="23"/>
@@ -2606,7 +2633,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{89D1A629-368D-0B4B-8525-B86A48878238}" name="delta.wye" displayName="delta.wye" ref="I2:I5" headerRowCount="0" totalsRowShown="0" headerRowDxfId="18" tableBorderDxfId="19">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{A3625009-C857-274F-A122-CFD46E3541C5}" name="Column1" headerRowDxfId="17"/>
@@ -2615,7 +2642,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{D6E2BF91-ACF1-C849-9AC2-F7ED9921C73E}" name="wye.delta" displayName="wye.delta" ref="J2:J5" headerRowCount="0" totalsRowShown="0" headerRowDxfId="15" tableBorderDxfId="16">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{147B4193-B138-D749-BACA-A6E839012CE7}" name="Column1" headerRowDxfId="14"/>
@@ -2624,7 +2651,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{32FF552F-94F8-5F4A-A3CD-0CF8C4344854}" name="wye.wye" displayName="wye.wye" ref="K2:K3" headerRowCount="0" totalsRowShown="0" headerRowDxfId="12" tableBorderDxfId="13">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{9713DCA2-8057-6941-AB28-861C6CAD34E9}" name="Column1" headerRowDxfId="11"/>
@@ -2633,7 +2660,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{F85F963E-7E0D-DA40-BC57-8F71010CE834}" name="Terminals" displayName="Terminals" ref="O1:O15" headerRowCount="0" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{B57E695F-4DAF-C041-9D98-90DA0E9FCF30}" name="Column1" dataDxfId="10"/>
@@ -2642,7 +2669,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{7C66977E-132E-CD40-9247-9F596B6AB81A}" name="MeterElement" displayName="MeterElement" ref="Q1:Q2" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{555D147D-0928-4C49-89D1-583C518DA5CB}" name="Column1"/>
@@ -2651,7 +2678,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E4FB8847-4274-D04D-A64C-15B4CD5C8D60}" name="OH" displayName="OH" ref="A1:K100" totalsRowShown="0">
   <autoFilter ref="A1:K100" xr:uid="{E4FB8847-4274-D04D-A64C-15B4CD5C8D60}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -2691,7 +2718,51 @@
 </table>
 </file>
 
-<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0AF27DE9-2ECA-6A4E-84A5-C298787FAAED}" name="LineGeo" displayName="LineGeo" ref="A1:P7" totalsRowShown="0">
+  <autoFilter ref="A1:P7" xr:uid="{0AF27DE9-2ECA-6A4E-84A5-C298787FAAED}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+    <filterColumn colId="7" hiddenButton="1"/>
+    <filterColumn colId="8" hiddenButton="1"/>
+    <filterColumn colId="9" hiddenButton="1"/>
+    <filterColumn colId="10" hiddenButton="1"/>
+    <filterColumn colId="11" hiddenButton="1"/>
+    <filterColumn colId="12" hiddenButton="1"/>
+    <filterColumn colId="13" hiddenButton="1"/>
+    <filterColumn colId="14" hiddenButton="1"/>
+    <filterColumn colId="15" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="16">
+    <tableColumn id="1" xr3:uid="{2280FF94-C83E-444E-8E42-3510351A4DF6}" name="LineGeo"/>
+    <tableColumn id="2" xr3:uid="{3DDFC765-300B-7846-9085-AB03B6A261F4}" name="Type"/>
+    <tableColumn id="3" xr3:uid="{02F910B6-BE16-CE4C-89A1-71F43049235B}" name="phase_cond"/>
+    <tableColumn id="4" xr3:uid="{520CD3FE-AB23-3943-8829-73CAAC013F53}" name="neutral_cond" dataDxfId="87">
+      <calculatedColumnFormula>IF(LineGeo[[#This Row],[Type]]="OH",1,0)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="13" xr3:uid="{DE9BDE1B-5E39-604D-9957-E0C3A3473BC8}" name="Nphases"/>
+    <tableColumn id="14" xr3:uid="{A59E67A1-D1C4-254C-9BE2-796679103A71}" name="Nconds"/>
+    <tableColumn id="5" xr3:uid="{7F74CB42-995F-3446-92C4-BDF24C8452BF}" name="1_x"/>
+    <tableColumn id="6" xr3:uid="{B455EBCF-14BE-7647-8388-140F641BA11E}" name="1_z"/>
+    <tableColumn id="7" xr3:uid="{6506C10F-9F62-5C4E-BFD2-1AB87F349ECA}" name="2_x"/>
+    <tableColumn id="8" xr3:uid="{0D2A84D3-3D0E-A24F-90E2-AA0E6A3F2051}" name="2_z"/>
+    <tableColumn id="9" xr3:uid="{022976D1-9937-8D45-8FBA-CB02DE3BB052}" name="3_x"/>
+    <tableColumn id="10" xr3:uid="{C4EA44B5-38D8-2B40-8B11-98D0B4BF5265}" name="3_z"/>
+    <tableColumn id="11" xr3:uid="{F2274653-629E-134E-BBF5-C325DBF3EA16}" name="4_x"/>
+    <tableColumn id="12" xr3:uid="{BD8B48A0-76F9-974B-9D8A-D27303D1602B}" name="4_z"/>
+    <tableColumn id="15" xr3:uid="{25261513-8FAF-4F4C-AB29-7DAD255766AB}" name="Units"/>
+    <tableColumn id="16" xr3:uid="{5C4EE22D-BF12-B440-B404-EE8CFF19B8DA}" name="cond_pos"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{661274D6-1D68-5542-8D94-45D5C86243F5}" name="CN" displayName="CN" ref="A1:V19" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57" tableBorderDxfId="56">
   <autoFilter ref="A1:V19" xr:uid="{661274D6-1D68-5542-8D94-45D5C86243F5}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -2769,51 +2840,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0AF27DE9-2ECA-6A4E-84A5-C298787FAAED}" name="LineGeo" displayName="LineGeo" ref="A1:P7" totalsRowShown="0">
-  <autoFilter ref="A1:P7" xr:uid="{0AF27DE9-2ECA-6A4E-84A5-C298787FAAED}">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-    <filterColumn colId="6" hiddenButton="1"/>
-    <filterColumn colId="7" hiddenButton="1"/>
-    <filterColumn colId="8" hiddenButton="1"/>
-    <filterColumn colId="9" hiddenButton="1"/>
-    <filterColumn colId="10" hiddenButton="1"/>
-    <filterColumn colId="11" hiddenButton="1"/>
-    <filterColumn colId="12" hiddenButton="1"/>
-    <filterColumn colId="13" hiddenButton="1"/>
-    <filterColumn colId="14" hiddenButton="1"/>
-    <filterColumn colId="15" hiddenButton="1"/>
-  </autoFilter>
-  <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{2280FF94-C83E-444E-8E42-3510351A4DF6}" name="LineGeo"/>
-    <tableColumn id="2" xr3:uid="{3DDFC765-300B-7846-9085-AB03B6A261F4}" name="Type"/>
-    <tableColumn id="3" xr3:uid="{02F910B6-BE16-CE4C-89A1-71F43049235B}" name="phase_cond"/>
-    <tableColumn id="4" xr3:uid="{520CD3FE-AB23-3943-8829-73CAAC013F53}" name="neutral_cond" dataDxfId="87">
-      <calculatedColumnFormula>IF(LineGeo[[#This Row],[Type]]="OH",1,0)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="13" xr3:uid="{DE9BDE1B-5E39-604D-9957-E0C3A3473BC8}" name="Nphases"/>
-    <tableColumn id="14" xr3:uid="{A59E67A1-D1C4-254C-9BE2-796679103A71}" name="Nconds"/>
-    <tableColumn id="5" xr3:uid="{7F74CB42-995F-3446-92C4-BDF24C8452BF}" name="1_x"/>
-    <tableColumn id="6" xr3:uid="{B455EBCF-14BE-7647-8388-140F641BA11E}" name="1_z"/>
-    <tableColumn id="7" xr3:uid="{6506C10F-9F62-5C4E-BFD2-1AB87F349ECA}" name="2_x"/>
-    <tableColumn id="8" xr3:uid="{0D2A84D3-3D0E-A24F-90E2-AA0E6A3F2051}" name="2_z"/>
-    <tableColumn id="9" xr3:uid="{022976D1-9937-8D45-8FBA-CB02DE3BB052}" name="3_x"/>
-    <tableColumn id="10" xr3:uid="{C4EA44B5-38D8-2B40-8B11-98D0B4BF5265}" name="3_z"/>
-    <tableColumn id="11" xr3:uid="{F2274653-629E-134E-BBF5-C325DBF3EA16}" name="4_x"/>
-    <tableColumn id="12" xr3:uid="{BD8B48A0-76F9-974B-9D8A-D27303D1602B}" name="4_z"/>
-    <tableColumn id="15" xr3:uid="{25261513-8FAF-4F4C-AB29-7DAD255766AB}" name="Units"/>
-    <tableColumn id="16" xr3:uid="{5C4EE22D-BF12-B440-B404-EE8CFF19B8DA}" name="cond_pos"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{13D01E9F-2651-EF45-A492-F190721E7BE9}" name="TS" displayName="TS" ref="A1:G10" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
   <autoFilter ref="A1:G10" xr:uid="{13D01E9F-2651-EF45-A492-F190721E7BE9}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -2862,6 +2889,32 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{D81C8915-A75B-ED43-95A0-D72233099B0F}" name="Regulators" displayName="Regulators" ref="A1:H4" totalsRowShown="0">
+  <autoFilter ref="A1:H4" xr:uid="{D81C8915-A75B-ED43-95A0-D72233099B0F}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+    <filterColumn colId="7" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{DD9993CA-F636-F542-8A5B-6DAC073E79A9}" name="bus"/>
+    <tableColumn id="3" xr3:uid="{84FEDC1F-56C2-BB45-865C-C02F4D8EC141}" name="kVA"/>
+    <tableColumn id="4" xr3:uid="{404E61D9-A76D-0C45-96A5-4A4A712B4B26}" name="phases"/>
+    <tableColumn id="5" xr3:uid="{179BA37A-338D-1347-BF3A-C124700B7B2D}" name="vbase"/>
+    <tableColumn id="6" xr3:uid="{D042B939-F5F9-214A-A065-F2166F8106E2}" name="vreg"/>
+    <tableColumn id="7" xr3:uid="{2E6849E2-BBE5-CD4D-B609-0AE8DC587667}" name="band"/>
+    <tableColumn id="8" xr3:uid="{D48784CE-6023-4848-AD45-7879BBE634CD}" name="CTprim"/>
+    <tableColumn id="9" xr3:uid="{749082FB-86EF-7F42-8281-B562EE77C531}" name="Ctsec"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{A014B023-656C-A64C-AD6B-78609FE9A464}" name="xfmrs" displayName="xfmrs" ref="A1:Q8" totalsRowShown="0">
   <autoFilter ref="A1:Q8" xr:uid="{A014B023-656C-A64C-AD6B-78609FE9A464}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -2927,7 +2980,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{BCDAB83C-3EF0-7E4F-917A-E03773467446}" name="xfmr_info" displayName="xfmr_info" ref="A1:L10" totalsRowShown="0">
   <autoFilter ref="A1:L10" xr:uid="{BCDAB83C-3EF0-7E4F-917A-E03773467446}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -2963,7 +3016,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{CDAC5F4F-CC5E-714A-A10A-32F2E90176D7}" name="Loads" displayName="Loads" ref="A1:F28" totalsRowShown="0" headerRowDxfId="68" dataDxfId="67">
   <autoFilter ref="A1:F28" xr:uid="{CDAC5F4F-CC5E-714A-A10A-32F2E90176D7}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -2987,7 +3040,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{7EF548C0-A884-944F-92C0-816F3D37F3C4}" name="Slack" displayName="Slack" ref="A1:H2" totalsRowShown="0">
   <autoFilter ref="A1:H2" xr:uid="{7EF548C0-A884-944F-92C0-816F3D37F3C4}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -3013,19 +3066,10 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{045739EA-1F28-0E41-AB74-C2C34C8286AB}" name="Type" displayName="Type" ref="A1:A3" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{CF2DB599-7394-FB45-9EE6-02953B6FA5D3}" name="Column1"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{197E6DD9-1E95-E144-A54E-7BD8668CA6E8}" name="Units" displayName="Units" ref="C1:C7" headerRowCount="0" totalsRowShown="0">
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{D4C1F671-A0A2-9147-89DB-D689DF977101}" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3330,7 +3374,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC2FAF4C-A38A-5148-8683-163D7FE8FD2D}">
   <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -3885,16 +3929,16 @@
         <v>175</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K1" s="15" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="M1" t="s">
         <v>191</v>
@@ -3903,7 +3947,7 @@
         <v>1</v>
       </c>
       <c r="Q1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -3935,7 +3979,7 @@
         <v>2</v>
       </c>
       <c r="Q2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -4048,32 +4092,32 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="O10" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="O11" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="O12" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="O13" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="O14" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="O15" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -10214,7 +10258,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11103,30 +11147,128 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2955D94-A9C5-924E-AFCA-D6295E4B752D}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>163</v>
+        <v>201</v>
       </c>
       <c r="B1" t="s">
-        <v>164</v>
+        <v>236</v>
       </c>
       <c r="C1" t="s">
-        <v>235</v>
+        <v>195</v>
       </c>
       <c r="D1" t="s">
-        <v>195</v>
+        <v>239</v>
+      </c>
+      <c r="E1" t="s">
+        <v>237</v>
+      </c>
+      <c r="F1" t="s">
+        <v>238</v>
+      </c>
+      <c r="G1" t="s">
+        <v>240</v>
+      </c>
+      <c r="H1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2">
+        <v>5000</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>120</v>
+      </c>
+      <c r="E2">
+        <v>126</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>600</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3">
+        <v>5000</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>120</v>
+      </c>
+      <c r="E3">
+        <v>124</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>600</v>
+      </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4">
+        <v>5000</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>120</v>
+      </c>
+      <c r="E4">
+        <v>124</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>600</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A4" xr:uid="{B78B59D8-45A0-C54C-8EC5-DA8054832273}">
+      <formula1>INDIRECT("Buses[Bus]")</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -11154,28 +11296,28 @@
         <v>193</v>
       </c>
       <c r="D1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="G1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="I1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J1" t="s">
         <v>195</v>
       </c>
       <c r="K1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="L1" t="s">
         <v>189</v>
@@ -11184,16 +11326,16 @@
         <v>190</v>
       </c>
       <c r="N1" t="s">
+        <v>221</v>
+      </c>
+      <c r="O1" t="s">
+        <v>219</v>
+      </c>
+      <c r="P1" t="s">
         <v>220</v>
       </c>
-      <c r="O1" t="s">
-        <v>218</v>
-      </c>
-      <c r="P1" t="s">
-        <v>219</v>
-      </c>
       <c r="Q1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -11251,10 +11393,10 @@
         <v>0.1</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="Q2" s="13"/>
     </row>
@@ -11313,10 +11455,10 @@
         <v>0.18</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="Q3" s="13"/>
     </row>
@@ -11375,10 +11517,10 @@
         <v>0.18</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="Q4" s="13"/>
     </row>
@@ -11390,7 +11532,7 @@
         <v>120</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D5">
         <f>_xlfn.XLOOKUP(xfmrs[[#This Row],[xfmr]],xfmr_info[name],xfmr_info[kV_hv])</f>
@@ -11499,10 +11641,10 @@
         <v>0.18</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="Q6" s="13"/>
     </row>
@@ -11623,10 +11765,10 @@
         <v>0.12</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="Q8" s="13"/>
     </row>
@@ -11701,7 +11843,7 @@
         <v>188</v>
       </c>
       <c r="H1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="I1" t="s">
         <v>189</v>
@@ -11710,7 +11852,7 @@
         <v>190</v>
       </c>
       <c r="K1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="L1" t="s">
         <v>194</v>
@@ -12079,8 +12221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CE5CFF8-7828-B948-AF88-0BAE820E01A6}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12099,10 +12241,10 @@
         <v>160</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -12204,7 +12346,7 @@
         <v>20</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F6" s="10">
         <v>0.41599999999999998</v>
@@ -12288,7 +12430,7 @@
         <v>10</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F10" s="10">
         <v>12.47</v>
@@ -12309,7 +12451,7 @@
         <v>13</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F11" s="10">
         <v>12.47</v>
@@ -12330,7 +12472,7 @@
         <v>20</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F12" s="10">
         <v>12.47</v>
@@ -12351,7 +12493,7 @@
         <v>15</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F13" s="10">
         <v>0.41599999999999998</v>
@@ -12414,7 +12556,7 @@
         <v>60</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F16" s="10">
         <v>0.41599999999999998</v>
@@ -12435,7 +12577,7 @@
         <v>23</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F17" s="10">
         <v>12.47</v>
@@ -12456,7 +12598,7 @@
         <v>20</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F18" s="10">
         <v>12.47</v>
@@ -12477,7 +12619,7 @@
         <v>10</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F19" s="10">
         <v>12.47</v>
@@ -12498,7 +12640,7 @@
         <v>12</v>
       </c>
       <c r="E20" s="21" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F20" s="10">
         <v>12.47</v>
@@ -12666,7 +12808,7 @@
         <v>70</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F28" s="10">
         <v>0.41599999999999998</v>
@@ -12701,28 +12843,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D1" t="s">
         <v>195</v>
       </c>
       <c r="E1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="F1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="G1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="H1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add voltage ts functions
</commit_message>
<xml_diff>
--- a/network-data/LineGeo_Selector.xlsx
+++ b/network-data/LineGeo_Selector.xlsx
@@ -8,24 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spenceregan/Repos/CU/Distribution_Systems/Project1/ECEN5437-Proj1/network-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA60558-0365-F343-B00E-AE8D88FB8548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA34C33-0F42-7D40-B5B5-95BB0E18A478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33400" yWindow="-480" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{7AEC5E2E-397B-8345-871E-9ED757579969}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{7AEC5E2E-397B-8345-871E-9ED757579969}"/>
   </bookViews>
   <sheets>
     <sheet name="Buses" sheetId="7" r:id="rId1"/>
     <sheet name="LineGeometry" sheetId="1" r:id="rId2"/>
     <sheet name="Lines" sheetId="6" r:id="rId3"/>
     <sheet name="Regulators" sheetId="13" r:id="rId4"/>
-    <sheet name="Transformers" sheetId="10" r:id="rId5"/>
-    <sheet name="Meters" sheetId="12" r:id="rId6"/>
-    <sheet name="Transformer Info" sheetId="9" r:id="rId7"/>
-    <sheet name="Loads" sheetId="8" r:id="rId8"/>
-    <sheet name="circuit" sheetId="11" r:id="rId9"/>
-    <sheet name="Ref" sheetId="5" r:id="rId10"/>
-    <sheet name="WireData" sheetId="2" r:id="rId11"/>
-    <sheet name="CNData" sheetId="3" r:id="rId12"/>
-    <sheet name="TSData" sheetId="4" r:id="rId13"/>
+    <sheet name="PV" sheetId="14" r:id="rId5"/>
+    <sheet name="Transformers" sheetId="10" r:id="rId6"/>
+    <sheet name="Meters" sheetId="12" r:id="rId7"/>
+    <sheet name="Transformer Info" sheetId="9" r:id="rId8"/>
+    <sheet name="Loads" sheetId="8" r:id="rId9"/>
+    <sheet name="circuit" sheetId="11" r:id="rId10"/>
+    <sheet name="Ref" sheetId="5" r:id="rId11"/>
+    <sheet name="WireData" sheetId="2" r:id="rId12"/>
+    <sheet name="CNData" sheetId="3" r:id="rId13"/>
+    <sheet name="TSData" sheetId="4" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="254">
   <si>
     <t>OH3p</t>
   </si>
@@ -795,6 +796,21 @@
   </si>
   <si>
     <t>conn</t>
+  </si>
+  <si>
+    <t>Pmpp</t>
+  </si>
+  <si>
+    <t>inv_curve</t>
+  </si>
+  <si>
+    <t>kvar_lim</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -2625,6 +2641,15 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{045739EA-1F28-0E41-AB74-C2C34C8286AB}" name="Type" displayName="Type" ref="A1:A3" headerRowCount="0" totalsRowShown="0">
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{CF2DB599-7394-FB45-9EE6-02953B6FA5D3}" name="Column1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{197E6DD9-1E95-E144-A54E-7BD8668CA6E8}" name="Units" displayName="Units" ref="C1:C7" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{D4C1F671-A0A2-9147-89DB-D689DF977101}" name="Column1"/>
@@ -2633,7 +2658,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{62FB5798-3249-9746-9DD5-608AFE9823D7}" name="Phases" displayName="Phases" ref="E1:E7" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{A5FD9FF9-B621-734F-9BCC-F153897F2CAB}" name="Column1"/>
@@ -2642,7 +2667,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{0D394314-B822-6C40-97B4-4F5CADFC1074}" name="xfmr_config" displayName="xfmr_config" ref="M1:M2" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{C224F9D5-0D1E-D648-9018-6D26270395C2}" name="Column1"/>
@@ -2651,7 +2676,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{5F3073CA-6F2C-7643-A086-B783E9581317}" name="delta.delta" displayName="delta.delta" ref="H2:H7" headerRowCount="0" totalsRowShown="0" headerRowDxfId="23" dataDxfId="24" tableBorderDxfId="26">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{50958CF2-21D9-984F-97B5-085C4560A350}" name="Column1" headerRowDxfId="22" dataDxfId="25"/>
@@ -2660,7 +2685,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{89D1A629-368D-0B4B-8525-B86A48878238}" name="delta.wye" displayName="delta.wye" ref="I2:I5" headerRowCount="0" totalsRowShown="0" headerRowDxfId="20" tableBorderDxfId="21">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{A3625009-C857-274F-A122-CFD46E3541C5}" name="Column1" headerRowDxfId="19"/>
@@ -2669,7 +2694,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{D6E2BF91-ACF1-C849-9AC2-F7ED9921C73E}" name="wye.delta" displayName="wye.delta" ref="J2:J5" headerRowCount="0" totalsRowShown="0" headerRowDxfId="17" tableBorderDxfId="18">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{147B4193-B138-D749-BACA-A6E839012CE7}" name="Column1" headerRowDxfId="16"/>
@@ -2678,7 +2703,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{32FF552F-94F8-5F4A-A3CD-0CF8C4344854}" name="wye.wye" displayName="wye.wye" ref="K2:K3" headerRowCount="0" totalsRowShown="0" headerRowDxfId="14" tableBorderDxfId="15">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{9713DCA2-8057-6941-AB28-861C6CAD34E9}" name="Column1" headerRowDxfId="13"/>
@@ -2687,7 +2712,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{F85F963E-7E0D-DA40-BC57-8F71010CE834}" name="Terminals" displayName="Terminals" ref="O1:O15" headerRowCount="0" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{B57E695F-4DAF-C041-9D98-90DA0E9FCF30}" name="Column1" dataDxfId="12"/>
@@ -2696,19 +2721,10 @@
 </table>
 </file>
 
-<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{7C66977E-132E-CD40-9247-9F596B6AB81A}" name="MeterElement" displayName="MeterElement" ref="Q1:Q2" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{555D147D-0928-4C49-89D1-583C518DA5CB}" name="Column1"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{59012749-ADB5-0341-AF22-07D1487AEE43}" name="bool" displayName="bool" ref="S1:S2" headerRowCount="0" totalsRowShown="0">
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{24BA7888-D19F-8140-9509-C843591C8D6F}" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2759,6 +2775,15 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{59012749-ADB5-0341-AF22-07D1487AEE43}" name="bool" displayName="bool" ref="S1:S2" headerRowCount="0" totalsRowShown="0">
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{24BA7888-D19F-8140-9509-C843591C8D6F}" name="Column1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{08B74F89-8C69-4646-999E-90CA377EC508}" name="RegType" displayName="RegType" ref="U1:U2" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{93757295-DECB-A342-BB2A-A812C879A53F}" name="Column1"/>
@@ -2767,7 +2792,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E4FB8847-4274-D04D-A64C-15B4CD5C8D60}" name="OH" displayName="OH" ref="A1:K100" totalsRowShown="0">
   <autoFilter ref="A1:K100" xr:uid="{E4FB8847-4274-D04D-A64C-15B4CD5C8D60}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -2807,7 +2832,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{661274D6-1D68-5542-8D94-45D5C86243F5}" name="CN" displayName="CN" ref="A1:V19" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59" tableBorderDxfId="58">
   <autoFilter ref="A1:V19" xr:uid="{661274D6-1D68-5542-8D94-45D5C86243F5}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -2885,7 +2910,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{13D01E9F-2651-EF45-A492-F190721E7BE9}" name="TS" displayName="TS" ref="A1:G10" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
   <autoFilter ref="A1:G10" xr:uid="{13D01E9F-2651-EF45-A492-F190721E7BE9}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -2974,6 +2999,26 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{E8E696DC-003E-2448-9B7F-4C97C724B059}" name="Table26" displayName="Table26" ref="A1:E7" totalsRowShown="0">
+  <autoFilter ref="A1:E7" xr:uid="{E8E696DC-003E-2448-9B7F-4C97C724B059}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{BA31837E-5B81-DF47-9042-8460B1AEEF42}" name="bus"/>
+    <tableColumn id="2" xr3:uid="{5363DCF8-99A3-ED49-9E87-3881745C2B1D}" name="kVA"/>
+    <tableColumn id="3" xr3:uid="{2FBFA86A-A1A4-774E-B4F4-8A3D4033D33F}" name="Pmpp"/>
+    <tableColumn id="4" xr3:uid="{1DF94CE5-644E-E543-A808-67DB3F9569AA}" name="inv_curve"/>
+    <tableColumn id="5" xr3:uid="{9BD28774-6D1B-614F-945C-703372656F1C}" name="kvar_lim"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{A014B023-656C-A64C-AD6B-78609FE9A464}" name="xfmrs" displayName="xfmrs" ref="A1:Q8" totalsRowShown="0">
   <autoFilter ref="A1:Q8" xr:uid="{A014B023-656C-A64C-AD6B-78609FE9A464}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -3039,7 +3084,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{BCDAB83C-3EF0-7E4F-917A-E03773467446}" name="xfmr_info" displayName="xfmr_info" ref="A1:L10" totalsRowShown="0">
   <autoFilter ref="A1:L10" xr:uid="{BCDAB83C-3EF0-7E4F-917A-E03773467446}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -3075,7 +3120,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{CDAC5F4F-CC5E-714A-A10A-32F2E90176D7}" name="Loads" displayName="Loads" ref="A1:F28" totalsRowShown="0" headerRowDxfId="70" dataDxfId="69">
   <autoFilter ref="A1:F28" xr:uid="{CDAC5F4F-CC5E-714A-A10A-32F2E90176D7}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -3099,7 +3144,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{7EF548C0-A884-944F-92C0-816F3D37F3C4}" name="Slack" displayName="Slack" ref="A1:H2" totalsRowShown="0">
   <autoFilter ref="A1:H2" xr:uid="{7EF548C0-A884-944F-92C0-816F3D37F3C4}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -3120,15 +3165,6 @@
     <tableColumn id="6" xr3:uid="{DD6A5CE7-18B2-FD4B-AE96-18F3300481E8}" name="X_1"/>
     <tableColumn id="7" xr3:uid="{91FAE540-34A4-1F40-97BE-B3FA0E795034}" name="R_0"/>
     <tableColumn id="8" xr3:uid="{E87410B6-E742-C442-AA86-2FFC5CA9681D}" name="X_0"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{045739EA-1F28-0E41-AB74-C2C34C8286AB}" name="Type" displayName="Type" ref="A1:A3" headerRowCount="0" totalsRowShown="0">
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{CF2DB599-7394-FB45-9EE6-02953B6FA5D3}" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3968,6 +4004,81 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E3FC359-2114-0F40-A6CA-BD1154039BEE}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F1" t="s">
+        <v>204</v>
+      </c>
+      <c r="G1" t="s">
+        <v>205</v>
+      </c>
+      <c r="H1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2">
+        <v>120</v>
+      </c>
+      <c r="C2">
+        <v>1.0329999999999999</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>0.3</v>
+      </c>
+      <c r="F2">
+        <v>0.3</v>
+      </c>
+      <c r="G2">
+        <v>0.7</v>
+      </c>
+      <c r="H2">
+        <v>0.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{0468B437-E2D3-304F-BB27-E264FA9991A9}">
+      <formula1>INDIRECT("Buses[bus]")</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37ABA1BE-A562-EA4D-912C-91965FAA05A8}">
   <dimension ref="A1:U15"/>
   <sheetViews>
@@ -4210,7 +4321,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5904AC-ECAC-4945-B9B6-B220AC818209}">
   <dimension ref="A1:N100"/>
   <sheetViews>
@@ -8178,7 +8289,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A60AA9E-251E-2D4D-A9AC-C0697DAD560B}">
   <dimension ref="A1:V20"/>
   <sheetViews>
@@ -9735,7 +9846,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67452CAF-D40E-2344-8B7E-ABD55E102AF6}">
   <dimension ref="A1:G10"/>
   <sheetViews>
@@ -11222,7 +11333,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2955D94-A9C5-924E-AFCA-D6295E4B752D}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -11413,6 +11524,151 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB54A0CB-1327-F543-85DC-D3F703CDF36F}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="11.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2">
+        <v>300</v>
+      </c>
+      <c r="C2">
+        <v>250</v>
+      </c>
+      <c r="D2" t="s">
+        <v>252</v>
+      </c>
+      <c r="E2">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>252</v>
+      </c>
+      <c r="E3">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4">
+        <v>50</v>
+      </c>
+      <c r="C4">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s">
+        <v>252</v>
+      </c>
+      <c r="E4">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5">
+        <v>300</v>
+      </c>
+      <c r="C5">
+        <v>300</v>
+      </c>
+      <c r="D5" t="s">
+        <v>253</v>
+      </c>
+      <c r="E5">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B6">
+        <v>70</v>
+      </c>
+      <c r="C6">
+        <v>70</v>
+      </c>
+      <c r="D6" t="s">
+        <v>253</v>
+      </c>
+      <c r="E6">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B7">
+        <v>40</v>
+      </c>
+      <c r="C7">
+        <v>40</v>
+      </c>
+      <c r="D7" t="s">
+        <v>253</v>
+      </c>
+      <c r="E7">
+        <v>0.44</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A7" xr:uid="{B3993603-09E4-E449-97A6-F5FAB170E3B4}">
+      <formula1>INDIRECT("Buses[Bus]")</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DEFE584-74FB-4243-A125-89ADE808B1CA}">
   <dimension ref="A1:Q8"/>
   <sheetViews>
@@ -11935,7 +12191,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75E43467-53F9-1D42-8F2F-AAAB7E7A2D54}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -11947,7 +12203,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{811BE620-6DAF-9740-B217-2EB0E7DBF9CC}">
   <dimension ref="A1:L10"/>
   <sheetViews>
@@ -12357,7 +12613,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CE5CFF8-7828-B948-AF88-0BAE820E01A6}">
   <dimension ref="A1:F28"/>
   <sheetViews>
@@ -12969,79 +13225,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E3FC359-2114-0F40-A6CA-BD1154039BEE}">
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>206</v>
-      </c>
-      <c r="B1" t="s">
-        <v>207</v>
-      </c>
-      <c r="C1" t="s">
-        <v>202</v>
-      </c>
-      <c r="D1" t="s">
-        <v>195</v>
-      </c>
-      <c r="E1" t="s">
-        <v>203</v>
-      </c>
-      <c r="F1" t="s">
-        <v>204</v>
-      </c>
-      <c r="G1" t="s">
-        <v>205</v>
-      </c>
-      <c r="H1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>154</v>
-      </c>
-      <c r="B2">
-        <v>120</v>
-      </c>
-      <c r="C2">
-        <v>1.0329999999999999</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>0.3</v>
-      </c>
-      <c r="F2">
-        <v>0.3</v>
-      </c>
-      <c r="G2">
-        <v>0.7</v>
-      </c>
-      <c r="H2">
-        <v>0.7</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{0468B437-E2D3-304F-BB27-E264FA9991A9}">
-      <formula1>INDIRECT("Buses[bus]")</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
add inverter constrols and irradiance time series
</commit_message>
<xml_diff>
--- a/network-data/LineGeo_Selector.xlsx
+++ b/network-data/LineGeo_Selector.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spenceregan/Repos/CU/Distribution_Systems/Project1/ECEN5437-Proj1/network-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA34C33-0F42-7D40-B5B5-95BB0E18A478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1983ED8C-4D45-D14B-8075-28B0B0B117FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{7AEC5E2E-397B-8345-871E-9ED757579969}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="261">
   <si>
     <t>OH3p</t>
   </si>
@@ -807,10 +807,31 @@
     <t>kvar_lim</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
+    <t>cont</t>
+  </si>
+  <si>
+    <t>deadband</t>
+  </si>
+  <si>
+    <t>priority</t>
+  </si>
+  <si>
+    <t>vars</t>
+  </si>
+  <si>
+    <t>watts</t>
+  </si>
+  <si>
+    <t>night_var_support</t>
+  </si>
+  <si>
+    <t>voltvar</t>
+  </si>
+  <si>
+    <t>voltwatt</t>
+  </si>
+  <si>
+    <t>vvmode</t>
   </si>
 </sst>
 </file>
@@ -2668,7 +2689,7 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{0D394314-B822-6C40-97B4-4F5CADFC1074}" name="xfmr_config" displayName="xfmr_config" ref="M1:M2" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{0D394314-B822-6C40-97B4-4F5CADFC1074}" name="xfmr_config" displayName="xfmr_config" ref="N1:N2" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{C224F9D5-0D1E-D648-9018-6D26270395C2}" name="Column1"/>
   </tableColumns>
@@ -2677,7 +2698,7 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{5F3073CA-6F2C-7643-A086-B783E9581317}" name="delta.delta" displayName="delta.delta" ref="H2:H7" headerRowCount="0" totalsRowShown="0" headerRowDxfId="23" dataDxfId="24" tableBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{5F3073CA-6F2C-7643-A086-B783E9581317}" name="delta.delta" displayName="delta.delta" ref="I2:I7" headerRowCount="0" totalsRowShown="0" headerRowDxfId="23" dataDxfId="24" tableBorderDxfId="26">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{50958CF2-21D9-984F-97B5-085C4560A350}" name="Column1" headerRowDxfId="22" dataDxfId="25"/>
   </tableColumns>
@@ -2686,7 +2707,7 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{89D1A629-368D-0B4B-8525-B86A48878238}" name="delta.wye" displayName="delta.wye" ref="I2:I5" headerRowCount="0" totalsRowShown="0" headerRowDxfId="20" tableBorderDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{89D1A629-368D-0B4B-8525-B86A48878238}" name="delta.wye" displayName="delta.wye" ref="J2:J5" headerRowCount="0" totalsRowShown="0" headerRowDxfId="20" tableBorderDxfId="21">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{A3625009-C857-274F-A122-CFD46E3541C5}" name="Column1" headerRowDxfId="19"/>
   </tableColumns>
@@ -2695,7 +2716,7 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{D6E2BF91-ACF1-C849-9AC2-F7ED9921C73E}" name="wye.delta" displayName="wye.delta" ref="J2:J5" headerRowCount="0" totalsRowShown="0" headerRowDxfId="17" tableBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{D6E2BF91-ACF1-C849-9AC2-F7ED9921C73E}" name="wye.delta" displayName="wye.delta" ref="K2:K5" headerRowCount="0" totalsRowShown="0" headerRowDxfId="17" tableBorderDxfId="18">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{147B4193-B138-D749-BACA-A6E839012CE7}" name="Column1" headerRowDxfId="16"/>
   </tableColumns>
@@ -2704,7 +2725,7 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{32FF552F-94F8-5F4A-A3CD-0CF8C4344854}" name="wye.wye" displayName="wye.wye" ref="K2:K3" headerRowCount="0" totalsRowShown="0" headerRowDxfId="14" tableBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{32FF552F-94F8-5F4A-A3CD-0CF8C4344854}" name="wye.wye" displayName="wye.wye" ref="L2:L3" headerRowCount="0" totalsRowShown="0" headerRowDxfId="14" tableBorderDxfId="15">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{9713DCA2-8057-6941-AB28-861C6CAD34E9}" name="Column1" headerRowDxfId="13"/>
   </tableColumns>
@@ -2713,7 +2734,7 @@
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{F85F963E-7E0D-DA40-BC57-8F71010CE834}" name="Terminals" displayName="Terminals" ref="O1:O15" headerRowCount="0" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{F85F963E-7E0D-DA40-BC57-8F71010CE834}" name="Terminals" displayName="Terminals" ref="P1:P15" headerRowCount="0" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{B57E695F-4DAF-C041-9D98-90DA0E9FCF30}" name="Column1" dataDxfId="12"/>
   </tableColumns>
@@ -2722,7 +2743,7 @@
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{7C66977E-132E-CD40-9247-9F596B6AB81A}" name="MeterElement" displayName="MeterElement" ref="Q1:Q2" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{7C66977E-132E-CD40-9247-9F596B6AB81A}" name="MeterElement" displayName="MeterElement" ref="R1:R2" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{555D147D-0928-4C49-89D1-583C518DA5CB}" name="Column1"/>
   </tableColumns>
@@ -2775,7 +2796,7 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{59012749-ADB5-0341-AF22-07D1487AEE43}" name="bool" displayName="bool" ref="S1:S2" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{59012749-ADB5-0341-AF22-07D1487AEE43}" name="bool" displayName="bool" ref="T1:T2" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{24BA7888-D19F-8140-9509-C843591C8D6F}" name="Column1"/>
   </tableColumns>
@@ -2784,7 +2805,7 @@
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{08B74F89-8C69-4646-999E-90CA377EC508}" name="RegType" displayName="RegType" ref="U1:U2" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{08B74F89-8C69-4646-999E-90CA377EC508}" name="RegType" displayName="RegType" ref="V1:V2" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{93757295-DECB-A342-BB2A-A812C879A53F}" name="Column1"/>
   </tableColumns>
@@ -2793,6 +2814,24 @@
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="27" xr:uid="{B16B0666-6FD4-8D4A-BA10-22E8DFB1D110}" name="varwatt" displayName="varwatt" ref="X1:X2" headerRowCount="0" totalsRowShown="0">
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{6C04ACB9-3586-E240-97E9-CBE6B938FC67}" name="Column1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="28" xr:uid="{D0852B96-5006-BF4D-A641-E1E97F0EE448}" name="pvmode" displayName="pvmode" ref="G1:G2" headerRowCount="0" totalsRowShown="0">
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{E2B47D87-BAF5-904E-B5D9-65A2074C7E75}" name="Column1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E4FB8847-4274-D04D-A64C-15B4CD5C8D60}" name="OH" displayName="OH" ref="A1:K100" totalsRowShown="0">
   <autoFilter ref="A1:K100" xr:uid="{E4FB8847-4274-D04D-A64C-15B4CD5C8D60}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -2832,7 +2871,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{661274D6-1D68-5542-8D94-45D5C86243F5}" name="CN" displayName="CN" ref="A1:V19" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59" tableBorderDxfId="58">
   <autoFilter ref="A1:V19" xr:uid="{661274D6-1D68-5542-8D94-45D5C86243F5}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -2910,7 +2949,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{13D01E9F-2651-EF45-A492-F190721E7BE9}" name="TS" displayName="TS" ref="A1:G10" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
   <autoFilter ref="A1:G10" xr:uid="{13D01E9F-2651-EF45-A492-F190721E7BE9}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -2999,20 +3038,26 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{E8E696DC-003E-2448-9B7F-4C97C724B059}" name="Table26" displayName="Table26" ref="A1:E7" totalsRowShown="0">
-  <autoFilter ref="A1:E7" xr:uid="{E8E696DC-003E-2448-9B7F-4C97C724B059}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{E8E696DC-003E-2448-9B7F-4C97C724B059}" name="PV" displayName="PV" ref="A1:H7" totalsRowShown="0">
+  <autoFilter ref="A1:H7" xr:uid="{E8E696DC-003E-2448-9B7F-4C97C724B059}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
     <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+    <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="5">
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{BA31837E-5B81-DF47-9042-8460B1AEEF42}" name="bus"/>
     <tableColumn id="2" xr3:uid="{5363DCF8-99A3-ED49-9E87-3881745C2B1D}" name="kVA"/>
     <tableColumn id="3" xr3:uid="{2FBFA86A-A1A4-774E-B4F4-8A3D4033D33F}" name="Pmpp"/>
     <tableColumn id="4" xr3:uid="{1DF94CE5-644E-E543-A808-67DB3F9569AA}" name="inv_curve"/>
     <tableColumn id="5" xr3:uid="{9BD28774-6D1B-614F-945C-703372656F1C}" name="kvar_lim"/>
+    <tableColumn id="6" xr3:uid="{D52FE9AA-C69B-C04A-894E-889686F45C26}" name="night_var_support"/>
+    <tableColumn id="7" xr3:uid="{D2471522-1189-C642-80B2-071F82E85412}" name="priority"/>
+    <tableColumn id="8" xr3:uid="{00D41B43-8424-4043-8891-2DED3648A15B}" name="vvmode"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4080,15 +4125,15 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37ABA1BE-A562-EA4D-912C-91965FAA05A8}">
-  <dimension ref="A1:U15"/>
+  <dimension ref="A1:X15"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>70</v>
       </c>
@@ -4098,35 +4143,41 @@
       <c r="E1" t="s">
         <v>175</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="G1" t="s">
+        <v>258</v>
+      </c>
+      <c r="I1" s="14" t="s">
         <v>215</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="J1" s="15" t="s">
         <v>216</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="K1" s="14" t="s">
         <v>217</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="L1" s="15" t="s">
         <v>218</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>191</v>
       </c>
-      <c r="O1" s="1">
+      <c r="P1" s="1">
         <v>1</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>231</v>
       </c>
-      <c r="S1" t="b">
+      <c r="T1" t="b">
         <v>1</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="X1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>71</v>
       </c>
@@ -4136,35 +4187,41 @@
       <c r="E2" t="s">
         <v>178</v>
       </c>
-      <c r="H2" s="16">
+      <c r="G2" t="s">
+        <v>259</v>
+      </c>
+      <c r="I2" s="16">
         <v>0</v>
-      </c>
-      <c r="I2" s="16">
-        <v>-30</v>
       </c>
       <c r="J2" s="16">
         <v>-30</v>
       </c>
       <c r="K2" s="16">
+        <v>-30</v>
+      </c>
+      <c r="L2" s="16">
         <v>0</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>192</v>
       </c>
-      <c r="O2" s="1">
+      <c r="P2" s="1">
         <v>2</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>232</v>
       </c>
-      <c r="S2" t="b">
+      <c r="T2" t="b">
         <v>0</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="X2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>72</v>
       </c>
@@ -4174,137 +4231,137 @@
       <c r="E3" t="s">
         <v>174</v>
       </c>
-      <c r="H3" s="17">
+      <c r="I3" s="17">
         <v>-60</v>
-      </c>
-      <c r="I3" s="17">
-        <v>-150</v>
       </c>
       <c r="J3" s="17">
         <v>-150</v>
       </c>
       <c r="K3" s="17">
+        <v>-150</v>
+      </c>
+      <c r="L3" s="17">
         <v>180</v>
       </c>
-      <c r="O3" s="1">
+      <c r="P3" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>78</v>
       </c>
       <c r="E4" t="s">
         <v>179</v>
       </c>
-      <c r="H4" s="16">
+      <c r="I4" s="16">
         <v>-120</v>
-      </c>
-      <c r="I4" s="16">
-        <v>150</v>
       </c>
       <c r="J4" s="16">
         <v>150</v>
       </c>
-      <c r="K4" s="18"/>
-      <c r="O4" s="1">
+      <c r="K4" s="16">
+        <v>150</v>
+      </c>
+      <c r="L4" s="18"/>
+      <c r="P4" s="1">
         <v>1.2</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
         <v>81</v>
       </c>
       <c r="E5" t="s">
         <v>180</v>
       </c>
-      <c r="H5" s="17">
+      <c r="I5" s="17">
         <v>-180</v>
-      </c>
-      <c r="I5" s="17">
-        <v>30</v>
       </c>
       <c r="J5" s="17">
         <v>30</v>
       </c>
-      <c r="K5" s="19"/>
-      <c r="O5" s="1">
+      <c r="K5" s="17">
+        <v>30</v>
+      </c>
+      <c r="L5" s="19"/>
+      <c r="P5" s="1">
         <v>1.3</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>82</v>
       </c>
       <c r="E6" t="s">
         <v>177</v>
       </c>
-      <c r="H6" s="16">
+      <c r="I6" s="16">
         <v>120</v>
       </c>
-      <c r="I6" s="18"/>
-      <c r="O6" s="1">
+      <c r="J6" s="18"/>
+      <c r="P6" s="1">
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
         <v>83</v>
       </c>
       <c r="E7" t="s">
         <v>181</v>
       </c>
-      <c r="H7" s="17">
+      <c r="I7" s="17">
         <v>60</v>
       </c>
-      <c r="I7" s="19"/>
-      <c r="O7" s="1">
+      <c r="J7" s="19"/>
+      <c r="P7" s="1">
         <v>2.1</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="O8" s="1">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="P8" s="1">
         <v>3.1</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="O9" s="1">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="P9" s="1">
         <v>3.2</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="O10" s="1" t="s">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="P10" s="1" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="O11" s="1" t="s">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="P11" s="1" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="O12" s="1" t="s">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="P12" s="1" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="O13" s="1" t="s">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="P13" s="1" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="O14" s="1" t="s">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="P14" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="O15" s="1" t="s">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="P15" s="1" t="s">
         <v>213</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="12">
+  <tableParts count="14">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
@@ -4317,6 +4374,8 @@
     <tablePart r:id="rId10"/>
     <tablePart r:id="rId11"/>
     <tablePart r:id="rId12"/>
+    <tablePart r:id="rId13"/>
+    <tablePart r:id="rId14"/>
   </tableParts>
 </worksheet>
 </file>
@@ -11334,7 +11393,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11525,10 +11584,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB54A0CB-1327-F543-85DC-D3F703CDF36F}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11536,7 +11595,7 @@
     <col min="4" max="4" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>201</v>
       </c>
@@ -11552,8 +11611,17 @@
       <c r="E1" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>257</v>
+      </c>
+      <c r="G1" t="s">
+        <v>254</v>
+      </c>
+      <c r="H1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>113</v>
       </c>
@@ -11569,8 +11637,17 @@
       <c r="E2">
         <v>0.44</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>255</v>
+      </c>
+      <c r="H2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>125</v>
       </c>
@@ -11586,8 +11663,17 @@
       <c r="E3">
         <v>0.44</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>255</v>
+      </c>
+      <c r="H3" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>133</v>
       </c>
@@ -11603,8 +11689,17 @@
       <c r="E4">
         <v>0.44</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>255</v>
+      </c>
+      <c r="H4" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>119</v>
       </c>
@@ -11620,8 +11715,17 @@
       <c r="E5">
         <v>0.44</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>255</v>
+      </c>
+      <c r="H5" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>142</v>
       </c>
@@ -11637,8 +11741,17 @@
       <c r="E6">
         <v>0.44</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>255</v>
+      </c>
+      <c r="H6" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>148</v>
       </c>
@@ -11654,11 +11767,29 @@
       <c r="E7">
         <v>0.44</v>
       </c>
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>255</v>
+      </c>
+      <c r="H7" t="s">
+        <v>258</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A7" xr:uid="{B3993603-09E4-E449-97A6-F5FAB170E3B4}">
       <formula1>INDIRECT("Buses[Bus]")</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F7" xr:uid="{AAC5B9BE-2925-0A4C-A29C-7E02CA2100A0}">
+      <formula1>INDIRECT("bool")</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G7" xr:uid="{9FCCB5BC-6CD2-1C4B-86A7-E1B8B7B428F8}">
+      <formula1>INDIRECT("varwatt")</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H7" xr:uid="{93C3B801-796C-C54E-81C8-78DFD8DF95C6}">
+      <formula1>INDIRECT("pvmode")</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12618,7 +12749,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add project 3 notebook
</commit_message>
<xml_diff>
--- a/network-data/LineGeo_Selector.xlsx
+++ b/network-data/LineGeo_Selector.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spenceregan/Repos/CU/Distribution_Systems/Project1/ECEN5437-Proj1/network-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1983ED8C-4D45-D14B-8075-28B0B0B117FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2182CB2E-7927-E54C-8046-C43904B005FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{7AEC5E2E-397B-8345-871E-9ED757579969}"/>
+    <workbookView xWindow="7840" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{7AEC5E2E-397B-8345-871E-9ED757579969}"/>
   </bookViews>
   <sheets>
     <sheet name="Buses" sheetId="7" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="261">
   <si>
     <t>OH3p</t>
   </si>
@@ -966,7 +966,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -982,14 +982,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -997,405 +992,6 @@
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="94">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <right style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </right>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <right style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </right>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -2285,6 +1881,384 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2380,6 +2354,27 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -2698,45 +2693,45 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{5F3073CA-6F2C-7643-A086-B783E9581317}" name="delta.delta" displayName="delta.delta" ref="I2:I7" headerRowCount="0" totalsRowShown="0" headerRowDxfId="23" dataDxfId="24" tableBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{5F3073CA-6F2C-7643-A086-B783E9581317}" name="delta.delta" displayName="delta.delta" ref="I2:I7" headerRowCount="0" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54" tableBorderDxfId="53">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{50958CF2-21D9-984F-97B5-085C4560A350}" name="Column1" headerRowDxfId="22" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{50958CF2-21D9-984F-97B5-085C4560A350}" name="Column1" headerRowDxfId="52" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{89D1A629-368D-0B4B-8525-B86A48878238}" name="delta.wye" displayName="delta.wye" ref="J2:J5" headerRowCount="0" totalsRowShown="0" headerRowDxfId="20" tableBorderDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{89D1A629-368D-0B4B-8525-B86A48878238}" name="delta.wye" displayName="delta.wye" ref="J2:J5" headerRowCount="0" totalsRowShown="0" headerRowDxfId="50" tableBorderDxfId="49">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{A3625009-C857-274F-A122-CFD46E3541C5}" name="Column1" headerRowDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{A3625009-C857-274F-A122-CFD46E3541C5}" name="Column1" headerRowDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{D6E2BF91-ACF1-C849-9AC2-F7ED9921C73E}" name="wye.delta" displayName="wye.delta" ref="K2:K5" headerRowCount="0" totalsRowShown="0" headerRowDxfId="17" tableBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{D6E2BF91-ACF1-C849-9AC2-F7ED9921C73E}" name="wye.delta" displayName="wye.delta" ref="K2:K5" headerRowCount="0" totalsRowShown="0" headerRowDxfId="47" tableBorderDxfId="46">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{147B4193-B138-D749-BACA-A6E839012CE7}" name="Column1" headerRowDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{147B4193-B138-D749-BACA-A6E839012CE7}" name="Column1" headerRowDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{32FF552F-94F8-5F4A-A3CD-0CF8C4344854}" name="wye.wye" displayName="wye.wye" ref="L2:L3" headerRowCount="0" totalsRowShown="0" headerRowDxfId="14" tableBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{32FF552F-94F8-5F4A-A3CD-0CF8C4344854}" name="wye.wye" displayName="wye.wye" ref="L2:L3" headerRowCount="0" totalsRowShown="0" headerRowDxfId="44" tableBorderDxfId="43">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{9713DCA2-8057-6941-AB28-861C6CAD34E9}" name="Column1" headerRowDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{9713DCA2-8057-6941-AB28-861C6CAD34E9}" name="Column1" headerRowDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{F85F963E-7E0D-DA40-BC57-8F71010CE834}" name="Terminals" displayName="Terminals" ref="P1:P15" headerRowCount="0" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{F85F963E-7E0D-DA40-BC57-8F71010CE834}" name="Terminals" displayName="Terminals" ref="P1:P15" headerRowCount="0" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{B57E695F-4DAF-C041-9D98-90DA0E9FCF30}" name="Column1" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{B57E695F-4DAF-C041-9D98-90DA0E9FCF30}" name="Column1" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2847,23 +2842,23 @@
     <filterColumn colId="10" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{E903BA16-38F3-EE44-A1B4-2B0F344DDB1D}" name="Type" dataDxfId="65">
+    <tableColumn id="1" xr3:uid="{E903BA16-38F3-EE44-A1B4-2B0F344DDB1D}" name="Type" dataDxfId="38">
       <calculatedColumnFormula>_xlfn.CONCAT(OH[[#This Row],[Size]], "_",OH[[#This Row],[Stranding]], "_", OH[[#This Row],[Material]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{B69CA351-3694-B545-8563-7479CF50BC67}" name="Size" dataDxfId="64"/>
+    <tableColumn id="2" xr3:uid="{B69CA351-3694-B545-8563-7479CF50BC67}" name="Size" dataDxfId="37"/>
     <tableColumn id="3" xr3:uid="{3576FC0F-75EE-6F4B-B709-5C5715FE540E}" name="Stranding"/>
     <tableColumn id="4" xr3:uid="{C31618D9-7DA8-804A-A013-69A802FF7774}" name="Material"/>
     <tableColumn id="5" xr3:uid="{804C85FC-06A5-4645-A278-FD8271A5F0ED}" name="Diam"/>
     <tableColumn id="6" xr3:uid="{ED80EC98-63E4-C94C-BAF3-F13294EE8381}" name="GMRac"/>
     <tableColumn id="7" xr3:uid="{41A91B17-FB89-1F4F-899A-3761661447FD}" name="rac"/>
     <tableColumn id="8" xr3:uid="{C9144B25-D7C0-D444-8605-CEBD77A9171D}" name="normamps"/>
-    <tableColumn id="13" xr3:uid="{041E70E4-975E-254A-81CF-95C5EF9E73D2}" name="GMRunits" dataDxfId="63">
+    <tableColumn id="13" xr3:uid="{041E70E4-975E-254A-81CF-95C5EF9E73D2}" name="GMRunits" dataDxfId="36">
       <calculatedColumnFormula>"ft"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{2AEFB39D-D6D8-D14D-A990-9BB4F5164639}" name="runits" dataDxfId="62">
+    <tableColumn id="14" xr3:uid="{2AEFB39D-D6D8-D14D-A990-9BB4F5164639}" name="runits" dataDxfId="35">
       <calculatedColumnFormula>"mi"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{21A61F38-5A94-2142-A9A8-D6E0BB77AB1E}" name="Size_Material" dataDxfId="61">
+    <tableColumn id="15" xr3:uid="{21A61F38-5A94-2142-A9A8-D6E0BB77AB1E}" name="Size_Material" dataDxfId="34">
       <calculatedColumnFormula>_xlfn.CONCAT(OH[[#This Row],[Size]], "_", OH[[#This Row],[Material]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2872,7 +2867,7 @@
 </file>
 
 <file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{661274D6-1D68-5542-8D94-45D5C86243F5}" name="CN" displayName="CN" ref="A1:V19" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59" tableBorderDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{661274D6-1D68-5542-8D94-45D5C86243F5}" name="CN" displayName="CN" ref="A1:V19" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32" tableBorderDxfId="31">
   <autoFilter ref="A1:V19" xr:uid="{661274D6-1D68-5542-8D94-45D5C86243F5}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2898,59 +2893,59 @@
     <filterColumn colId="21" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="22">
-    <tableColumn id="9" xr3:uid="{869F190C-19C4-2243-84CA-F6CB8F4281C2}" name="Type" dataDxfId="57">
+    <tableColumn id="9" xr3:uid="{869F190C-19C4-2243-84CA-F6CB8F4281C2}" name="Type" dataDxfId="30">
       <calculatedColumnFormula>_xlfn.CONCAT(CN[[#This Row],[Neutral Ampacity]], "_", CN[[#This Row],[Conductor Size]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{1DFBB787-8CEC-A946-969E-C8B3E35D5AEB}" name="Neutral Ampacity" dataDxfId="56"/>
-    <tableColumn id="2" xr3:uid="{EFDAEEF3-E5BA-4B49-BA44-2340320EA290}" name="Conductor Size" dataDxfId="55"/>
-    <tableColumn id="18" xr3:uid="{703A2A0A-5882-4349-9ACB-A05C1C032238}" name="Phase Conductor Name" dataDxfId="54">
+    <tableColumn id="1" xr3:uid="{1DFBB787-8CEC-A946-969E-C8B3E35D5AEB}" name="Neutral Ampacity" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{EFDAEEF3-E5BA-4B49-BA44-2340320EA290}" name="Conductor Size" dataDxfId="28"/>
+    <tableColumn id="18" xr3:uid="{703A2A0A-5882-4349-9ACB-A05C1C032238}" name="Phase Conductor Name" dataDxfId="27">
       <calculatedColumnFormula>_xlfn.XLOOKUP(_xlfn.CONCAT(LEFT(CN[[#This Row],[Conductor Size]], SEARCH("(", CN[[#This Row],[Conductor Size]])-1), "_AA"), OH[Size_Material], OH[Type], NA(),-1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8E5F5E70-58CE-0D4E-A970-1B53EA80FE07}" name="DiaIns" dataDxfId="53"/>
-    <tableColumn id="4" xr3:uid="{D154B6B5-D516-AC44-879B-B0BC6ACADF64}" name="Diameter Over Screen (in)" dataDxfId="52"/>
-    <tableColumn id="5" xr3:uid="{51092775-E14C-4945-BD12-6F609313AC1A}" name="DiaCable" dataDxfId="51"/>
-    <tableColumn id="6" xr3:uid="{FE25AF87-2C02-C642-B28A-81AF2224011F}" name="Copper Neutral" dataDxfId="50"/>
-    <tableColumn id="7" xr3:uid="{167EFF3D-5388-5C47-9405-F0CE90C78333}" name="Ampacity in Underground Duct (A)" dataDxfId="49"/>
-    <tableColumn id="8" xr3:uid="{D4CA2780-FAB4-FE44-BAA2-A16B53A68DE8}" name="Voltage Rating (kV)" dataDxfId="48"/>
-    <tableColumn id="11" xr3:uid="{830817DB-B122-D444-8DFC-58C1CE7D7901}" name="Neutral Strand AWG" dataDxfId="47" dataCellStyle="Percent">
+    <tableColumn id="3" xr3:uid="{8E5F5E70-58CE-0D4E-A970-1B53EA80FE07}" name="DiaIns" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{D154B6B5-D516-AC44-879B-B0BC6ACADF64}" name="Diameter Over Screen (in)" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{51092775-E14C-4945-BD12-6F609313AC1A}" name="DiaCable" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{FE25AF87-2C02-C642-B28A-81AF2224011F}" name="Copper Neutral" dataDxfId="23"/>
+    <tableColumn id="7" xr3:uid="{167EFF3D-5388-5C47-9405-F0CE90C78333}" name="Ampacity in Underground Duct (A)" dataDxfId="22"/>
+    <tableColumn id="8" xr3:uid="{D4CA2780-FAB4-FE44-BAA2-A16B53A68DE8}" name="Voltage Rating (kV)" dataDxfId="21"/>
+    <tableColumn id="11" xr3:uid="{830817DB-B122-D444-8DFC-58C1CE7D7901}" name="Neutral Strand AWG" dataDxfId="20" dataCellStyle="Percent">
       <calculatedColumnFormula>VALUE(RIGHT(CN[[#This Row],[Copper Neutral]],2))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{A0775550-BA03-5542-A01E-64482C59971C}" name="Rstrand" dataDxfId="46">
+    <tableColumn id="10" xr3:uid="{A0775550-BA03-5542-A01E-64482C59971C}" name="Rstrand" dataDxfId="19">
       <calculatedColumnFormula>_xlfn.XLOOKUP(CN[[#This Row],[Neutral Strand AWG]], OH[Size], OH[rac])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{4B541559-291A-4941-9353-F59C621A9E18}" name="k" dataDxfId="45">
+    <tableColumn id="12" xr3:uid="{4B541559-291A-4941-9353-F59C621A9E18}" name="k" dataDxfId="18">
       <calculatedColumnFormula>VALUE(LEFT(CN[[#This Row],[Copper Neutral]], SEARCH(" ",CN[[#This Row],[Copper Neutral]])-1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{60128454-1EE5-9C4B-9AA2-D0CE6F9C4CF7}" name="GMRac" dataDxfId="44">
+    <tableColumn id="13" xr3:uid="{60128454-1EE5-9C4B-9AA2-D0CE6F9C4CF7}" name="GMRac" dataDxfId="17">
       <calculatedColumnFormula>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]], OH[Type], OH[GMRac])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{AA242217-BC74-AB48-8D9A-86A3970B8399}" name="GmrStrand" dataDxfId="43">
+    <tableColumn id="14" xr3:uid="{AA242217-BC74-AB48-8D9A-86A3970B8399}" name="GmrStrand" dataDxfId="16">
       <calculatedColumnFormula>_xlfn.XLOOKUP(CN[[#This Row],[Neutral Strand AWG]], OH[Size], OH[GMRac])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{BDF03C79-D2AE-394A-9557-0FEAE0AA392C}" name="GMRunits" dataDxfId="42"/>
-    <tableColumn id="16" xr3:uid="{E6B7FA4C-2968-AE41-84BD-9EA25CF9A089}" name="Rac" dataDxfId="41">
+    <tableColumn id="15" xr3:uid="{BDF03C79-D2AE-394A-9557-0FEAE0AA392C}" name="GMRunits" dataDxfId="15"/>
+    <tableColumn id="16" xr3:uid="{E6B7FA4C-2968-AE41-84BD-9EA25CF9A089}" name="Rac" dataDxfId="14">
       <calculatedColumnFormula>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[rac])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{60CA6D09-ACAD-FA47-9A7F-D8BCB54C2191}" name="Runits" dataDxfId="40">
+    <tableColumn id="17" xr3:uid="{60CA6D09-ACAD-FA47-9A7F-D8BCB54C2191}" name="Runits" dataDxfId="13">
       <calculatedColumnFormula>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[runits])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{A335B60A-8482-494F-9920-64B3CC7615EB}" name="diam" dataDxfId="39">
+    <tableColumn id="19" xr3:uid="{A335B60A-8482-494F-9920-64B3CC7615EB}" name="diam" dataDxfId="12">
       <calculatedColumnFormula>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[Diam])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{D37687B3-1580-7845-A711-F39AB1A49147}" name="normamps" dataDxfId="38">
+    <tableColumn id="20" xr3:uid="{D37687B3-1580-7845-A711-F39AB1A49147}" name="normamps" dataDxfId="11">
       <calculatedColumnFormula>_xlfn.XLOOKUP(CN[[#This Row],[Phase Conductor Name]],OH[Type], OH[normamps])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{D2E6A1F4-79B9-0D45-BE31-8E41DE3A29BC}" name="DiaStrand" dataDxfId="37">
+    <tableColumn id="22" xr3:uid="{D2E6A1F4-79B9-0D45-BE31-8E41DE3A29BC}" name="DiaStrand" dataDxfId="10">
       <calculatedColumnFormula>_xlfn.XLOOKUP(CN[[#This Row],[Neutral Strand AWG]], OH[Size], OH[Diam])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{E3B20767-C678-7E4D-8C37-6DA7A2305EDB}" name="Radunits" dataDxfId="36"/>
+    <tableColumn id="23" xr3:uid="{E3B20767-C678-7E4D-8C37-6DA7A2305EDB}" name="Radunits" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{13D01E9F-2651-EF45-A492-F190721E7BE9}" name="TS" displayName="TS" ref="A1:G10" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{13D01E9F-2651-EF45-A492-F190721E7BE9}" name="TS" displayName="TS" ref="A1:G10" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A1:G10" xr:uid="{13D01E9F-2651-EF45-A492-F190721E7BE9}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2961,13 +2956,13 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{19CDDA2D-9812-404F-A70E-F8C42AD526DB}" name="Type" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{C1A0B38B-F04B-0A4C-913A-B68BB0D6C78E}" name="Diameter Over Insulation (in)" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{D6D141BB-2B57-4B4B-8667-6762392800DB}" name="Diameter Over Screen (in)" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{401114E4-AC5F-DA47-A949-534E36354F8D}" name="Jacket Thickness (mils)" dataDxfId="30"/>
-    <tableColumn id="5" xr3:uid="{244E8C6F-E27A-B344-A042-CF80AF18FA7C}" name="Outside Diameter" dataDxfId="29"/>
-    <tableColumn id="6" xr3:uid="{D80F22EC-CB8C-E549-AC7C-4BA81E9F5164}" name="Ampacity in UG Duct (A)" dataDxfId="28"/>
-    <tableColumn id="7" xr3:uid="{A989CB28-4027-F249-A88C-9A2D66CB1557}" name="Rated Voltage (kV)" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{19CDDA2D-9812-404F-A70E-F8C42AD526DB}" name="Type" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{C1A0B38B-F04B-0A4C-913A-B68BB0D6C78E}" name="Diameter Over Insulation (in)" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{D6D141BB-2B57-4B4B-8667-6762392800DB}" name="Diameter Over Screen (in)" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{401114E4-AC5F-DA47-A949-534E36354F8D}" name="Jacket Thickness (mils)" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{244E8C6F-E27A-B344-A042-CF80AF18FA7C}" name="Outside Diameter" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{D80F22EC-CB8C-E549-AC7C-4BA81E9F5164}" name="Ampacity in UG Duct (A)" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{A989CB28-4027-F249-A88C-9A2D66CB1557}" name="Rated Voltage (kV)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2998,8 +2993,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{D81C8915-A75B-ED43-95A0-D72233099B0F}" name="Regulators" displayName="Regulators" ref="A1:M4" totalsRowShown="0">
-  <autoFilter ref="A1:M4" xr:uid="{D81C8915-A75B-ED43-95A0-D72233099B0F}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{D81C8915-A75B-ED43-95A0-D72233099B0F}" name="Regulators" displayName="Regulators" ref="A1:O4" totalsRowShown="0">
+  <autoFilter ref="A1:O4" xr:uid="{D81C8915-A75B-ED43-95A0-D72233099B0F}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -3013,8 +3008,10 @@
     <filterColumn colId="10" hiddenButton="1"/>
     <filterColumn colId="11" hiddenButton="1"/>
     <filterColumn colId="12" hiddenButton="1"/>
+    <filterColumn colId="13" hiddenButton="1"/>
+    <filterColumn colId="14" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="13">
+  <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{DD9993CA-F636-F542-8A5B-6DAC073E79A9}" name="bus"/>
     <tableColumn id="3" xr3:uid="{84FEDC1F-56C2-BB45-865C-C02F4D8EC141}" name="kVA"/>
     <tableColumn id="4" xr3:uid="{404E61D9-A76D-0C45-96A5-4A4A712B4B26}" name="phases"/>
@@ -3023,15 +3020,17 @@
     <tableColumn id="7" xr3:uid="{2E6849E2-BBE5-CD4D-B609-0AE8DC587667}" name="band"/>
     <tableColumn id="8" xr3:uid="{D48784CE-6023-4848-AD45-7879BBE634CD}" name="CTprim"/>
     <tableColumn id="9" xr3:uid="{749082FB-86EF-7F42-8281-B562EE77C531}" name="CTsec"/>
-    <tableColumn id="10" xr3:uid="{A7506B33-3767-7B43-95E3-F8C20357BA5B}" name="delay" dataDxfId="1">
+    <tableColumn id="10" xr3:uid="{A7506B33-3767-7B43-95E3-F8C20357BA5B}" name="delay" dataDxfId="80">
       <calculatedColumnFormula>5*60</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{144DC39C-081C-7D44-8113-D0C6BE9258CE}" name="tapdelay" dataDxfId="0">
+    <tableColumn id="11" xr3:uid="{144DC39C-081C-7D44-8113-D0C6BE9258CE}" name="tapdelay" dataDxfId="79">
       <calculatedColumnFormula>5*60</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="12" xr3:uid="{7DE72D75-9286-744B-96F9-A683BB821A6A}" name="gang_operated"/>
     <tableColumn id="13" xr3:uid="{78933179-2764-AF4F-880F-A8B43FBD2801}" name="type"/>
     <tableColumn id="14" xr3:uid="{2AE35168-8842-6249-AE09-1028DFFEFFC2}" name="conn"/>
+    <tableColumn id="2" xr3:uid="{072A2A71-5530-824A-B7BE-34D85F523DB6}" name="X"/>
+    <tableColumn id="15" xr3:uid="{50E74F09-52AA-C840-8BF5-2968D3D29F92}" name="R"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3088,42 +3087,42 @@
     <tableColumn id="1" xr3:uid="{C58B47F9-739B-7B49-8572-5CF966DE57BF}" name="bus1"/>
     <tableColumn id="2" xr3:uid="{158E1C6F-2E86-A24E-A99E-F710460471A4}" name="bus2"/>
     <tableColumn id="3" xr3:uid="{1B8A6996-3AB7-224A-9AD8-27ED161B7D10}" name="xfmr"/>
-    <tableColumn id="4" xr3:uid="{A79FA7AF-C14D-2742-9392-2561ECAD3C4C}" name="kV1" dataDxfId="80">
+    <tableColumn id="4" xr3:uid="{A79FA7AF-C14D-2742-9392-2561ECAD3C4C}" name="kV1" dataDxfId="78">
       <calculatedColumnFormula>_xlfn.XLOOKUP(xfmrs[[#This Row],[xfmr]],xfmr_info[name],xfmr_info[kV_hv])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{8898BF2A-8518-E04A-9A6E-42AD088D8F6E}" name="kV2" dataDxfId="79">
+    <tableColumn id="5" xr3:uid="{8898BF2A-8518-E04A-9A6E-42AD088D8F6E}" name="kV2" dataDxfId="77">
       <calculatedColumnFormula>_xlfn.XLOOKUP(xfmrs[[#This Row],[xfmr]],xfmr_info[name],xfmr_info[kV_lv])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{D42902E7-C227-5B41-97A8-6AC8DF21E53C}" name="kVA1" dataDxfId="78">
+    <tableColumn id="6" xr3:uid="{D42902E7-C227-5B41-97A8-6AC8DF21E53C}" name="kVA1" dataDxfId="76">
       <calculatedColumnFormula>_xlfn.XLOOKUP(xfmrs[[#This Row],[xfmr]],xfmr_info[name],xfmr_info[kVA_hv])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{0BB098D2-D583-2146-8233-4EB095563D38}" name="kVA2" dataDxfId="77">
+    <tableColumn id="7" xr3:uid="{0BB098D2-D583-2146-8233-4EB095563D38}" name="kVA2" dataDxfId="75">
       <calculatedColumnFormula>_xlfn.XLOOKUP(xfmrs[[#This Row],[xfmr]],xfmr_info[name],xfmr_info[kVA_lv])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{1CE6ACB7-BD5A-BC43-86B4-D28A657C67B3}" name="conn1" dataDxfId="76">
+    <tableColumn id="8" xr3:uid="{1CE6ACB7-BD5A-BC43-86B4-D28A657C67B3}" name="conn1" dataDxfId="74">
       <calculatedColumnFormula>_xlfn.XLOOKUP(xfmrs[[#This Row],[xfmr]],xfmr_info[name],xfmr_info[Conn_hv])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{C1CD392B-A1E0-0E4D-9644-885A2CBC3563}" name="conn2" dataDxfId="75">
+    <tableColumn id="9" xr3:uid="{C1CD392B-A1E0-0E4D-9644-885A2CBC3563}" name="conn2" dataDxfId="73">
       <calculatedColumnFormula>_xlfn.XLOOKUP(xfmrs[[#This Row],[xfmr]],xfmr_info[name],xfmr_info[Conn_lv])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{D8DF443B-AF1C-264C-B64F-7EA66CBF65CC}" name="phases" dataDxfId="74">
+    <tableColumn id="10" xr3:uid="{D8DF443B-AF1C-264C-B64F-7EA66CBF65CC}" name="phases" dataDxfId="72">
       <calculatedColumnFormula>_xlfn.XLOOKUP(xfmrs[[#This Row],[xfmr]],xfmr_info[name],xfmr_info[Phases])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{5D9B233F-211C-BB47-9D7B-6B064811AE23}" name="windings" dataDxfId="6">
+    <tableColumn id="17" xr3:uid="{5D9B233F-211C-BB47-9D7B-6B064811AE23}" name="windings" dataDxfId="71">
       <calculatedColumnFormula>_xlfn.XLOOKUP(xfmrs[[#This Row],[xfmr]],xfmr_info[name],xfmr_info[Windings])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{2F73D725-1EF1-1646-AA1B-30806683307E}" name="R" dataDxfId="73">
+    <tableColumn id="11" xr3:uid="{2F73D725-1EF1-1646-AA1B-30806683307E}" name="R" dataDxfId="70">
       <calculatedColumnFormula>_xlfn.XLOOKUP(xfmrs[[#This Row],[xfmr]],xfmr_info[name],xfmr_info[R])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{5F54EB82-97EC-3641-9FD1-9EEAA4487A8C}" name="X" dataDxfId="72">
+    <tableColumn id="12" xr3:uid="{5F54EB82-97EC-3641-9FD1-9EEAA4487A8C}" name="X" dataDxfId="69">
       <calculatedColumnFormula>_xlfn.XLOOKUP(xfmrs[[#This Row],[xfmr]],xfmr_info[name],xfmr_info[X])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{5282C155-D5E7-FE49-8966-957D05B4F3D9}" name="nll" dataDxfId="7">
+    <tableColumn id="16" xr3:uid="{5282C155-D5E7-FE49-8966-957D05B4F3D9}" name="nll" dataDxfId="68">
       <calculatedColumnFormula>_xlfn.XLOOKUP(xfmrs[[#This Row],[xfmr]],xfmr_info[name],xfmr_info[nll])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{E19CAE52-E835-E54E-AC02-9A56DE7EC44D}" name="wnd1_terms" dataDxfId="9"/>
-    <tableColumn id="15" xr3:uid="{2AB55424-E657-6C44-A327-3B7EE71D6C9C}" name="wnd2_terms" dataDxfId="8"/>
-    <tableColumn id="18" xr3:uid="{69DA4BCE-2C58-0041-8D38-B07D3A767A8F}" name="wnd3_terms" dataDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{E19CAE52-E835-E54E-AC02-9A56DE7EC44D}" name="wnd1_terms" dataDxfId="67"/>
+    <tableColumn id="15" xr3:uid="{2AB55424-E657-6C44-A327-3B7EE71D6C9C}" name="wnd2_terms" dataDxfId="66"/>
+    <tableColumn id="18" xr3:uid="{69DA4BCE-2C58-0041-8D38-B07D3A767A8F}" name="wnd3_terms" dataDxfId="65"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3157,7 +3156,7 @@
     <tableColumn id="8" xr3:uid="{09E2D732-A304-6944-A2A0-1E51DBA4E1E9}" name="R"/>
     <tableColumn id="9" xr3:uid="{A6AD2380-16CB-204C-9DFD-B5F4D1F1AE3E}" name="X"/>
     <tableColumn id="11" xr3:uid="{54C6ABFF-F2E2-8047-9CFE-C8400D4265CF}" name="nll"/>
-    <tableColumn id="10" xr3:uid="{3027DC48-8D18-414F-A817-B76322236057}" name="name" dataDxfId="71">
+    <tableColumn id="10" xr3:uid="{3027DC48-8D18-414F-A817-B76322236057}" name="name" dataDxfId="64">
       <calculatedColumnFormula>_xlfn.CONCAT(xfmr_info[[#This Row],[Phases]],"p_",xfmr_info[[#This Row],[kV_hv]],"_",xfmr_info[[#This Row],[kV_lv]],"_",xfmr_info[[#This Row],[kVA_hv]],"_",LEFT(xfmr_info[[#This Row],[Conn_hv]],1),LEFT(xfmr_info[[#This Row],[Conn_lv]],1))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3166,7 +3165,7 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{CDAC5F4F-CC5E-714A-A10A-32F2E90176D7}" name="Loads" displayName="Loads" ref="A1:F28" totalsRowShown="0" headerRowDxfId="70" dataDxfId="69">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{CDAC5F4F-CC5E-714A-A10A-32F2E90176D7}" name="Loads" displayName="Loads" ref="A1:F28" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62">
   <autoFilter ref="A1:F28" xr:uid="{CDAC5F4F-CC5E-714A-A10A-32F2E90176D7}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3176,14 +3175,14 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{49EC89B8-2142-0A4A-B8EF-264BCDD715FA}" name="Bus" dataDxfId="68"/>
-    <tableColumn id="4" xr3:uid="{82843DB1-8D81-4741-83BB-3717AB506BFA}" name="Phases" dataDxfId="67">
+    <tableColumn id="1" xr3:uid="{49EC89B8-2142-0A4A-B8EF-264BCDD715FA}" name="Bus" dataDxfId="61"/>
+    <tableColumn id="4" xr3:uid="{82843DB1-8D81-4741-83BB-3717AB506BFA}" name="Phases" dataDxfId="60">
       <calculatedColumnFormula>_xlfn.XLOOKUP(Loads[[#This Row],[Bus]],Lines[bus2],Lines[phases],_xlfn.XLOOKUP(Loads[[#This Row],[Bus]],xfmrs[bus2],xfmrs[phases],0,0),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{13C1D0C2-6357-484D-ADEB-105711D6B1A5}" name="kW" dataDxfId="66"/>
-    <tableColumn id="3" xr3:uid="{A5C493EA-CBB6-854A-A97A-1FDDCAB8D84F}" name="kVAr" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{8D3CD5DC-3C01-EA41-B07F-F5CDB2FF56B0}" name="CondPos" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{65FC770D-1F3B-D142-9FDE-8782A4D0FBBA}" name="kV" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{13C1D0C2-6357-484D-ADEB-105711D6B1A5}" name="kW" dataDxfId="59"/>
+    <tableColumn id="3" xr3:uid="{A5C493EA-CBB6-854A-A97A-1FDDCAB8D84F}" name="kVAr" dataDxfId="58"/>
+    <tableColumn id="5" xr3:uid="{8D3CD5DC-3C01-EA41-B07F-F5CDB2FF56B0}" name="CondPos" dataDxfId="57"/>
+    <tableColumn id="6" xr3:uid="{65FC770D-1F3B-D142-9FDE-8782A4D0FBBA}" name="kV" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4146,16 +4145,16 @@
       <c r="G1" t="s">
         <v>258</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="14" t="s">
         <v>216</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="13" t="s">
         <v>217</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="L1" s="14" t="s">
         <v>218</v>
       </c>
       <c r="N1" t="s">
@@ -4190,16 +4189,16 @@
       <c r="G2" t="s">
         <v>259</v>
       </c>
-      <c r="I2" s="16">
+      <c r="I2" s="15">
         <v>0</v>
       </c>
-      <c r="J2" s="16">
+      <c r="J2" s="15">
         <v>-30</v>
       </c>
-      <c r="K2" s="16">
+      <c r="K2" s="15">
         <v>-30</v>
       </c>
-      <c r="L2" s="16">
+      <c r="L2" s="15">
         <v>0</v>
       </c>
       <c r="N2" t="s">
@@ -4231,16 +4230,16 @@
       <c r="E3" t="s">
         <v>174</v>
       </c>
-      <c r="I3" s="17">
+      <c r="I3" s="6">
         <v>-60</v>
       </c>
-      <c r="J3" s="17">
+      <c r="J3" s="6">
         <v>-150</v>
       </c>
-      <c r="K3" s="17">
+      <c r="K3" s="6">
         <v>-150</v>
       </c>
-      <c r="L3" s="17">
+      <c r="L3" s="6">
         <v>180</v>
       </c>
       <c r="P3" s="1">
@@ -4254,16 +4253,15 @@
       <c r="E4" t="s">
         <v>179</v>
       </c>
-      <c r="I4" s="16">
+      <c r="I4" s="15">
         <v>-120</v>
       </c>
-      <c r="J4" s="16">
+      <c r="J4" s="15">
         <v>150</v>
       </c>
-      <c r="K4" s="16">
+      <c r="K4" s="15">
         <v>150</v>
       </c>
-      <c r="L4" s="18"/>
       <c r="P4" s="1">
         <v>1.2</v>
       </c>
@@ -4275,16 +4273,15 @@
       <c r="E5" t="s">
         <v>180</v>
       </c>
-      <c r="I5" s="17">
+      <c r="I5" s="6">
         <v>-180</v>
       </c>
-      <c r="J5" s="17">
+      <c r="J5" s="6">
         <v>30</v>
       </c>
-      <c r="K5" s="17">
+      <c r="K5" s="6">
         <v>30</v>
       </c>
-      <c r="L5" s="19"/>
       <c r="P5" s="1">
         <v>1.3</v>
       </c>
@@ -4296,10 +4293,9 @@
       <c r="E6" t="s">
         <v>177</v>
       </c>
-      <c r="I6" s="16">
+      <c r="I6" s="15">
         <v>120</v>
       </c>
-      <c r="J6" s="18"/>
       <c r="P6" s="1">
         <v>2.2999999999999998</v>
       </c>
@@ -4311,10 +4307,9 @@
       <c r="E7" t="s">
         <v>181</v>
       </c>
-      <c r="I7" s="17">
+      <c r="I7" s="6">
         <v>60</v>
       </c>
-      <c r="J7" s="19"/>
       <c r="P7" s="1">
         <v>2.1</v>
       </c>
@@ -11390,10 +11385,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2955D94-A9C5-924E-AFCA-D6295E4B752D}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11401,7 +11396,7 @@
     <col min="12" max="12" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>201</v>
       </c>
@@ -11441,8 +11436,14 @@
       <c r="M1" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N1" t="s">
+        <v>190</v>
+      </c>
+      <c r="O1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>109</v>
       </c>
@@ -11456,7 +11457,7 @@
         <v>120</v>
       </c>
       <c r="E2">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F2">
         <v>2</v>
@@ -11468,11 +11469,11 @@
         <v>5</v>
       </c>
       <c r="I2">
-        <f t="shared" ref="I2:I4" si="0">5*60</f>
+        <f t="shared" ref="I2" si="0">5*60</f>
         <v>300</v>
       </c>
       <c r="J2">
-        <f t="shared" ref="J2:J4" si="1">5*60</f>
+        <f t="shared" ref="J2" si="1">5*60</f>
         <v>300</v>
       </c>
       <c r="K2" t="b">
@@ -11481,8 +11482,14 @@
       <c r="L2" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N2">
+        <v>0.01</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>112</v>
       </c>
@@ -11521,8 +11528,14 @@
       <c r="L3" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N3">
+        <v>0.01</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>114</v>
       </c>
@@ -11559,8 +11572,15 @@
       <c r="L4" t="s">
         <v>245</v>
       </c>
+      <c r="N4">
+        <v>0.01</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A4" xr:uid="{B78B59D8-45A0-C54C-8EC5-DA8054832273}">
       <formula1>INDIRECT("Buses[Bus]")</formula1>
@@ -11586,8 +11606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB54A0CB-1327-F543-85DC-D3F703CDF36F}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11925,7 +11945,6 @@
       <c r="P2" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="Q2" s="13"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -11987,7 +12006,6 @@
       <c r="P3" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="Q3" s="13"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -12049,7 +12067,6 @@
       <c r="P4" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="Q4" s="13"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -12111,7 +12128,6 @@
       <c r="P5" s="1">
         <v>1.3</v>
       </c>
-      <c r="Q5" s="13"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -12173,7 +12189,6 @@
       <c r="P6" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="Q6" s="13"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -12235,7 +12250,6 @@
       <c r="P7" s="1">
         <v>2</v>
       </c>
-      <c r="Q7" s="13"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -12297,7 +12311,6 @@
       <c r="P8" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="Q8" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -12767,10 +12780,10 @@
       <c r="D1" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="11" t="s">
         <v>233</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="11" t="s">
         <v>234</v>
       </c>
     </row>
@@ -12788,7 +12801,7 @@
       <c r="D2" s="10">
         <v>2</v>
       </c>
-      <c r="E2" s="21">
+      <c r="E2" s="16">
         <v>1.3</v>
       </c>
       <c r="F2" s="10">
@@ -12809,7 +12822,7 @@
       <c r="D3" s="10">
         <v>2</v>
       </c>
-      <c r="E3" s="21">
+      <c r="E3" s="16">
         <v>1.3</v>
       </c>
       <c r="F3" s="10">
@@ -12830,7 +12843,7 @@
       <c r="D4" s="10">
         <v>4.5</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="16">
         <v>1.3</v>
       </c>
       <c r="F4" s="10">
@@ -12851,7 +12864,7 @@
       <c r="D5" s="10">
         <v>4</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="16">
         <v>1.3</v>
       </c>
       <c r="F5" s="10">
@@ -12872,7 +12885,7 @@
       <c r="D6" s="10">
         <v>20</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="16" t="s">
         <v>209</v>
       </c>
       <c r="F6" s="10">
@@ -12893,7 +12906,7 @@
       <c r="D7" s="10">
         <v>0.5</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="16">
         <v>1.3</v>
       </c>
       <c r="F7" s="10">
@@ -12914,7 +12927,7 @@
       <c r="D8" s="10">
         <v>1</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="16">
         <v>1.3</v>
       </c>
       <c r="F8" s="10">
@@ -12935,7 +12948,7 @@
       <c r="D9" s="10">
         <v>4</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="16">
         <v>1.3</v>
       </c>
       <c r="F9" s="10">
@@ -12956,7 +12969,7 @@
       <c r="D10" s="10">
         <v>10</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="16" t="s">
         <v>209</v>
       </c>
       <c r="F10" s="10">
@@ -12977,7 +12990,7 @@
       <c r="D11" s="10">
         <v>13</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="16" t="s">
         <v>209</v>
       </c>
       <c r="F11" s="10">
@@ -12998,7 +13011,7 @@
       <c r="D12" s="10">
         <v>20</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="E12" s="16" t="s">
         <v>209</v>
       </c>
       <c r="F12" s="10">
@@ -13019,7 +13032,7 @@
       <c r="D13" s="10">
         <v>15</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="16" t="s">
         <v>209</v>
       </c>
       <c r="F13" s="10">
@@ -13040,7 +13053,7 @@
       <c r="D14" s="10">
         <v>35</v>
       </c>
-      <c r="E14" s="21">
+      <c r="E14" s="16">
         <v>2</v>
       </c>
       <c r="F14" s="10">
@@ -13061,7 +13074,7 @@
       <c r="D15" s="10">
         <v>33</v>
       </c>
-      <c r="E15" s="21">
+      <c r="E15" s="16">
         <v>2</v>
       </c>
       <c r="F15" s="10">
@@ -13082,7 +13095,7 @@
       <c r="D16" s="10">
         <v>60</v>
       </c>
-      <c r="E16" s="21" t="s">
+      <c r="E16" s="16" t="s">
         <v>209</v>
       </c>
       <c r="F16" s="10">
@@ -13103,7 +13116,7 @@
       <c r="D17" s="10">
         <v>23</v>
       </c>
-      <c r="E17" s="21" t="s">
+      <c r="E17" s="16" t="s">
         <v>209</v>
       </c>
       <c r="F17" s="10">
@@ -13124,7 +13137,7 @@
       <c r="D18" s="10">
         <v>20</v>
       </c>
-      <c r="E18" s="21" t="s">
+      <c r="E18" s="16" t="s">
         <v>209</v>
       </c>
       <c r="F18" s="10">
@@ -13145,7 +13158,7 @@
       <c r="D19" s="10">
         <v>10</v>
       </c>
-      <c r="E19" s="21" t="s">
+      <c r="E19" s="16" t="s">
         <v>209</v>
       </c>
       <c r="F19" s="10">
@@ -13166,7 +13179,7 @@
       <c r="D20" s="10">
         <v>12</v>
       </c>
-      <c r="E20" s="21" t="s">
+      <c r="E20" s="16" t="s">
         <v>209</v>
       </c>
       <c r="F20" s="10">
@@ -13187,7 +13200,7 @@
       <c r="D21" s="10">
         <v>16</v>
       </c>
-      <c r="E21" s="21">
+      <c r="E21" s="16">
         <v>2</v>
       </c>
       <c r="F21" s="10">
@@ -13208,7 +13221,7 @@
       <c r="D22" s="10">
         <v>25</v>
       </c>
-      <c r="E22" s="21">
+      <c r="E22" s="16">
         <v>2</v>
       </c>
       <c r="F22" s="10">
@@ -13229,7 +13242,7 @@
       <c r="D23" s="10">
         <v>16</v>
       </c>
-      <c r="E23" s="21">
+      <c r="E23" s="16">
         <v>2</v>
       </c>
       <c r="F23" s="10">
@@ -13250,7 +13263,7 @@
       <c r="D24" s="10">
         <v>2</v>
       </c>
-      <c r="E24" s="21">
+      <c r="E24" s="16">
         <v>2</v>
       </c>
       <c r="F24" s="10">
@@ -13271,7 +13284,7 @@
       <c r="D25" s="10">
         <v>3</v>
       </c>
-      <c r="E25" s="21">
+      <c r="E25" s="16">
         <v>2</v>
       </c>
       <c r="F25" s="10">
@@ -13292,7 +13305,7 @@
       <c r="D26" s="10">
         <v>2</v>
       </c>
-      <c r="E26" s="21">
+      <c r="E26" s="16">
         <v>2</v>
       </c>
       <c r="F26" s="10">
@@ -13313,7 +13326,7 @@
       <c r="D27" s="10">
         <v>7</v>
       </c>
-      <c r="E27" s="21">
+      <c r="E27" s="16">
         <v>2</v>
       </c>
       <c r="F27" s="10">
@@ -13334,7 +13347,7 @@
       <c r="D28" s="10">
         <v>70</v>
       </c>
-      <c r="E28" s="21" t="s">
+      <c r="E28" s="16" t="s">
         <v>209</v>
       </c>
       <c r="F28" s="10">

</xml_diff>